<commit_message>
1.25-1.27 trie,review bfs&dfs,did matrix 48,54,59,agg knowledge
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F1D7CA2-60A9-1049-8ED8-3D2EE5A633E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B7D2A9F-A23C-AB41-90BD-48E6FF27B66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="800" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
+    <workbookView xWindow="780" yWindow="740" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="238">
   <si>
     <t>144</t>
   </si>
@@ -691,6 +691,60 @@
   </si>
   <si>
     <t>Word Search II</t>
+  </si>
+  <si>
+    <t>Matrix</t>
+  </si>
+  <si>
+    <t>Rotate Image</t>
+  </si>
+  <si>
+    <t>Spiral Matrix</t>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Sparse Matrix Multiplication</t>
+  </si>
+  <si>
+    <t>Longest Increasing Path in a Matrix</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element in a Sorted Matrix</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix II</t>
+  </si>
+  <si>
+    <t>Range Addition</t>
+  </si>
+  <si>
+    <t>Word Search</t>
+  </si>
+  <si>
+    <t>Best Meeting Point</t>
+  </si>
+  <si>
+    <t>Bomb Enemy</t>
+  </si>
+  <si>
+    <t>Shortest Distance from All Buildings</t>
+  </si>
+  <si>
+    <t>Smallest Rectangle Enclosing Black Pixels</t>
+  </si>
+  <si>
+    <t>Valid Sudoku</t>
+  </si>
+  <si>
+    <t>Sudoku Solver</t>
   </si>
 </sst>
 </file>
@@ -760,7 +814,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -770,8 +824,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1088,10 +1140,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
-  <dimension ref="A1:D233"/>
+  <dimension ref="A1:D255"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" workbookViewId="0">
-      <selection activeCell="F208" sqref="F208"/>
+    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
+      <selection activeCell="B211" sqref="B211"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2443,19 +2495,19 @@
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B115" s="11"/>
+      <c r="B115" s="9"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B116" s="11"/>
+      <c r="B116" s="9"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B117" s="11"/>
+      <c r="B117" s="9"/>
     </row>
     <row r="118" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B118" s="11"/>
+      <c r="B118" s="9"/>
     </row>
     <row r="119" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A119" s="7" t="s">
@@ -3392,22 +3444,18 @@
     </row>
     <row r="207" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A207" s="7">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C207" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D207" s="7"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="208" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A208" s="7">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>2</v>
@@ -3416,51 +3464,43 @@
     </row>
     <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A209" s="7">
-        <v>126</v>
+        <v>52</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B210" s="11"/>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B211" s="11"/>
-    </row>
-    <row r="212" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A212" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D209" s="7"/>
+    </row>
+    <row r="212" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A212" s="7"/>
+      <c r="B212" s="4"/>
+      <c r="C212" s="2"/>
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A213" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B212" s="11"/>
-    </row>
-    <row r="213" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A213" s="7" t="s">
+      <c r="B213" s="9"/>
+    </row>
+    <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A214" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B213" s="8"/>
-      <c r="C213" s="7" t="s">
+      <c r="B214" s="8"/>
+      <c r="C214" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A214" s="7">
-        <v>261</v>
-      </c>
-      <c r="B214" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C214" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D214" s="7"/>
     </row>
     <row r="215" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A215" s="7">
-        <v>323</v>
+        <v>261</v>
       </c>
       <c r="B215" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C215" s="2" t="s">
         <v>2</v>
@@ -3469,62 +3509,62 @@
     </row>
     <row r="216" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A216" s="7">
+        <v>323</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D216" s="7"/>
+    </row>
+    <row r="217" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A217" s="7">
         <v>305</v>
       </c>
-      <c r="B216" s="4" t="s">
+      <c r="B217" s="4" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B217" s="11"/>
-    </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B218" s="11"/>
-    </row>
-    <row r="219" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A219" s="6" t="s">
+      <c r="B218" s="9"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B219" s="9"/>
+    </row>
+    <row r="220" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A220" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B219" s="11"/>
-    </row>
-    <row r="220" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A220" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B220" s="8"/>
-      <c r="C220" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D220" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="B220" s="9"/>
     </row>
     <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A221" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B221" s="8"/>
+      <c r="C221" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D221" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A222" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B221" s="8"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="7"/>
-    </row>
-    <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A222" s="7">
-        <v>133</v>
-      </c>
-      <c r="B222" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="C222" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B222" s="8"/>
+      <c r="C222" s="7"/>
       <c r="D222" s="7"/>
     </row>
     <row r="223" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="7">
-        <v>399</v>
+        <v>133</v>
       </c>
       <c r="B223" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
@@ -3533,74 +3573,74 @@
     </row>
     <row r="224" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A224" s="7">
+        <v>399</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="C224" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D224" s="7"/>
+    </row>
+    <row r="225" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A225" s="7">
         <v>310</v>
       </c>
-      <c r="B224" s="3" t="s">
+      <c r="B225" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="C224" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D224" s="7"/>
-    </row>
-    <row r="225" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A225" s="7" t="s">
+      <c r="C225" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D225" s="7"/>
+    </row>
+    <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A226" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B225" s="9"/>
-      <c r="C225" s="7"/>
-      <c r="D225" s="7"/>
-    </row>
-    <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="7">
+      <c r="B226" s="8"/>
+      <c r="C226" s="7"/>
+      <c r="D226" s="7"/>
+    </row>
+    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A227" s="7">
         <v>149</v>
       </c>
-      <c r="B226" s="3" t="s">
+      <c r="B227" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C226" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D226" s="7"/>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B227" s="10"/>
+      <c r="C227" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D227" s="7"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B228" s="10"/>
-    </row>
-    <row r="229" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A229" s="6" t="s">
+      <c r="B228" s="9"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B229" s="9"/>
+    </row>
+    <row r="230" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A230" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B229" s="10"/>
-    </row>
-    <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A230" s="7" t="s">
+      <c r="B230" s="9"/>
+    </row>
+    <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A231" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B230" s="9"/>
-      <c r="C230" s="7" t="s">
+      <c r="B231" s="8"/>
+      <c r="C231" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A231" s="7">
-        <v>211</v>
-      </c>
-      <c r="B231" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C231" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D231" s="7"/>
     </row>
     <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" s="7">
         <v>208</v>
       </c>
-      <c r="B232" s="3" t="s">
+      <c r="B232" s="4" t="s">
         <v>218</v>
       </c>
       <c r="C232" s="2" t="s">
@@ -3610,15 +3650,241 @@
     </row>
     <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="7">
+        <v>211</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="C233" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D233" s="7"/>
+    </row>
+    <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A234" s="7">
         <v>212</v>
       </c>
-      <c r="B233" s="3" t="s">
+      <c r="B234" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="C233" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D233" s="7"/>
+      <c r="C234" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D234" s="7"/>
+    </row>
+    <row r="237" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A237" s="6" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A238" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B238" s="7"/>
+      <c r="C238" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A239" s="7">
+        <v>48</v>
+      </c>
+      <c r="B239" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C239" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D239" s="7"/>
+    </row>
+    <row r="240" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A240" s="7">
+        <v>54</v>
+      </c>
+      <c r="B240" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C240" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D240" s="7"/>
+    </row>
+    <row r="241" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A241" s="7">
+        <v>59</v>
+      </c>
+      <c r="B241" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C241" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D241" s="7"/>
+    </row>
+    <row r="242" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A242" s="7">
+        <v>73</v>
+      </c>
+      <c r="B242" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C242" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D242" s="7"/>
+    </row>
+    <row r="243" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A243" s="7">
+        <v>311</v>
+      </c>
+      <c r="B243" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C243" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D243" s="7"/>
+    </row>
+    <row r="244" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A244" s="7">
+        <v>329</v>
+      </c>
+      <c r="B244" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" s="7"/>
+    </row>
+    <row r="245" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A245" s="7">
+        <v>378</v>
+      </c>
+      <c r="B245" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C245" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D245" s="7"/>
+    </row>
+    <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A246" s="7">
+        <v>74</v>
+      </c>
+      <c r="B246" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C246" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D246" s="7"/>
+    </row>
+    <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A247" s="7">
+        <v>240</v>
+      </c>
+      <c r="B247" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C247" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D247" s="7"/>
+    </row>
+    <row r="248" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A248" s="7">
+        <v>370</v>
+      </c>
+      <c r="B248" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C248" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D248" s="7"/>
+    </row>
+    <row r="249" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A249" s="7">
+        <v>79</v>
+      </c>
+      <c r="B249" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C249" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D249" s="7"/>
+    </row>
+    <row r="250" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A250" s="7">
+        <v>296</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250" s="7"/>
+    </row>
+    <row r="251" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A251" s="7">
+        <v>361</v>
+      </c>
+      <c r="B251" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D251" s="7"/>
+    </row>
+    <row r="252" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A252" s="7">
+        <v>317</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D252" s="7"/>
+    </row>
+    <row r="253" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A253" s="7">
+        <v>302</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D253" s="7"/>
+    </row>
+    <row r="254" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A254" s="7">
+        <v>36</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D254" s="7"/>
+    </row>
+    <row r="255" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A255" s="7">
+        <v>37</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>237</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3737,16 +4003,16 @@
     <hyperlink ref="C205" r:id="rId112" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
     <hyperlink ref="B206" r:id="rId113" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
     <hyperlink ref="C206" r:id="rId114" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
-    <hyperlink ref="B207" r:id="rId115" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
-    <hyperlink ref="C207" r:id="rId116" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
-    <hyperlink ref="B208" r:id="rId117" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
-    <hyperlink ref="C208" r:id="rId118" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
-    <hyperlink ref="B209" r:id="rId119" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
-    <hyperlink ref="B214" r:id="rId120" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
-    <hyperlink ref="C214" r:id="rId121" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
-    <hyperlink ref="B215" r:id="rId122" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
-    <hyperlink ref="C215" r:id="rId123" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
-    <hyperlink ref="B216" r:id="rId124" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
+    <hyperlink ref="B208" r:id="rId115" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
+    <hyperlink ref="C208" r:id="rId116" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
+    <hyperlink ref="B209" r:id="rId117" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
+    <hyperlink ref="C209" r:id="rId118" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
+    <hyperlink ref="B207" r:id="rId119" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
+    <hyperlink ref="B215" r:id="rId120" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
+    <hyperlink ref="C215" r:id="rId121" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
+    <hyperlink ref="B216" r:id="rId122" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
+    <hyperlink ref="C216" r:id="rId123" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
+    <hyperlink ref="B217" r:id="rId124" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
     <hyperlink ref="B85" r:id="rId125" display="https://leetcode.com/problems/minimum-depth-of-binary-tree/description/" xr:uid="{89D22C44-568D-2A43-84A7-D669E16D4993}"/>
     <hyperlink ref="C85" r:id="rId126" display="https://cspiration.com/login" xr:uid="{CDC90D9B-21B1-9F4E-BBAE-19128D12CFDA}"/>
     <hyperlink ref="B87" r:id="rId127" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/description/" xr:uid="{93D570CB-F2FC-D841-9EFB-185B9F3C2E70}"/>
@@ -3963,20 +4229,53 @@
     <hyperlink ref="C66" r:id="rId338" display="https://cspiration.com/login" xr:uid="{C5087984-A06B-4248-8E74-E2539F4CAF6A}"/>
     <hyperlink ref="B67" r:id="rId339" display="https://leetcode.com/problems/repeated-dna-sequences/description/" xr:uid="{52566213-99F8-BA41-B322-FDF32A868B37}"/>
     <hyperlink ref="C67" r:id="rId340" display="https://cspiration.com/login" xr:uid="{149752EA-7A00-384E-BE6B-4D94705BC736}"/>
-    <hyperlink ref="B222" r:id="rId341" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
-    <hyperlink ref="C222" r:id="rId342" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
-    <hyperlink ref="B223" r:id="rId343" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
-    <hyperlink ref="C223" r:id="rId344" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
-    <hyperlink ref="B224" r:id="rId345" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
-    <hyperlink ref="C224" r:id="rId346" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
-    <hyperlink ref="B226" r:id="rId347" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
-    <hyperlink ref="C226" r:id="rId348" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
-    <hyperlink ref="B231" r:id="rId349" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
-    <hyperlink ref="C231" r:id="rId350" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
+    <hyperlink ref="B223" r:id="rId341" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
+    <hyperlink ref="C223" r:id="rId342" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
+    <hyperlink ref="B224" r:id="rId343" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
+    <hyperlink ref="C224" r:id="rId344" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
+    <hyperlink ref="B225" r:id="rId345" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
+    <hyperlink ref="C225" r:id="rId346" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
+    <hyperlink ref="B227" r:id="rId347" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
+    <hyperlink ref="C227" r:id="rId348" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
+    <hyperlink ref="B233" r:id="rId349" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
+    <hyperlink ref="C233" r:id="rId350" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
     <hyperlink ref="B232" r:id="rId351" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
     <hyperlink ref="C232" r:id="rId352" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
-    <hyperlink ref="B233" r:id="rId353" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
-    <hyperlink ref="C233" r:id="rId354" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
+    <hyperlink ref="B234" r:id="rId353" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
+    <hyperlink ref="C234" r:id="rId354" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
+    <hyperlink ref="B239" r:id="rId355" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
+    <hyperlink ref="C239" r:id="rId356" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
+    <hyperlink ref="B240" r:id="rId357" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
+    <hyperlink ref="C240" r:id="rId358" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
+    <hyperlink ref="B241" r:id="rId359" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
+    <hyperlink ref="C241" r:id="rId360" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
+    <hyperlink ref="B242" r:id="rId361" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
+    <hyperlink ref="C242" r:id="rId362" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
+    <hyperlink ref="B243" r:id="rId363" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
+    <hyperlink ref="C243" r:id="rId364" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
+    <hyperlink ref="B244" r:id="rId365" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
+    <hyperlink ref="C244" r:id="rId366" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
+    <hyperlink ref="B245" r:id="rId367" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
+    <hyperlink ref="C245" r:id="rId368" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
+    <hyperlink ref="B246" r:id="rId369" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
+    <hyperlink ref="C246" r:id="rId370" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
+    <hyperlink ref="B247" r:id="rId371" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
+    <hyperlink ref="C247" r:id="rId372" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
+    <hyperlink ref="B248" r:id="rId373" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
+    <hyperlink ref="C248" r:id="rId374" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
+    <hyperlink ref="B249" r:id="rId375" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
+    <hyperlink ref="C249" r:id="rId376" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
+    <hyperlink ref="B250" r:id="rId377" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
+    <hyperlink ref="C250" r:id="rId378" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
+    <hyperlink ref="B251" r:id="rId379" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
+    <hyperlink ref="C251" r:id="rId380" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
+    <hyperlink ref="B252" r:id="rId381" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
+    <hyperlink ref="C252" r:id="rId382" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
+    <hyperlink ref="B253" r:id="rId383" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
+    <hyperlink ref="C253" r:id="rId384" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
+    <hyperlink ref="B254" r:id="rId385" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
+    <hyperlink ref="C254" r:id="rId386" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
+    <hyperlink ref="B255" r:id="rId387" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
5.20 review dfs&bfs, topo
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB878773-D308-774D-90AF-C1A147A4212C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55DC811D-5FB0-F747-B238-3346F021E73A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="291">
   <si>
     <t>144</t>
   </si>
@@ -903,6 +903,9 @@
   </si>
   <si>
     <t>Design HashSet</t>
+  </si>
+  <si>
+    <t>Longest String Chain</t>
   </si>
 </sst>
 </file>
@@ -1298,10 +1301,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
-  <dimension ref="A1:H323"/>
+  <dimension ref="A1:H324"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B125" sqref="B125"/>
+    <sheetView tabSelected="1" topLeftCell="A192" zoomScale="138" workbookViewId="0">
+      <selection activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2708,7 +2711,7 @@
       <c r="A122" s="7">
         <v>254</v>
       </c>
-      <c r="B122" s="3" t="s">
+      <c r="B122" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -2720,7 +2723,7 @@
       <c r="A123" s="7">
         <v>46</v>
       </c>
-      <c r="B123" s="3" t="s">
+      <c r="B123" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -2732,7 +2735,7 @@
       <c r="A124" s="7">
         <v>47</v>
       </c>
-      <c r="B124" s="3" t="s">
+      <c r="B124" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -2744,7 +2747,7 @@
       <c r="A125" s="7">
         <v>31</v>
       </c>
-      <c r="B125" s="3" t="s">
+      <c r="B125" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C125" s="2" t="s">
@@ -2840,7 +2843,7 @@
       <c r="A133" s="7">
         <v>93</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="B133" s="4" t="s">
         <v>288</v>
       </c>
     </row>
@@ -3059,56 +3062,54 @@
     </row>
     <row r="154" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A154" s="7">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B154" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C154" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="C154" s="2"/>
       <c r="D154" s="7"/>
     </row>
     <row r="155" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A155" s="7">
+        <v>85</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A156" s="7">
         <v>363</v>
       </c>
-      <c r="B155" s="4" t="s">
+      <c r="B156" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C155" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D155" s="7" t="s">
+      <c r="C156" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D156" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A156" s="7" t="s">
+    <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A157" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B156" s="8"/>
-      <c r="C156" s="7"/>
-      <c r="D156" s="7"/>
-    </row>
-    <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="7">
-        <v>198</v>
-      </c>
-      <c r="B157" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C157" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B157" s="8"/>
+      <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
     <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A158" s="7">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B158" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>2</v>
@@ -3117,10 +3118,10 @@
     </row>
     <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="7">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>2</v>
@@ -3129,10 +3130,10 @@
     </row>
     <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="7">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>2</v>
@@ -3141,10 +3142,10 @@
     </row>
     <row r="161" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="7">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>2</v>
@@ -3153,52 +3154,60 @@
     </row>
     <row r="162" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="7">
+        <v>10</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A163" s="7">
         <v>44</v>
       </c>
-      <c r="B162" s="4" t="s">
+      <c r="B163" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A165" s="6" t="s">
+    <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A164" s="7">
+        <v>1048</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A166" s="6" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B166" s="7"/>
-      <c r="C166" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B167" s="7"/>
+      <c r="C167" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A168" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B167" s="7"/>
-      <c r="C167" s="7"/>
-      <c r="D167" s="7"/>
-    </row>
-    <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="7">
-        <v>206</v>
-      </c>
-      <c r="B168" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B168" s="7"/>
+      <c r="C168" s="7"/>
       <c r="D168" s="7"/>
     </row>
     <row r="169" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="7">
-        <v>141</v>
+        <v>206</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>2</v>
@@ -3207,10 +3216,10 @@
     </row>
     <row r="170" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="7">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="B170" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>2</v>
@@ -3219,10 +3228,10 @@
     </row>
     <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="7">
-        <v>328</v>
+        <v>24</v>
       </c>
       <c r="B171" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>2</v>
@@ -3231,10 +3240,10 @@
     </row>
     <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="7">
-        <v>92</v>
+        <v>328</v>
       </c>
       <c r="B172" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>2</v>
@@ -3243,10 +3252,10 @@
     </row>
     <row r="173" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="7">
-        <v>237</v>
+        <v>92</v>
       </c>
       <c r="B173" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>2</v>
@@ -3255,10 +3264,10 @@
     </row>
     <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="7">
-        <v>19</v>
+        <v>237</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>2</v>
@@ -3267,10 +3276,10 @@
     </row>
     <row r="175" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="7">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>2</v>
@@ -3279,10 +3288,10 @@
     </row>
     <row r="176" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A176" s="7">
-        <v>203</v>
+        <v>83</v>
       </c>
       <c r="B176" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>2</v>
@@ -3291,10 +3300,10 @@
     </row>
     <row r="177" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A177" s="7">
-        <v>82</v>
+        <v>203</v>
       </c>
       <c r="B177" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>2</v>
@@ -3303,10 +3312,10 @@
     </row>
     <row r="178" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A178" s="7">
-        <v>369</v>
+        <v>82</v>
       </c>
       <c r="B178" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>2</v>
@@ -3315,10 +3324,10 @@
     </row>
     <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A179" s="7">
-        <v>2</v>
+        <v>369</v>
       </c>
       <c r="B179" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>2</v>
@@ -3327,10 +3336,10 @@
     </row>
     <row r="180" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="7">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="B180" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>2</v>
@@ -3339,42 +3348,42 @@
     </row>
     <row r="181" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="7">
+        <v>160</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C181" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D181" s="7"/>
+    </row>
+    <row r="182" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A182" s="7">
         <v>21</v>
       </c>
-      <c r="B181" s="4" t="s">
+      <c r="B182" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C181" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D181" s="7"/>
-    </row>
-    <row r="182" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="7" t="s">
+      <c r="C182" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D182" s="7"/>
+    </row>
+    <row r="183" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A183" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B182" s="8"/>
-      <c r="C182" s="7"/>
-      <c r="D182" s="7"/>
-    </row>
-    <row r="183" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="7">
-        <v>234</v>
-      </c>
-      <c r="B183" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C183" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B183" s="8"/>
+      <c r="C183" s="7"/>
       <c r="D183" s="7"/>
     </row>
     <row r="184" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="7">
-        <v>143</v>
+        <v>234</v>
       </c>
       <c r="B184" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3383,10 +3392,10 @@
     </row>
     <row r="185" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="7">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B185" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3395,10 +3404,10 @@
     </row>
     <row r="186" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="7">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B186" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3407,10 +3416,10 @@
     </row>
     <row r="187" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="7">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="B187" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3419,10 +3428,10 @@
     </row>
     <row r="188" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="7">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B188" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
@@ -3431,10 +3440,10 @@
     </row>
     <row r="189" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="7">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B189" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
@@ -3443,10 +3452,10 @@
     </row>
     <row r="190" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="7">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>2</v>
@@ -3455,44 +3464,44 @@
     </row>
     <row r="191" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="7">
+        <v>23</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A192" s="7">
         <v>147</v>
       </c>
-      <c r="B191" s="4" t="s">
+      <c r="B192" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="194" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A194" s="6" t="s">
+    <row r="195" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A195" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="195" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" s="7" t="s">
+    <row r="196" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A196" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B195" s="7"/>
-      <c r="C195" s="7" t="s">
+      <c r="B196" s="7"/>
+      <c r="C196" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="196" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="7">
-        <v>200</v>
-      </c>
-      <c r="B196" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C196" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D196" s="7"/>
     </row>
     <row r="197" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="7">
-        <v>286</v>
-      </c>
-      <c r="B197" s="4" t="s">
-        <v>131</v>
+        <v>200</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>2</v>
@@ -3501,10 +3510,10 @@
     </row>
     <row r="198" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="7">
-        <v>130</v>
-      </c>
-      <c r="B198" s="4" t="s">
-        <v>132</v>
+        <v>286</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>2</v>
@@ -3513,10 +3522,10 @@
     </row>
     <row r="199" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="7">
-        <v>339</v>
-      </c>
-      <c r="B199" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>2</v>
@@ -3525,10 +3534,10 @@
     </row>
     <row r="200" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="7">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>2</v>
@@ -3537,10 +3546,10 @@
     </row>
     <row r="201" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="7">
-        <v>127</v>
+        <v>364</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>2</v>
@@ -3549,75 +3558,75 @@
     </row>
     <row r="202" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="7">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C202" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D202" s="7"/>
     </row>
     <row r="203" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="7">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C203" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D203" s="7"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="204" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A204" s="7">
+        <v>51</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C204" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D204" s="7"/>
+    </row>
+    <row r="205" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A205" s="7">
         <v>52</v>
       </c>
-      <c r="B204" s="4" t="s">
+      <c r="B205" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C204" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D204" s="7"/>
-    </row>
-    <row r="207" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A207" s="7"/>
-      <c r="B207" s="4"/>
-      <c r="C207" s="2"/>
-      <c r="D207" s="7"/>
-    </row>
-    <row r="208" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A208" s="6" t="s">
+      <c r="C205" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D205" s="7"/>
+    </row>
+    <row r="208" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A208" s="7"/>
+      <c r="B208" s="4"/>
+      <c r="C208" s="2"/>
+      <c r="D208" s="7"/>
+    </row>
+    <row r="209" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A209" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B208" s="9"/>
-    </row>
-    <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A209" s="7" t="s">
+      <c r="B209" s="9"/>
+    </row>
+    <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A210" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B209" s="8"/>
-      <c r="C209" s="7" t="s">
+      <c r="B210" s="8"/>
+      <c r="C210" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A210" s="7">
-        <v>261</v>
-      </c>
-      <c r="B210" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="C210" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D210" s="7"/>
     </row>
     <row r="211" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="7">
-        <v>323</v>
+        <v>261</v>
       </c>
       <c r="B211" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>2</v>
@@ -3626,62 +3635,62 @@
     </row>
     <row r="212" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="7">
+        <v>323</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C212" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A213" s="7">
         <v>305</v>
       </c>
-      <c r="B212" s="4" t="s">
+      <c r="B213" s="4" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B213" s="9"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B214" s="9"/>
     </row>
-    <row r="215" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A215" s="6" t="s">
+    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B215" s="9"/>
+    </row>
+    <row r="216" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A216" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="B215" s="9"/>
-    </row>
-    <row r="216" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A216" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B216" s="8"/>
-      <c r="C216" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D216" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="B216" s="9"/>
     </row>
     <row r="217" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A217" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B217" s="8"/>
+      <c r="C217" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D217" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A218" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="B217" s="8"/>
-      <c r="C217" s="7"/>
-      <c r="D217" s="7"/>
-    </row>
-    <row r="218" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A218" s="7">
-        <v>133</v>
-      </c>
-      <c r="B218" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="C218" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B218" s="8"/>
+      <c r="C218" s="7"/>
       <c r="D218" s="7"/>
     </row>
     <row r="219" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A219" s="7">
-        <v>399</v>
+        <v>133</v>
       </c>
       <c r="B219" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>2</v>
@@ -3690,75 +3699,75 @@
     </row>
     <row r="220" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A220" s="7">
+        <v>399</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="C220" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D220" s="7"/>
+    </row>
+    <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A221" s="7">
         <v>310</v>
       </c>
-      <c r="B220" s="4" t="s">
+      <c r="B221" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="C220" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D220" s="7"/>
-    </row>
-    <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A221" s="7" t="s">
+      <c r="C221" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D221" s="7"/>
+    </row>
+    <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A222" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B221" s="8"/>
-      <c r="C221" s="7"/>
-      <c r="D221" s="7"/>
-    </row>
-    <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A222" s="7">
+      <c r="B222" s="8"/>
+      <c r="C222" s="7"/>
+      <c r="D222" s="7"/>
+    </row>
+    <row r="223" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A223" s="7">
         <v>149</v>
       </c>
-      <c r="B222" s="4" t="s">
+      <c r="B223" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="C222" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D222" s="7"/>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B223" s="9"/>
+      <c r="C223" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D223" s="7"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B224" s="9"/>
     </row>
-    <row r="225" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A225" s="6" t="s">
+    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B225" s="9"/>
+    </row>
+    <row r="226" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A226" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="B225" s="9"/>
-    </row>
-    <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="7" t="s">
+      <c r="B226" s="9"/>
+    </row>
+    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A227" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B226" s="8"/>
-      <c r="C226" s="7" t="s">
+      <c r="B227" s="8"/>
+      <c r="C227" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A227" s="7">
-        <v>208</v>
-      </c>
-      <c r="B227" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D227" s="7"/>
     </row>
     <row r="228" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="7">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B228" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>2</v>
@@ -3767,48 +3776,48 @@
     </row>
     <row r="229" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="7">
+        <v>211</v>
+      </c>
+      <c r="B229" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="B229" s="4" t="s">
+      <c r="C229" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D229" s="7"/>
+    </row>
+    <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A230" s="7">
+        <v>212</v>
+      </c>
+      <c r="B230" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="C229" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D229" s="7"/>
-    </row>
-    <row r="232" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A232" s="6" t="s">
+      <c r="C230" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D230" s="7"/>
+    </row>
+    <row r="233" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A233" s="6" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A233" s="7" t="s">
+    <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A234" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B233" s="7"/>
-      <c r="C233" s="7" t="s">
+      <c r="B234" s="7"/>
+      <c r="C234" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A234" s="7">
-        <v>48</v>
-      </c>
-      <c r="B234" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C234" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D234" s="7"/>
     </row>
     <row r="235" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A235" s="7">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C235" s="2" t="s">
         <v>2</v>
@@ -3817,10 +3826,10 @@
     </row>
     <row r="236" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="7">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C236" s="2" t="s">
         <v>2</v>
@@ -3829,10 +3838,10 @@
     </row>
     <row r="237" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A237" s="7">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C237" s="2" t="s">
         <v>2</v>
@@ -3841,10 +3850,10 @@
     </row>
     <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A238" s="7">
-        <v>311</v>
+        <v>73</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C238" s="2" t="s">
         <v>2</v>
@@ -3853,10 +3862,10 @@
     </row>
     <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="7">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>2</v>
@@ -3865,10 +3874,10 @@
     </row>
     <row r="240" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="7">
-        <v>378</v>
+        <v>329</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>2</v>
@@ -3877,10 +3886,10 @@
     </row>
     <row r="241" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A241" s="7">
-        <v>74</v>
+        <v>378</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>2</v>
@@ -3889,10 +3898,10 @@
     </row>
     <row r="242" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="7">
-        <v>240</v>
+        <v>74</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>2</v>
@@ -3901,10 +3910,10 @@
     </row>
     <row r="243" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="7">
-        <v>370</v>
+        <v>240</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>2</v>
@@ -3913,10 +3922,10 @@
     </row>
     <row r="244" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A244" s="7">
-        <v>79</v>
+        <v>370</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>2</v>
@@ -3925,10 +3934,10 @@
     </row>
     <row r="245" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A245" s="7">
-        <v>296</v>
+        <v>79</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C245" s="2" t="s">
         <v>2</v>
@@ -3937,10 +3946,10 @@
     </row>
     <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="7">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>2</v>
@@ -3949,10 +3958,10 @@
     </row>
     <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A247" s="7">
-        <v>317</v>
+        <v>361</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>2</v>
@@ -3961,10 +3970,10 @@
     </row>
     <row r="248" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="7">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>2</v>
@@ -3973,10 +3982,10 @@
     </row>
     <row r="249" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="7">
-        <v>36</v>
+        <v>302</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>2</v>
@@ -3985,51 +3994,51 @@
     </row>
     <row r="250" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A250" s="7">
+        <v>36</v>
+      </c>
+      <c r="B250" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C250" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D250" s="7"/>
+    </row>
+    <row r="251" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A251" s="7">
         <v>37</v>
       </c>
-      <c r="B250" s="2" t="s">
+      <c r="B251" s="2" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="254" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A254" s="6" t="s">
+    <row r="255" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A255" s="6" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A255" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B255" s="7"/>
-      <c r="C255" s="7"/>
-      <c r="D255" s="7"/>
     </row>
     <row r="256" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A256" s="7" t="s">
-        <v>234</v>
+        <v>53</v>
       </c>
       <c r="B256" s="7"/>
       <c r="C256" s="7"/>
       <c r="D256" s="7"/>
     </row>
     <row r="257" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A257" s="7">
-        <v>155</v>
-      </c>
-      <c r="B257" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C257" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A257" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B257" s="7"/>
+      <c r="C257" s="7"/>
       <c r="D257" s="7"/>
     </row>
     <row r="258" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A258" s="7">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4038,10 +4047,10 @@
     </row>
     <row r="259" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="7">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4050,10 +4059,10 @@
     </row>
     <row r="260" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" s="7">
-        <v>150</v>
+        <v>225</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4062,10 +4071,10 @@
     </row>
     <row r="261" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A261" s="7">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -4074,10 +4083,10 @@
     </row>
     <row r="262" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" s="7">
-        <v>388</v>
+        <v>71</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>2</v>
@@ -4086,10 +4095,10 @@
     </row>
     <row r="263" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A263" s="7">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>2</v>
@@ -4098,10 +4107,10 @@
     </row>
     <row r="264" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A264" s="7">
-        <v>224</v>
-      </c>
-      <c r="B264" s="4" t="s">
-        <v>242</v>
+        <v>394</v>
+      </c>
+      <c r="B264" s="2" t="s">
+        <v>241</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>2</v>
@@ -4110,10 +4119,10 @@
     </row>
     <row r="265" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="7">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B265" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>2</v>
@@ -4122,10 +4131,10 @@
     </row>
     <row r="266" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" s="7">
-        <v>385</v>
+        <v>227</v>
       </c>
       <c r="B266" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>2</v>
@@ -4134,42 +4143,42 @@
     </row>
     <row r="267" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A267" s="7">
+        <v>385</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C267" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D267" s="7"/>
+    </row>
+    <row r="268" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A268" s="7">
         <v>84</v>
       </c>
-      <c r="B267" s="4" t="s">
+      <c r="B268" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C267" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D267" s="7"/>
-    </row>
-    <row r="268" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A268" s="7" t="s">
+      <c r="C268" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D268" s="7"/>
+    </row>
+    <row r="269" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A269" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="B268" s="8"/>
-      <c r="C268" s="7"/>
-      <c r="D268" s="7"/>
-    </row>
-    <row r="269" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A269" s="7">
-        <v>215</v>
-      </c>
-      <c r="B269" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C269" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B269" s="8"/>
+      <c r="C269" s="7"/>
       <c r="D269" s="7"/>
     </row>
     <row r="270" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A270" s="7">
-        <v>347</v>
+        <v>215</v>
       </c>
       <c r="B270" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>2</v>
@@ -4178,10 +4187,10 @@
     </row>
     <row r="271" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" s="7">
-        <v>218</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>249</v>
+        <v>347</v>
+      </c>
+      <c r="B271" s="4" t="s">
+        <v>248</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>2</v>
@@ -4190,10 +4199,10 @@
     </row>
     <row r="272" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A272" s="7">
-        <v>332</v>
-      </c>
-      <c r="B272" s="3" t="s">
-        <v>250</v>
+        <v>218</v>
+      </c>
+      <c r="B272" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>2</v>
@@ -4202,47 +4211,47 @@
     </row>
     <row r="273" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A273" s="7">
+        <v>332</v>
+      </c>
+      <c r="B273" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D273" s="7"/>
+    </row>
+    <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A274" s="7">
         <v>341</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="B274" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="274" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B274" s="9"/>
-    </row>
-    <row r="277" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A277" s="6" t="s">
+    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B275" s="9"/>
+    </row>
+    <row r="278" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A278" s="6" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="278" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A278" s="7" t="s">
+    <row r="279" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A279" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B278" s="7"/>
-      <c r="C278" s="7" t="s">
+      <c r="B279" s="7"/>
+      <c r="C279" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="279" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A279" s="7">
-        <v>389</v>
-      </c>
-      <c r="B279" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="C279" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D279" s="7"/>
     </row>
     <row r="280" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" s="7">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="B280" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>2</v>
@@ -4251,44 +4260,44 @@
     </row>
     <row r="281" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="7">
+        <v>136</v>
+      </c>
+      <c r="B281" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="C281" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D281" s="7"/>
+    </row>
+    <row r="282" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A282" s="7">
         <v>318</v>
       </c>
-      <c r="B281" s="4" t="s">
+      <c r="B282" s="4" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="284" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A284" s="6" t="s">
+    <row r="285" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A285" s="6" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="285" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A285" s="7" t="s">
+    <row r="286" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A286" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B285" s="7"/>
-      <c r="C285" s="7" t="s">
+      <c r="B286" s="7"/>
+      <c r="C286" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="286" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A286" s="7">
-        <v>207</v>
-      </c>
-      <c r="B286" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C286" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D286" s="7"/>
     </row>
     <row r="287" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A287" s="7">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C287" s="2" t="s">
         <v>2</v>
@@ -4297,44 +4306,44 @@
     </row>
     <row r="288" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A288" s="7">
+        <v>210</v>
+      </c>
+      <c r="B288" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="C288" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D288" s="7"/>
+    </row>
+    <row r="289" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A289" s="7">
         <v>269</v>
       </c>
-      <c r="B288" s="2" t="s">
+      <c r="B289" s="2" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="291" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A291" s="6" t="s">
+    <row r="292" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A292" s="6" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="292" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A292" s="7" t="s">
+    <row r="293" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A293" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B292" s="7"/>
-      <c r="C292" s="7" t="s">
+      <c r="B293" s="7"/>
+      <c r="C293" s="7" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="293" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A293" s="7">
-        <v>384</v>
-      </c>
-      <c r="B293" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="C293" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D293" s="7"/>
     </row>
     <row r="294" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A294" s="7">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B294" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>2</v>
@@ -4343,10 +4352,10 @@
     </row>
     <row r="295" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A295" s="7">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>2</v>
@@ -4355,10 +4364,10 @@
     </row>
     <row r="296" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A296" s="7">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>2</v>
@@ -4367,10 +4376,10 @@
     </row>
     <row r="297" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A297" s="7">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C297" s="2" t="s">
         <v>2</v>
@@ -4379,69 +4388,69 @@
     </row>
     <row r="298" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A298" s="7">
+        <v>381</v>
+      </c>
+      <c r="B298" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C298" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D298" s="7"/>
+    </row>
+    <row r="299" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A299" s="7">
         <v>138</v>
       </c>
-      <c r="B298" s="2" t="s">
+      <c r="B299" s="2" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="301" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A301" s="6" t="s">
+    <row r="302" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A302" s="6" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="302" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A302" s="7" t="s">
+    <row r="303" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A303" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B302" s="7"/>
-      <c r="C302" s="7"/>
-      <c r="D302" s="7"/>
-    </row>
-    <row r="303" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A303" s="7">
-        <v>359</v>
-      </c>
-      <c r="B303" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="C303" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B303" s="7"/>
+      <c r="C303" s="7"/>
       <c r="D303" s="7"/>
     </row>
     <row r="304" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A304" s="7">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="B304" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C304" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D304" s="7" t="s">
-        <v>179</v>
-      </c>
+      <c r="D304" s="7"/>
     </row>
     <row r="305" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A305" s="7">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B305" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C305" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D305" s="7"/>
+      <c r="D305" s="7" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="306" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A306" s="7">
-        <v>281</v>
+        <v>362</v>
       </c>
       <c r="B306" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C306" s="2" t="s">
         <v>2</v>
@@ -4450,10 +4459,10 @@
     </row>
     <row r="307" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A307" s="7">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B307" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C307" s="2" t="s">
         <v>2</v>
@@ -4462,10 +4471,10 @@
     </row>
     <row r="308" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A308" s="7">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="B308" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>2</v>
@@ -4474,10 +4483,10 @@
     </row>
     <row r="309" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A309" s="7">
-        <v>288</v>
+        <v>251</v>
       </c>
       <c r="B309" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>2</v>
@@ -4486,10 +4495,10 @@
     </row>
     <row r="310" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A310" s="7">
-        <v>170</v>
-      </c>
-      <c r="B310" s="2" t="s">
-        <v>275</v>
+        <v>288</v>
+      </c>
+      <c r="B310" s="4" t="s">
+        <v>274</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>2</v>
@@ -4498,10 +4507,10 @@
     </row>
     <row r="311" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A311" s="7">
-        <v>348</v>
+        <v>170</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -4510,10 +4519,10 @@
     </row>
     <row r="312" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A312" s="7">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -4522,10 +4531,10 @@
     </row>
     <row r="313" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A313" s="7">
-        <v>353</v>
+        <v>379</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C313" s="2" t="s">
         <v>2</v>
@@ -4534,10 +4543,10 @@
     </row>
     <row r="314" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A314" s="7">
-        <v>146</v>
+        <v>353</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C314" s="2" t="s">
         <v>2</v>
@@ -4546,10 +4555,10 @@
     </row>
     <row r="315" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A315" s="7">
-        <v>355</v>
+        <v>146</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C315" s="2" t="s">
         <v>2</v>
@@ -4558,10 +4567,10 @@
     </row>
     <row r="316" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A316" s="7">
-        <v>303</v>
+        <v>355</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C316" s="2" t="s">
         <v>2</v>
@@ -4570,10 +4579,10 @@
     </row>
     <row r="317" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A317" s="7">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C317" s="2" t="s">
         <v>2</v>
@@ -4582,24 +4591,22 @@
     </row>
     <row r="318" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A318" s="7">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D318" s="7" t="s">
-        <v>284</v>
-      </c>
+      <c r="D318" s="7"/>
     </row>
     <row r="319" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A319" s="7">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
@@ -4610,22 +4617,36 @@
     </row>
     <row r="320" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A320" s="7">
+        <v>308</v>
+      </c>
+      <c r="B320" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D320" s="7" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A321" s="7">
         <v>705</v>
       </c>
-      <c r="B320" s="2" t="s">
+      <c r="B321" s="2" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="322" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A322" s="7">
+    <row r="323" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A323" s="7">
         <v>3.31</v>
       </c>
     </row>
-    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A323">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324">
         <v>697</v>
       </c>
-      <c r="B323" t="s">
+      <c r="B324" t="s">
         <v>287</v>
       </c>
     </row>
@@ -4674,88 +4695,88 @@
     <hyperlink ref="C152" r:id="rId41" display="https://cspiration.com/login" xr:uid="{6C5529D1-8C55-094E-A7F6-EE2EE2045AA3}"/>
     <hyperlink ref="B153" r:id="rId42" display="https://leetcode.com/problems/maximal-square/description/" xr:uid="{4A8B0E3C-5E97-5C47-9A6E-2C2EDA6A9395}"/>
     <hyperlink ref="C153" r:id="rId43" display="https://cspiration.com/login" xr:uid="{74A87B70-E6B2-4E4F-922E-9B55F53872E6}"/>
-    <hyperlink ref="B154" r:id="rId44" display="https://leetcode.com/problems/maximal-rectangle/description/" xr:uid="{3ADA6959-F24D-6146-B3F0-E982EB0C68F5}"/>
-    <hyperlink ref="C154" r:id="rId45" display="https://cspiration.com/login" xr:uid="{8B14C05B-DD8F-D443-8EAA-F17CA50D7366}"/>
-    <hyperlink ref="B155" r:id="rId46" display="https://leetcode.com/problems/max-sum-of-rectangle-no-larger-than-k/description/" xr:uid="{4AA58D7A-2220-7E48-94A8-240A6AFC7EB7}"/>
-    <hyperlink ref="C155" r:id="rId47" display="https://cspiration.com/login" xr:uid="{38081C3C-1B84-3A42-8B82-08867C75BE08}"/>
-    <hyperlink ref="B157" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
-    <hyperlink ref="C157" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
-    <hyperlink ref="B158" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
-    <hyperlink ref="C158" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
-    <hyperlink ref="B159" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
-    <hyperlink ref="C159" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
-    <hyperlink ref="B160" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
-    <hyperlink ref="C160" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
-    <hyperlink ref="B161" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
-    <hyperlink ref="C161" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
-    <hyperlink ref="B162" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
-    <hyperlink ref="B168" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
-    <hyperlink ref="C168" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
-    <hyperlink ref="B169" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
-    <hyperlink ref="C169" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
-    <hyperlink ref="B170" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
-    <hyperlink ref="C170" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
-    <hyperlink ref="B171" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
-    <hyperlink ref="C171" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
-    <hyperlink ref="B172" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
-    <hyperlink ref="C172" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
-    <hyperlink ref="B173" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
-    <hyperlink ref="C173" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
-    <hyperlink ref="B174" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
-    <hyperlink ref="C174" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
-    <hyperlink ref="B175" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
-    <hyperlink ref="C175" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
-    <hyperlink ref="B176" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
-    <hyperlink ref="C176" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
-    <hyperlink ref="B177" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
-    <hyperlink ref="C177" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
-    <hyperlink ref="B178" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
-    <hyperlink ref="C178" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
-    <hyperlink ref="B179" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
-    <hyperlink ref="C179" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
-    <hyperlink ref="B180" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
-    <hyperlink ref="C180" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
-    <hyperlink ref="B181" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
-    <hyperlink ref="C181" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
-    <hyperlink ref="B183" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
-    <hyperlink ref="C183" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
-    <hyperlink ref="B184" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
-    <hyperlink ref="C184" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
-    <hyperlink ref="B185" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
-    <hyperlink ref="C185" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
-    <hyperlink ref="B186" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
-    <hyperlink ref="C186" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
-    <hyperlink ref="B187" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
-    <hyperlink ref="C187" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
-    <hyperlink ref="B188" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
-    <hyperlink ref="C188" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
-    <hyperlink ref="B189" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
-    <hyperlink ref="C189" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
-    <hyperlink ref="B190" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
-    <hyperlink ref="C190" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
-    <hyperlink ref="B191" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
-    <hyperlink ref="B196" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
-    <hyperlink ref="C196" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
-    <hyperlink ref="B197" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
-    <hyperlink ref="C197" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
-    <hyperlink ref="B198" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
-    <hyperlink ref="C198" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
-    <hyperlink ref="B199" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
-    <hyperlink ref="C199" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
-    <hyperlink ref="B200" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
-    <hyperlink ref="C200" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
-    <hyperlink ref="B201" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
-    <hyperlink ref="C201" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
-    <hyperlink ref="B203" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
-    <hyperlink ref="C203" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
-    <hyperlink ref="B204" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
-    <hyperlink ref="C204" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
-    <hyperlink ref="B202" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
-    <hyperlink ref="B210" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
-    <hyperlink ref="C210" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
-    <hyperlink ref="B211" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
-    <hyperlink ref="C211" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
-    <hyperlink ref="B212" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
+    <hyperlink ref="B155" r:id="rId44" display="https://leetcode.com/problems/maximal-rectangle/description/" xr:uid="{3ADA6959-F24D-6146-B3F0-E982EB0C68F5}"/>
+    <hyperlink ref="C155" r:id="rId45" display="https://cspiration.com/login" xr:uid="{8B14C05B-DD8F-D443-8EAA-F17CA50D7366}"/>
+    <hyperlink ref="B156" r:id="rId46" display="https://leetcode.com/problems/max-sum-of-rectangle-no-larger-than-k/description/" xr:uid="{4AA58D7A-2220-7E48-94A8-240A6AFC7EB7}"/>
+    <hyperlink ref="C156" r:id="rId47" display="https://cspiration.com/login" xr:uid="{38081C3C-1B84-3A42-8B82-08867C75BE08}"/>
+    <hyperlink ref="B158" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
+    <hyperlink ref="C158" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
+    <hyperlink ref="B159" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
+    <hyperlink ref="C159" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
+    <hyperlink ref="B160" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
+    <hyperlink ref="C160" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
+    <hyperlink ref="B161" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
+    <hyperlink ref="C161" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
+    <hyperlink ref="B162" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
+    <hyperlink ref="C162" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
+    <hyperlink ref="B163" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
+    <hyperlink ref="B169" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
+    <hyperlink ref="C169" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
+    <hyperlink ref="B170" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
+    <hyperlink ref="C170" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
+    <hyperlink ref="B171" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
+    <hyperlink ref="C171" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
+    <hyperlink ref="B172" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
+    <hyperlink ref="C172" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
+    <hyperlink ref="B173" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
+    <hyperlink ref="C173" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
+    <hyperlink ref="B174" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
+    <hyperlink ref="C174" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
+    <hyperlink ref="B175" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
+    <hyperlink ref="C175" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
+    <hyperlink ref="B176" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
+    <hyperlink ref="C176" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
+    <hyperlink ref="B177" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
+    <hyperlink ref="C177" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
+    <hyperlink ref="B178" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
+    <hyperlink ref="C178" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
+    <hyperlink ref="B179" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
+    <hyperlink ref="C179" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
+    <hyperlink ref="B180" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
+    <hyperlink ref="C180" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
+    <hyperlink ref="B181" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
+    <hyperlink ref="C181" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
+    <hyperlink ref="B182" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
+    <hyperlink ref="C182" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
+    <hyperlink ref="B184" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
+    <hyperlink ref="C184" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
+    <hyperlink ref="B185" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
+    <hyperlink ref="C185" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
+    <hyperlink ref="B186" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
+    <hyperlink ref="C186" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
+    <hyperlink ref="B187" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
+    <hyperlink ref="C187" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
+    <hyperlink ref="B188" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
+    <hyperlink ref="C188" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
+    <hyperlink ref="B189" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
+    <hyperlink ref="C189" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
+    <hyperlink ref="B190" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
+    <hyperlink ref="C190" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
+    <hyperlink ref="B191" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
+    <hyperlink ref="C191" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
+    <hyperlink ref="B192" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
+    <hyperlink ref="B197" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
+    <hyperlink ref="C197" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
+    <hyperlink ref="B198" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
+    <hyperlink ref="C198" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
+    <hyperlink ref="B199" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
+    <hyperlink ref="C199" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
+    <hyperlink ref="B200" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
+    <hyperlink ref="C200" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
+    <hyperlink ref="B201" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
+    <hyperlink ref="C201" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
+    <hyperlink ref="B202" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
+    <hyperlink ref="C202" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
+    <hyperlink ref="B204" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
+    <hyperlink ref="C204" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
+    <hyperlink ref="B205" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
+    <hyperlink ref="C205" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
+    <hyperlink ref="B203" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
+    <hyperlink ref="B211" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
+    <hyperlink ref="C211" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
+    <hyperlink ref="B212" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
+    <hyperlink ref="C212" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
+    <hyperlink ref="B213" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
     <hyperlink ref="B80" r:id="rId126" display="https://leetcode.com/problems/minimum-depth-of-binary-tree/description/" xr:uid="{89D22C44-568D-2A43-84A7-D669E16D4993}"/>
     <hyperlink ref="C80" r:id="rId127" display="https://cspiration.com/login" xr:uid="{CDC90D9B-21B1-9F4E-BBAE-19128D12CFDA}"/>
     <hyperlink ref="B82" r:id="rId128" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/description/" xr:uid="{93D570CB-F2FC-D841-9EFB-185B9F3C2E70}"/>
@@ -4966,141 +4987,143 @@
     <hyperlink ref="C61" r:id="rId333" display="https://cspiration.com/login" xr:uid="{C5087984-A06B-4248-8E74-E2539F4CAF6A}"/>
     <hyperlink ref="B62" r:id="rId334" display="https://leetcode.com/problems/repeated-dna-sequences/description/" xr:uid="{52566213-99F8-BA41-B322-FDF32A868B37}"/>
     <hyperlink ref="C62" r:id="rId335" display="https://cspiration.com/login" xr:uid="{149752EA-7A00-384E-BE6B-4D94705BC736}"/>
-    <hyperlink ref="B218" r:id="rId336" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
-    <hyperlink ref="C218" r:id="rId337" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
-    <hyperlink ref="B219" r:id="rId338" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
-    <hyperlink ref="C219" r:id="rId339" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
-    <hyperlink ref="B220" r:id="rId340" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
-    <hyperlink ref="C220" r:id="rId341" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
-    <hyperlink ref="B222" r:id="rId342" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
-    <hyperlink ref="C222" r:id="rId343" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
-    <hyperlink ref="B228" r:id="rId344" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
-    <hyperlink ref="C228" r:id="rId345" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
-    <hyperlink ref="B227" r:id="rId346" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
-    <hyperlink ref="C227" r:id="rId347" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
-    <hyperlink ref="B229" r:id="rId348" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
-    <hyperlink ref="C229" r:id="rId349" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
-    <hyperlink ref="B234" r:id="rId350" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
-    <hyperlink ref="C234" r:id="rId351" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
-    <hyperlink ref="B235" r:id="rId352" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
-    <hyperlink ref="C235" r:id="rId353" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
-    <hyperlink ref="B236" r:id="rId354" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
-    <hyperlink ref="C236" r:id="rId355" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
-    <hyperlink ref="B237" r:id="rId356" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
-    <hyperlink ref="C237" r:id="rId357" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
-    <hyperlink ref="B238" r:id="rId358" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
-    <hyperlink ref="C238" r:id="rId359" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
-    <hyperlink ref="B239" r:id="rId360" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
-    <hyperlink ref="C239" r:id="rId361" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
-    <hyperlink ref="B240" r:id="rId362" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
-    <hyperlink ref="C240" r:id="rId363" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
-    <hyperlink ref="B241" r:id="rId364" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
-    <hyperlink ref="C241" r:id="rId365" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
-    <hyperlink ref="B242" r:id="rId366" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
-    <hyperlink ref="C242" r:id="rId367" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
-    <hyperlink ref="B243" r:id="rId368" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
-    <hyperlink ref="C243" r:id="rId369" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
-    <hyperlink ref="B244" r:id="rId370" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
-    <hyperlink ref="C244" r:id="rId371" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
-    <hyperlink ref="B245" r:id="rId372" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
-    <hyperlink ref="C245" r:id="rId373" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
-    <hyperlink ref="B246" r:id="rId374" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
-    <hyperlink ref="C246" r:id="rId375" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
-    <hyperlink ref="B247" r:id="rId376" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
-    <hyperlink ref="C247" r:id="rId377" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
-    <hyperlink ref="B248" r:id="rId378" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
-    <hyperlink ref="C248" r:id="rId379" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
-    <hyperlink ref="B249" r:id="rId380" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
-    <hyperlink ref="C249" r:id="rId381" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
-    <hyperlink ref="B250" r:id="rId382" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
-    <hyperlink ref="B257" r:id="rId383" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
-    <hyperlink ref="C257" r:id="rId384" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
-    <hyperlink ref="B258" r:id="rId385" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{156CAAE5-6351-9947-BB71-247BCB4199E4}"/>
-    <hyperlink ref="C258" r:id="rId386" display="https://cspiration.com/login" xr:uid="{B32FCD33-3793-1145-9B85-1C19988C5512}"/>
-    <hyperlink ref="B259" r:id="rId387" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{988FA989-097D-3643-AFD0-51D5DE85FC28}"/>
-    <hyperlink ref="C259" r:id="rId388" display="https://cspiration.com/login" xr:uid="{236098E8-3353-2343-96D1-B31CFD341154}"/>
-    <hyperlink ref="B260" r:id="rId389" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
-    <hyperlink ref="C260" r:id="rId390" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
-    <hyperlink ref="B261" r:id="rId391" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
-    <hyperlink ref="C261" r:id="rId392" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
-    <hyperlink ref="B262" r:id="rId393" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
-    <hyperlink ref="C262" r:id="rId394" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
-    <hyperlink ref="B263" r:id="rId395" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
-    <hyperlink ref="C263" r:id="rId396" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
-    <hyperlink ref="B264" r:id="rId397" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
-    <hyperlink ref="C264" r:id="rId398" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
-    <hyperlink ref="B265" r:id="rId399" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
-    <hyperlink ref="C265" r:id="rId400" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
-    <hyperlink ref="B266" r:id="rId401" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
-    <hyperlink ref="C266" r:id="rId402" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
-    <hyperlink ref="B267" r:id="rId403" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
-    <hyperlink ref="C267" r:id="rId404" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
-    <hyperlink ref="B269" r:id="rId405" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
-    <hyperlink ref="C269" r:id="rId406" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
-    <hyperlink ref="B270" r:id="rId407" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
-    <hyperlink ref="C270" r:id="rId408" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
-    <hyperlink ref="B271" r:id="rId409" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
-    <hyperlink ref="C271" r:id="rId410" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
-    <hyperlink ref="B272" r:id="rId411" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
-    <hyperlink ref="C272" r:id="rId412" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
-    <hyperlink ref="B273" r:id="rId413" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
-    <hyperlink ref="B279" r:id="rId414" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
-    <hyperlink ref="C279" r:id="rId415" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
-    <hyperlink ref="B280" r:id="rId416" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
-    <hyperlink ref="C280" r:id="rId417" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
-    <hyperlink ref="B281" r:id="rId418" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
-    <hyperlink ref="B286" r:id="rId419" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
-    <hyperlink ref="C286" r:id="rId420" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
-    <hyperlink ref="B287" r:id="rId421" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
-    <hyperlink ref="C287" r:id="rId422" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
-    <hyperlink ref="B288" r:id="rId423" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
-    <hyperlink ref="B293" r:id="rId424" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
-    <hyperlink ref="C293" r:id="rId425" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
-    <hyperlink ref="B294" r:id="rId426" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
-    <hyperlink ref="C294" r:id="rId427" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
-    <hyperlink ref="B295" r:id="rId428" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
-    <hyperlink ref="C295" r:id="rId429" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
-    <hyperlink ref="B296" r:id="rId430" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
-    <hyperlink ref="C296" r:id="rId431" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
-    <hyperlink ref="B297" r:id="rId432" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
-    <hyperlink ref="C297" r:id="rId433" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
-    <hyperlink ref="B298" r:id="rId434" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
-    <hyperlink ref="B303" r:id="rId435" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
-    <hyperlink ref="C303" r:id="rId436" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
-    <hyperlink ref="B304" r:id="rId437" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
-    <hyperlink ref="C304" r:id="rId438" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
-    <hyperlink ref="B305" r:id="rId439" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
-    <hyperlink ref="C305" r:id="rId440" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
-    <hyperlink ref="B306" r:id="rId441" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
-    <hyperlink ref="C306" r:id="rId442" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
-    <hyperlink ref="B307" r:id="rId443" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
-    <hyperlink ref="C307" r:id="rId444" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
-    <hyperlink ref="B308" r:id="rId445" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
-    <hyperlink ref="C308" r:id="rId446" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
-    <hyperlink ref="B309" r:id="rId447" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
-    <hyperlink ref="C309" r:id="rId448" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
-    <hyperlink ref="B310" r:id="rId449" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
-    <hyperlink ref="C310" r:id="rId450" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
-    <hyperlink ref="B311" r:id="rId451" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
-    <hyperlink ref="C311" r:id="rId452" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
-    <hyperlink ref="B312" r:id="rId453" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
-    <hyperlink ref="C312" r:id="rId454" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
-    <hyperlink ref="B313" r:id="rId455" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
-    <hyperlink ref="C313" r:id="rId456" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
-    <hyperlink ref="B314" r:id="rId457" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
-    <hyperlink ref="C314" r:id="rId458" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
-    <hyperlink ref="B315" r:id="rId459" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
-    <hyperlink ref="C315" r:id="rId460" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
-    <hyperlink ref="B316" r:id="rId461" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
-    <hyperlink ref="C316" r:id="rId462" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
-    <hyperlink ref="B317" r:id="rId463" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
-    <hyperlink ref="C317" r:id="rId464" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
-    <hyperlink ref="B318" r:id="rId465" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
-    <hyperlink ref="C318" r:id="rId466" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
-    <hyperlink ref="B319" r:id="rId467" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
-    <hyperlink ref="C319" r:id="rId468" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
-    <hyperlink ref="B320" r:id="rId469" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
+    <hyperlink ref="B219" r:id="rId336" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
+    <hyperlink ref="C219" r:id="rId337" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
+    <hyperlink ref="B220" r:id="rId338" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
+    <hyperlink ref="C220" r:id="rId339" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
+    <hyperlink ref="B221" r:id="rId340" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
+    <hyperlink ref="C221" r:id="rId341" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
+    <hyperlink ref="B223" r:id="rId342" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
+    <hyperlink ref="C223" r:id="rId343" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
+    <hyperlink ref="B229" r:id="rId344" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
+    <hyperlink ref="C229" r:id="rId345" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
+    <hyperlink ref="B228" r:id="rId346" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
+    <hyperlink ref="C228" r:id="rId347" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
+    <hyperlink ref="B230" r:id="rId348" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
+    <hyperlink ref="C230" r:id="rId349" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
+    <hyperlink ref="B235" r:id="rId350" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
+    <hyperlink ref="C235" r:id="rId351" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
+    <hyperlink ref="B236" r:id="rId352" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
+    <hyperlink ref="C236" r:id="rId353" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
+    <hyperlink ref="B237" r:id="rId354" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
+    <hyperlink ref="C237" r:id="rId355" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
+    <hyperlink ref="B238" r:id="rId356" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
+    <hyperlink ref="C238" r:id="rId357" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
+    <hyperlink ref="B239" r:id="rId358" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
+    <hyperlink ref="C239" r:id="rId359" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
+    <hyperlink ref="B240" r:id="rId360" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
+    <hyperlink ref="C240" r:id="rId361" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
+    <hyperlink ref="B241" r:id="rId362" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
+    <hyperlink ref="C241" r:id="rId363" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
+    <hyperlink ref="B242" r:id="rId364" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
+    <hyperlink ref="C242" r:id="rId365" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
+    <hyperlink ref="B243" r:id="rId366" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
+    <hyperlink ref="C243" r:id="rId367" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
+    <hyperlink ref="B244" r:id="rId368" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
+    <hyperlink ref="C244" r:id="rId369" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
+    <hyperlink ref="B245" r:id="rId370" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
+    <hyperlink ref="C245" r:id="rId371" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
+    <hyperlink ref="B246" r:id="rId372" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
+    <hyperlink ref="C246" r:id="rId373" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
+    <hyperlink ref="B247" r:id="rId374" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
+    <hyperlink ref="C247" r:id="rId375" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
+    <hyperlink ref="B248" r:id="rId376" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
+    <hyperlink ref="C248" r:id="rId377" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
+    <hyperlink ref="B249" r:id="rId378" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
+    <hyperlink ref="C249" r:id="rId379" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
+    <hyperlink ref="B250" r:id="rId380" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
+    <hyperlink ref="C250" r:id="rId381" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
+    <hyperlink ref="B251" r:id="rId382" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
+    <hyperlink ref="B258" r:id="rId383" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
+    <hyperlink ref="C258" r:id="rId384" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
+    <hyperlink ref="B259" r:id="rId385" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{156CAAE5-6351-9947-BB71-247BCB4199E4}"/>
+    <hyperlink ref="C259" r:id="rId386" display="https://cspiration.com/login" xr:uid="{B32FCD33-3793-1145-9B85-1C19988C5512}"/>
+    <hyperlink ref="B260" r:id="rId387" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{988FA989-097D-3643-AFD0-51D5DE85FC28}"/>
+    <hyperlink ref="C260" r:id="rId388" display="https://cspiration.com/login" xr:uid="{236098E8-3353-2343-96D1-B31CFD341154}"/>
+    <hyperlink ref="B261" r:id="rId389" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
+    <hyperlink ref="C261" r:id="rId390" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
+    <hyperlink ref="B262" r:id="rId391" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
+    <hyperlink ref="C262" r:id="rId392" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
+    <hyperlink ref="B263" r:id="rId393" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
+    <hyperlink ref="C263" r:id="rId394" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
+    <hyperlink ref="B264" r:id="rId395" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
+    <hyperlink ref="C264" r:id="rId396" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
+    <hyperlink ref="B265" r:id="rId397" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
+    <hyperlink ref="C265" r:id="rId398" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
+    <hyperlink ref="B266" r:id="rId399" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
+    <hyperlink ref="C266" r:id="rId400" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
+    <hyperlink ref="B267" r:id="rId401" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
+    <hyperlink ref="C267" r:id="rId402" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
+    <hyperlink ref="B268" r:id="rId403" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
+    <hyperlink ref="C268" r:id="rId404" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
+    <hyperlink ref="B270" r:id="rId405" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
+    <hyperlink ref="C270" r:id="rId406" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
+    <hyperlink ref="B271" r:id="rId407" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
+    <hyperlink ref="C271" r:id="rId408" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
+    <hyperlink ref="B272" r:id="rId409" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
+    <hyperlink ref="C272" r:id="rId410" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
+    <hyperlink ref="B273" r:id="rId411" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
+    <hyperlink ref="C273" r:id="rId412" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
+    <hyperlink ref="B274" r:id="rId413" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
+    <hyperlink ref="B280" r:id="rId414" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
+    <hyperlink ref="C280" r:id="rId415" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
+    <hyperlink ref="B281" r:id="rId416" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
+    <hyperlink ref="C281" r:id="rId417" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
+    <hyperlink ref="B282" r:id="rId418" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
+    <hyperlink ref="B287" r:id="rId419" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
+    <hyperlink ref="C287" r:id="rId420" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
+    <hyperlink ref="B288" r:id="rId421" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
+    <hyperlink ref="C288" r:id="rId422" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
+    <hyperlink ref="B289" r:id="rId423" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
+    <hyperlink ref="B294" r:id="rId424" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
+    <hyperlink ref="C294" r:id="rId425" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
+    <hyperlink ref="B295" r:id="rId426" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
+    <hyperlink ref="C295" r:id="rId427" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
+    <hyperlink ref="B296" r:id="rId428" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
+    <hyperlink ref="C296" r:id="rId429" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
+    <hyperlink ref="B297" r:id="rId430" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
+    <hyperlink ref="C297" r:id="rId431" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
+    <hyperlink ref="B298" r:id="rId432" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
+    <hyperlink ref="C298" r:id="rId433" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
+    <hyperlink ref="B299" r:id="rId434" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
+    <hyperlink ref="B304" r:id="rId435" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
+    <hyperlink ref="C304" r:id="rId436" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
+    <hyperlink ref="B305" r:id="rId437" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
+    <hyperlink ref="C305" r:id="rId438" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
+    <hyperlink ref="B306" r:id="rId439" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
+    <hyperlink ref="C306" r:id="rId440" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
+    <hyperlink ref="B307" r:id="rId441" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
+    <hyperlink ref="C307" r:id="rId442" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
+    <hyperlink ref="B308" r:id="rId443" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
+    <hyperlink ref="C308" r:id="rId444" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
+    <hyperlink ref="B309" r:id="rId445" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
+    <hyperlink ref="C309" r:id="rId446" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
+    <hyperlink ref="B310" r:id="rId447" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
+    <hyperlink ref="C310" r:id="rId448" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
+    <hyperlink ref="B311" r:id="rId449" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
+    <hyperlink ref="C311" r:id="rId450" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
+    <hyperlink ref="B312" r:id="rId451" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
+    <hyperlink ref="C312" r:id="rId452" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
+    <hyperlink ref="B313" r:id="rId453" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
+    <hyperlink ref="C313" r:id="rId454" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
+    <hyperlink ref="B314" r:id="rId455" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
+    <hyperlink ref="C314" r:id="rId456" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
+    <hyperlink ref="B315" r:id="rId457" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
+    <hyperlink ref="C315" r:id="rId458" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
+    <hyperlink ref="B316" r:id="rId459" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
+    <hyperlink ref="C316" r:id="rId460" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
+    <hyperlink ref="B317" r:id="rId461" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
+    <hyperlink ref="C317" r:id="rId462" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
+    <hyperlink ref="B318" r:id="rId463" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
+    <hyperlink ref="C318" r:id="rId464" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
+    <hyperlink ref="B319" r:id="rId465" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
+    <hyperlink ref="C319" r:id="rId466" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
+    <hyperlink ref="B320" r:id="rId467" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
+    <hyperlink ref="C320" r:id="rId468" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
+    <hyperlink ref="B321" r:id="rId469" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
     <hyperlink ref="B133" r:id="rId470" xr:uid="{6E505C5D-7486-774A-8436-0B2D9A806CE7}"/>
+    <hyperlink ref="B154" r:id="rId471" xr:uid="{8066B6F4-349C-104A-B6B1-4C5FDFBC5FE9}"/>
+    <hyperlink ref="B164" r:id="rId472" xr:uid="{13747061-B8D2-6041-B323-BA395125DCAA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
added ms practiced Questions, updated track
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B37D3B-E712-8A45-8EA2-01EC9A104E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEE86D7-B59B-3544-85B7-E149783DB13F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="310">
   <si>
     <t>144</t>
   </si>
@@ -743,179 +743,233 @@
     <t>Min Stack</t>
   </si>
   <si>
+    <t>Evaluate Reverse Polish Notation</t>
+  </si>
+  <si>
+    <t>Simplify Path</t>
+  </si>
+  <si>
+    <t>Longest Absolute File Path</t>
+  </si>
+  <si>
+    <t>Decode String</t>
+  </si>
+  <si>
+    <t>Basic Calculator</t>
+  </si>
+  <si>
+    <t>Basic Calculator II</t>
+  </si>
+  <si>
+    <t>Mini Parser</t>
+  </si>
+  <si>
+    <t>Largest Rectangle in Histogram</t>
+  </si>
+  <si>
+    <t>PriorityQueue</t>
+  </si>
+  <si>
+    <t>Kth Largest Element in an Array</t>
+  </si>
+  <si>
+    <t>Top K Frequent Elements</t>
+  </si>
+  <si>
+    <t>The Skyline Problem</t>
+  </si>
+  <si>
+    <t>Reconstruct Itinerary</t>
+  </si>
+  <si>
+    <t>Flatten Nested List Iterator</t>
+  </si>
+  <si>
+    <t>Bit Manipulation</t>
+  </si>
+  <si>
+    <t>Find the Difference</t>
+  </si>
+  <si>
+    <t>Single Number</t>
+  </si>
+  <si>
+    <t>Maximum Product of Word Lengths</t>
+  </si>
+  <si>
+    <t>Topological Sort</t>
+  </si>
+  <si>
+    <t>Course Schedule</t>
+  </si>
+  <si>
+    <t>Course Schedule II</t>
+  </si>
+  <si>
+    <t>Alien Dictionary</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Shuffle an Array</t>
+  </si>
+  <si>
+    <t>Random Pick Index</t>
+  </si>
+  <si>
+    <t>Linked List Random Node</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1)</t>
+  </si>
+  <si>
+    <t>Insert Delete GetRandom O(1) - Duplicates allowed</t>
+  </si>
+  <si>
+    <t>Copy List with Random Pointer</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Logger Rate Limiter</t>
+  </si>
+  <si>
+    <t>Moving Average from Data Stream</t>
+  </si>
+  <si>
+    <t>Design Hit Counter</t>
+  </si>
+  <si>
+    <t>Zigzag Iterator</t>
+  </si>
+  <si>
+    <t>Peeking Iterator</t>
+  </si>
+  <si>
+    <t>Flatten 2D Vector</t>
+  </si>
+  <si>
+    <t>Unique Word Abbreviation</t>
+  </si>
+  <si>
+    <t>Two Sum III - Data structure design</t>
+  </si>
+  <si>
+    <t>Design Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>Design Phone Directory</t>
+  </si>
+  <si>
+    <t>Design Snake Game</t>
+  </si>
+  <si>
+    <t>LRU Cache</t>
+  </si>
+  <si>
+    <t>Design Twitter</t>
+  </si>
+  <si>
+    <t>Range Sum Query - Immutable</t>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Immutable</t>
+  </si>
+  <si>
+    <t>Range Sum Query - Mutable</t>
+  </si>
+  <si>
+    <t>BIT &amp; ST</t>
+  </si>
+  <si>
+    <t>Range Sum Query 2D - Mutable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                       </t>
+  </si>
+  <si>
+    <t>Degree of an Array</t>
+  </si>
+  <si>
+    <t>Restore IP Addresses</t>
+  </si>
+  <si>
+    <t>Design HashSet</t>
+  </si>
+  <si>
+    <t>Longest String Chain</t>
+  </si>
+  <si>
+    <t>Critical Connections in a Network</t>
+  </si>
+  <si>
+    <t>Binary Search</t>
+  </si>
+  <si>
+    <t>Search Insert Position</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Search in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array</t>
+  </si>
+  <si>
+    <t>Find Minimum in Rotated Sorted Array II</t>
+  </si>
+  <si>
+    <t>Find Peak Element </t>
+  </si>
+  <si>
+    <t>Guess Number Higher or Lower</t>
+  </si>
+  <si>
+    <t>Find First and Last Position of Element in Sorted Array</t>
+  </si>
+  <si>
+    <t>Count of Smaller Numbers After Self</t>
+  </si>
+  <si>
+    <t>Longest Increasing Subsequence</t>
+  </si>
+  <si>
+    <t>Russian Doll Envelopes</t>
+  </si>
+  <si>
+    <t>Hash table</t>
+  </si>
+  <si>
+    <t>Keyboard Row</t>
+  </si>
+  <si>
+    <t>Largest 1-Bordered Square</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>Tallest Billboard</t>
+  </si>
+  <si>
+    <t>Remove Outermost Parentheses</t>
+  </si>
+  <si>
     <t>Implement Queue using Stacks</t>
   </si>
   <si>
     <t>Implement Stack using Queues</t>
-  </si>
-  <si>
-    <t>Evaluate Reverse Polish Notation</t>
-  </si>
-  <si>
-    <t>Simplify Path</t>
-  </si>
-  <si>
-    <t>Longest Absolute File Path</t>
-  </si>
-  <si>
-    <t>Decode String</t>
-  </si>
-  <si>
-    <t>Basic Calculator</t>
-  </si>
-  <si>
-    <t>Basic Calculator II</t>
-  </si>
-  <si>
-    <t>Mini Parser</t>
-  </si>
-  <si>
-    <t>Largest Rectangle in Histogram</t>
-  </si>
-  <si>
-    <t>PriorityQueue</t>
-  </si>
-  <si>
-    <t>Kth Largest Element in an Array</t>
-  </si>
-  <si>
-    <t>Top K Frequent Elements</t>
-  </si>
-  <si>
-    <t>The Skyline Problem</t>
-  </si>
-  <si>
-    <t>Reconstruct Itinerary</t>
-  </si>
-  <si>
-    <t>Flatten Nested List Iterator</t>
-  </si>
-  <si>
-    <t>Bit Manipulation</t>
-  </si>
-  <si>
-    <t>Find the Difference</t>
-  </si>
-  <si>
-    <t>Single Number</t>
-  </si>
-  <si>
-    <t>Maximum Product of Word Lengths</t>
-  </si>
-  <si>
-    <t>Topological Sort</t>
-  </si>
-  <si>
-    <t>Course Schedule</t>
-  </si>
-  <si>
-    <t>Course Schedule II</t>
-  </si>
-  <si>
-    <t>Alien Dictionary</t>
-  </si>
-  <si>
-    <t>Random</t>
-  </si>
-  <si>
-    <t>Shuffle an Array</t>
-  </si>
-  <si>
-    <t>Random Pick Index</t>
-  </si>
-  <si>
-    <t>Linked List Random Node</t>
-  </si>
-  <si>
-    <t>Insert Delete GetRandom O(1)</t>
-  </si>
-  <si>
-    <t>Insert Delete GetRandom O(1) - Duplicates allowed</t>
-  </si>
-  <si>
-    <t>Copy List with Random Pointer</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Logger Rate Limiter</t>
-  </si>
-  <si>
-    <t>Moving Average from Data Stream</t>
-  </si>
-  <si>
-    <t>Design Hit Counter</t>
-  </si>
-  <si>
-    <t>Zigzag Iterator</t>
-  </si>
-  <si>
-    <t>Peeking Iterator</t>
-  </si>
-  <si>
-    <t>Flatten 2D Vector</t>
-  </si>
-  <si>
-    <t>Unique Word Abbreviation</t>
-  </si>
-  <si>
-    <t>Two Sum III - Data structure design</t>
-  </si>
-  <si>
-    <t>Design Tic-Tac-Toe</t>
-  </si>
-  <si>
-    <t>Design Phone Directory</t>
-  </si>
-  <si>
-    <t>Design Snake Game</t>
-  </si>
-  <si>
-    <t>LRU Cache</t>
-  </si>
-  <si>
-    <t>Design Twitter</t>
-  </si>
-  <si>
-    <t>Range Sum Query - Immutable</t>
-  </si>
-  <si>
-    <t>Range Sum Query 2D - Immutable</t>
-  </si>
-  <si>
-    <t>Range Sum Query - Mutable</t>
-  </si>
-  <si>
-    <t>BIT &amp; ST</t>
-  </si>
-  <si>
-    <t>Range Sum Query 2D - Mutable</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                       </t>
-  </si>
-  <si>
-    <t>Degree of an Array</t>
-  </si>
-  <si>
-    <t>Restore IP Addresses</t>
-  </si>
-  <si>
-    <t>Design HashSet</t>
-  </si>
-  <si>
-    <t>Longest String Chain</t>
-  </si>
-  <si>
-    <t>Critical Connections in a Network</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -950,6 +1004,14 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -972,7 +1034,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -982,6 +1044,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1297,10 +1360,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
-  <dimension ref="A1:H324"/>
+  <dimension ref="A1:H357"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="138" workbookViewId="0">
-      <selection activeCell="B230" sqref="B230"/>
+    <sheetView tabSelected="1" topLeftCell="A272" zoomScale="150" workbookViewId="0">
+      <selection activeCell="C271" sqref="C271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1433,7 +1496,7 @@
       </c>
       <c r="D11" s="6"/>
       <c r="H11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -2840,7 +2903,7 @@
         <v>93</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="25" x14ac:dyDescent="0.25">
@@ -3061,7 +3124,7 @@
         <v>84</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C154" s="2"/>
       <c r="D154" s="6"/>
@@ -3093,31 +3156,22 @@
       </c>
     </row>
     <row r="157" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A157" s="6" t="s">
+      <c r="D157" s="6"/>
+    </row>
+    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A158" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B157" s="7"/>
-      <c r="C157" s="6"/>
-      <c r="D157" s="6"/>
-    </row>
-    <row r="158" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="6">
-        <v>198</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C158" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B158" s="7"/>
+      <c r="C158" s="6"/>
       <c r="D158" s="6"/>
     </row>
     <row r="159" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A159" s="6">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>2</v>
@@ -3126,10 +3180,10 @@
     </row>
     <row r="160" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A160" s="6">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>2</v>
@@ -3138,10 +3192,10 @@
     </row>
     <row r="161" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A161" s="6">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>2</v>
@@ -3150,10 +3204,10 @@
     </row>
     <row r="162" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A162" s="6">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>2</v>
@@ -3162,180 +3216,137 @@
     </row>
     <row r="163" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A163" s="6">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C163" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D163" s="6"/>
     </row>
     <row r="164" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A164" s="6">
+        <v>44</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A165" s="6">
         <v>1048</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A166" s="5" t="s">
-        <v>103</v>
-      </c>
+      <c r="B165" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A166" s="6" t="s">
+        <v>305</v>
+      </c>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A167" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B167" s="6"/>
-      <c r="C167" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="A167" s="6">
+        <v>746</v>
+      </c>
+      <c r="B167" s="3"/>
+      <c r="C167" s="2"/>
     </row>
     <row r="168" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A168" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B168" s="6"/>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
+      <c r="A168" s="6">
+        <v>1025</v>
+      </c>
+      <c r="B168" s="3"/>
+      <c r="C168" s="2"/>
     </row>
     <row r="169" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A169" s="6">
-        <v>206</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D169" s="6"/>
+        <v>1139</v>
+      </c>
+      <c r="B169" s="3"/>
+      <c r="C169" s="2"/>
     </row>
     <row r="170" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A170" s="6">
-        <v>141</v>
+        <v>1139</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D170" s="6"/>
+        <v>304</v>
+      </c>
+      <c r="C170" s="2"/>
     </row>
     <row r="171" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A171" s="6">
-        <v>24</v>
-      </c>
-      <c r="B171" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C171" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D171" s="6"/>
+        <v>740</v>
+      </c>
+      <c r="C171" s="2"/>
     </row>
     <row r="172" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A172" s="6">
-        <v>328</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D172" s="6"/>
+        <v>464</v>
+      </c>
+      <c r="B172" s="3"/>
+      <c r="C172" s="2"/>
     </row>
     <row r="173" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A173" s="6">
-        <v>92</v>
-      </c>
-      <c r="B173" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D173" s="6"/>
+        <v>523</v>
+      </c>
+      <c r="B173" s="3"/>
+      <c r="C173" s="2"/>
     </row>
     <row r="174" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A174" s="6">
-        <v>237</v>
+        <v>956</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D174" s="6"/>
+        <v>306</v>
+      </c>
+      <c r="C174" s="2"/>
     </row>
     <row r="175" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A175" s="6">
-        <v>19</v>
-      </c>
-      <c r="B175" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C175" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D175" s="6"/>
+        <v>1320</v>
+      </c>
+      <c r="B175" s="3"/>
+      <c r="C175" s="2"/>
     </row>
     <row r="176" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A176" s="6">
-        <v>83</v>
-      </c>
-      <c r="B176" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D176" s="6"/>
-    </row>
-    <row r="177" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A177" s="6">
-        <v>203</v>
-      </c>
-      <c r="B177" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D177" s="6"/>
+      <c r="A176" s="6"/>
+      <c r="B176" s="3"/>
+      <c r="C176" s="2"/>
+    </row>
+    <row r="177" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A177" s="5" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="178" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A178" s="6">
-        <v>82</v>
-      </c>
-      <c r="B178" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D178" s="6"/>
+      <c r="A178" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B178" s="6"/>
+      <c r="C178" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="179" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A179" s="6">
-        <v>369</v>
-      </c>
-      <c r="B179" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C179" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A179" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B179" s="6"/>
+      <c r="C179" s="6"/>
       <c r="D179" s="6"/>
     </row>
     <row r="180" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A180" s="6">
-        <v>2</v>
+        <v>206</v>
       </c>
       <c r="B180" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>2</v>
@@ -3344,10 +3355,10 @@
     </row>
     <row r="181" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A181" s="6">
-        <v>160</v>
+        <v>141</v>
       </c>
       <c r="B181" s="3" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>2</v>
@@ -3356,10 +3367,10 @@
     </row>
     <row r="182" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A182" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B182" s="3" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="C182" s="2" t="s">
         <v>2</v>
@@ -3367,19 +3378,23 @@
       <c r="D182" s="6"/>
     </row>
     <row r="183" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="B183" s="7"/>
-      <c r="C183" s="6"/>
+      <c r="A183" s="6">
+        <v>328</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C183" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D183" s="6"/>
     </row>
     <row r="184" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A184" s="6">
-        <v>234</v>
+        <v>92</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>2</v>
@@ -3388,10 +3403,10 @@
     </row>
     <row r="185" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A185" s="6">
-        <v>143</v>
+        <v>237</v>
       </c>
       <c r="B185" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>2</v>
@@ -3400,10 +3415,10 @@
     </row>
     <row r="186" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A186" s="6">
-        <v>142</v>
+        <v>19</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>2</v>
@@ -3412,10 +3427,10 @@
     </row>
     <row r="187" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A187" s="6">
-        <v>148</v>
+        <v>83</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>2</v>
@@ -3424,10 +3439,10 @@
     </row>
     <row r="188" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A188" s="6">
-        <v>25</v>
+        <v>203</v>
       </c>
       <c r="B188" s="3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>2</v>
@@ -3436,10 +3451,10 @@
     </row>
     <row r="189" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A189" s="6">
-        <v>61</v>
+        <v>82</v>
       </c>
       <c r="B189" s="3" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>2</v>
@@ -3448,10 +3463,10 @@
     </row>
     <row r="190" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A190" s="6">
-        <v>86</v>
+        <v>369</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>2</v>
@@ -3460,10 +3475,10 @@
     </row>
     <row r="191" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A191" s="6">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>2</v>
@@ -3472,32 +3487,66 @@
     </row>
     <row r="192" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A192" s="6">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="B192" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="195" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A195" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D192" s="6"/>
+    </row>
+    <row r="193" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A193" s="6">
+        <v>21</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D193" s="6"/>
+    </row>
+    <row r="194" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A194" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="B194" s="7"/>
+      <c r="C194" s="6"/>
+      <c r="D194" s="6"/>
+    </row>
+    <row r="195" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A195" s="6">
+        <v>234</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C195" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D195" s="6"/>
     </row>
     <row r="196" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B196" s="6"/>
-      <c r="C196" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="A196" s="6">
+        <v>143</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C196" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D196" s="6"/>
     </row>
     <row r="197" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A197" s="6">
-        <v>200</v>
+        <v>142</v>
       </c>
       <c r="B197" s="3" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>2</v>
@@ -3506,10 +3555,10 @@
     </row>
     <row r="198" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A198" s="6">
-        <v>286</v>
+        <v>148</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>2</v>
@@ -3518,10 +3567,10 @@
     </row>
     <row r="199" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A199" s="6">
-        <v>130</v>
+        <v>25</v>
       </c>
       <c r="B199" s="3" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>2</v>
@@ -3530,10 +3579,10 @@
     </row>
     <row r="200" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A200" s="6">
-        <v>339</v>
+        <v>61</v>
       </c>
       <c r="B200" s="3" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>2</v>
@@ -3542,10 +3591,10 @@
     </row>
     <row r="201" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A201" s="6">
-        <v>364</v>
+        <v>86</v>
       </c>
       <c r="B201" s="3" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>2</v>
@@ -3554,10 +3603,10 @@
     </row>
     <row r="202" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A202" s="6">
+        <v>23</v>
+      </c>
+      <c r="B202" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="B202" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>2</v>
@@ -3566,71 +3615,68 @@
     </row>
     <row r="203" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A203" s="6">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B203" s="3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="204" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A204" s="6">
-        <v>51</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C204" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D204" s="6"/>
-    </row>
-    <row r="205" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A205" s="6">
-        <v>52</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="C205" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D205" s="6"/>
-    </row>
-    <row r="206" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A206" s="6">
-        <v>1192</v>
-      </c>
-      <c r="B206" s="3" t="s">
-        <v>291</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A206" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A207" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B207" s="6"/>
+      <c r="C207" s="6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="208" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A208" s="6"/>
-      <c r="B208" s="3"/>
-      <c r="C208" s="2"/>
+      <c r="A208" s="6">
+        <v>200</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C208" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D208" s="6"/>
     </row>
-    <row r="209" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A209" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B209" s="8"/>
+    <row r="209" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A209" s="6">
+        <v>286</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C209" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D209" s="6"/>
     </row>
     <row r="210" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A210" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B210" s="7"/>
-      <c r="C210" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="A210" s="6">
+        <v>130</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C210" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D210" s="6"/>
     </row>
     <row r="211" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A211" s="6">
-        <v>261</v>
+        <v>339</v>
       </c>
       <c r="B211" s="3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C211" s="2" t="s">
         <v>2</v>
@@ -3639,10 +3685,10 @@
     </row>
     <row r="212" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A212" s="6">
-        <v>323</v>
+        <v>364</v>
       </c>
       <c r="B212" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>2</v>
@@ -3651,225 +3697,224 @@
     </row>
     <row r="213" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A213" s="6">
-        <v>305</v>
+        <v>127</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B214" s="8"/>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B215" s="8"/>
-    </row>
-    <row r="216" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A216" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="B216" s="8"/>
+        <v>135</v>
+      </c>
+      <c r="C213" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D213" s="6"/>
+    </row>
+    <row r="214" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A214" s="6">
+        <v>126</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A215" s="6">
+        <v>51</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C215" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D215" s="6"/>
+    </row>
+    <row r="216" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A216" s="6">
+        <v>52</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C216" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D216" s="6"/>
     </row>
     <row r="217" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A217" s="6" t="s">
+      <c r="A217" s="6">
+        <v>1192</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A219" s="6"/>
+      <c r="B219" s="3"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="6"/>
+    </row>
+    <row r="220" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A220" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B220" s="8"/>
+    </row>
+    <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A221" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B217" s="7"/>
-      <c r="C217" s="6" t="s">
+      <c r="B221" s="7"/>
+      <c r="C221" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="D217" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A218" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="B218" s="7"/>
-      <c r="C218" s="6"/>
-      <c r="D218" s="6"/>
-    </row>
-    <row r="219" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A219" s="6">
-        <v>133</v>
-      </c>
-      <c r="B219" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="C219" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D219" s="6"/>
-    </row>
-    <row r="220" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A220" s="6">
-        <v>399</v>
-      </c>
-      <c r="B220" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="C220" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D220" s="6"/>
-    </row>
-    <row r="221" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A221" s="6">
-        <v>310</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="C221" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D221" s="6"/>
     </row>
     <row r="222" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A222" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="B222" s="7"/>
-      <c r="C222" s="6"/>
+      <c r="A222" s="6">
+        <v>261</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C222" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D222" s="6"/>
     </row>
     <row r="223" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A223" s="6">
-        <v>149</v>
+        <v>323</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>210</v>
+        <v>141</v>
       </c>
       <c r="C223" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D223" s="6"/>
     </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B224" s="8"/>
+    <row r="224" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A224" s="6">
+        <v>305</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B225" s="8"/>
     </row>
-    <row r="226" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A226" s="5" t="s">
-        <v>211</v>
-      </c>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B226" s="8"/>
     </row>
-    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A227" s="6" t="s">
+    <row r="227" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A227" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B227" s="8"/>
+    </row>
+    <row r="228" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A228" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B227" s="7"/>
-      <c r="C227" s="6" t="s">
+      <c r="B228" s="7"/>
+      <c r="C228" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A228" s="6">
-        <v>208</v>
-      </c>
-      <c r="B228" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="C228" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D228" s="6"/>
+      <c r="D228" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="229" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A229" s="6">
-        <v>211</v>
-      </c>
-      <c r="B229" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C229" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A229" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B229" s="7"/>
+      <c r="C229" s="6"/>
       <c r="D229" s="6"/>
     </row>
     <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" s="6">
-        <v>212</v>
+        <v>133</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D230" s="6"/>
     </row>
-    <row r="233" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A233" s="5" t="s">
-        <v>215</v>
-      </c>
+    <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A231" s="6">
+        <v>399</v>
+      </c>
+      <c r="B231" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C231" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D231" s="6"/>
+    </row>
+    <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A232" s="6">
+        <v>310</v>
+      </c>
+      <c r="B232" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C232" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D232" s="6"/>
+    </row>
+    <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A233" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="B233" s="7"/>
+      <c r="C233" s="6"/>
+      <c r="D233" s="6"/>
     </row>
     <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A234" s="6" t="s">
+      <c r="A234" s="6">
+        <v>149</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D234" s="6"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B235" s="8"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B236" s="8"/>
+    </row>
+    <row r="237" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A237" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B237" s="8"/>
+    </row>
+    <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A238" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B234" s="6"/>
-      <c r="C234" s="6" t="s">
+      <c r="B238" s="7"/>
+      <c r="C238" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A235" s="6">
-        <v>48</v>
-      </c>
-      <c r="B235" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D235" s="6"/>
-    </row>
-    <row r="236" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A236" s="6">
-        <v>54</v>
-      </c>
-      <c r="B236" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="C236" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D236" s="6"/>
-    </row>
-    <row r="237" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A237" s="6">
-        <v>59</v>
-      </c>
-      <c r="B237" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C237" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D237" s="6"/>
-    </row>
-    <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A238" s="6">
-        <v>73</v>
-      </c>
-      <c r="B238" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C238" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D238" s="6"/>
     </row>
     <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A239" s="6">
-        <v>311</v>
-      </c>
-      <c r="B239" s="2" t="s">
-        <v>220</v>
+        <v>208</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>213</v>
       </c>
       <c r="C239" s="2" t="s">
         <v>2</v>
@@ -3878,10 +3923,10 @@
     </row>
     <row r="240" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="6">
-        <v>329</v>
-      </c>
-      <c r="B240" s="2" t="s">
-        <v>221</v>
+        <v>211</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>212</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>2</v>
@@ -3890,70 +3935,36 @@
     </row>
     <row r="241" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A241" s="6">
-        <v>378</v>
-      </c>
-      <c r="B241" s="2" t="s">
-        <v>222</v>
+        <v>212</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>214</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D241" s="6"/>
     </row>
-    <row r="242" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A242" s="6">
-        <v>74</v>
-      </c>
-      <c r="B242" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C242" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D242" s="6"/>
-    </row>
-    <row r="243" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A243" s="6">
-        <v>240</v>
-      </c>
-      <c r="B243" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C243" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D243" s="6"/>
-    </row>
-    <row r="244" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A244" s="6">
-        <v>370</v>
-      </c>
-      <c r="B244" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C244" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D244" s="6"/>
+    <row r="244" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A244" s="5" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="245" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A245" s="6">
-        <v>79</v>
-      </c>
-      <c r="B245" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C245" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D245" s="6"/>
+      <c r="A245" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B245" s="6"/>
+      <c r="C245" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A246" s="6">
-        <v>296</v>
+        <v>48</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="C246" s="2" t="s">
         <v>2</v>
@@ -3962,10 +3973,10 @@
     </row>
     <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A247" s="6">
-        <v>361</v>
+        <v>54</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C247" s="2" t="s">
         <v>2</v>
@@ -3974,10 +3985,10 @@
     </row>
     <row r="248" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="6">
-        <v>317</v>
+        <v>59</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C248" s="2" t="s">
         <v>2</v>
@@ -3986,10 +3997,10 @@
     </row>
     <row r="249" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="6">
-        <v>302</v>
+        <v>73</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C249" s="2" t="s">
         <v>2</v>
@@ -3998,10 +4009,10 @@
     </row>
     <row r="250" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A250" s="6">
-        <v>36</v>
+        <v>311</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C250" s="2" t="s">
         <v>2</v>
@@ -4010,39 +4021,94 @@
     </row>
     <row r="251" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A251" s="6">
-        <v>37</v>
+        <v>329</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="255" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A255" s="5" t="s">
-        <v>233</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="C251" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D251" s="6"/>
+    </row>
+    <row r="252" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A252" s="6">
+        <v>378</v>
+      </c>
+      <c r="B252" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C252" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D252" s="6"/>
+    </row>
+    <row r="253" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A253" s="6">
+        <v>74</v>
+      </c>
+      <c r="B253" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C253" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D253" s="6"/>
+    </row>
+    <row r="254" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A254" s="6">
+        <v>240</v>
+      </c>
+      <c r="B254" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C254" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D254" s="6"/>
+    </row>
+    <row r="255" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A255" s="6">
+        <v>370</v>
+      </c>
+      <c r="B255" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C255" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D255" s="6"/>
     </row>
     <row r="256" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A256" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B256" s="6"/>
-      <c r="C256" s="6"/>
+      <c r="A256" s="6">
+        <v>79</v>
+      </c>
+      <c r="B256" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C256" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D256" s="6"/>
     </row>
     <row r="257" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A257" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="B257" s="6"/>
-      <c r="C257" s="6"/>
+      <c r="A257" s="6">
+        <v>296</v>
+      </c>
+      <c r="B257" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C257" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D257" s="6"/>
     </row>
     <row r="258" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A258" s="6">
-        <v>155</v>
+        <v>361</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="C258" s="2" t="s">
         <v>2</v>
@@ -4051,10 +4117,10 @@
     </row>
     <row r="259" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="6">
-        <v>232</v>
+        <v>317</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="C259" s="2" t="s">
         <v>2</v>
@@ -4063,10 +4129,10 @@
     </row>
     <row r="260" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A260" s="6">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="C260" s="2" t="s">
         <v>2</v>
@@ -4075,10 +4141,10 @@
     </row>
     <row r="261" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A261" s="6">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -4087,126 +4153,71 @@
     </row>
     <row r="262" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" s="6">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C262" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D262" s="6"/>
-    </row>
-    <row r="263" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A263" s="6">
-        <v>388</v>
-      </c>
-      <c r="B263" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C263" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D263" s="6"/>
-    </row>
-    <row r="264" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A264" s="6">
-        <v>394</v>
-      </c>
-      <c r="B264" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="C264" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D264" s="6"/>
-    </row>
-    <row r="265" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A265" s="6">
-        <v>224</v>
-      </c>
-      <c r="B265" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C265" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D265" s="6"/>
-    </row>
-    <row r="266" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A266" s="6">
-        <v>227</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="C266" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D266" s="6"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="266" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A266" s="5" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="267" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A267" s="6">
-        <v>385</v>
-      </c>
-      <c r="B267" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="C267" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A267" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B267" s="6"/>
+      <c r="C267" s="6"/>
       <c r="D267" s="6"/>
     </row>
     <row r="268" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A268" s="6">
-        <v>84</v>
-      </c>
-      <c r="B268" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="C268" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A268" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="B268" s="6"/>
+      <c r="C268" s="6"/>
       <c r="D268" s="6"/>
     </row>
     <row r="269" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A269" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="B269" s="7"/>
-      <c r="C269" s="6"/>
+      <c r="A269" s="6">
+        <v>155</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="C269" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D269" s="6"/>
     </row>
     <row r="270" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A270" s="6">
-        <v>215</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>247</v>
+      <c r="A270" s="1">
+        <v>232</v>
+      </c>
+      <c r="B270" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D270" s="6"/>
+      <c r="D270" s="1"/>
     </row>
     <row r="271" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A271" s="6">
-        <v>347</v>
-      </c>
-      <c r="B271" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C271" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D271" s="6"/>
+      <c r="A271" s="1">
+        <v>225</v>
+      </c>
+      <c r="B271" s="2" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="272" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A272" s="6">
-        <v>218</v>
+        <v>150</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>2</v>
@@ -4215,10 +4226,10 @@
     </row>
     <row r="273" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A273" s="6">
-        <v>332</v>
+        <v>71</v>
       </c>
       <c r="B273" s="3" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C273" s="2" t="s">
         <v>2</v>
@@ -4227,47 +4238,90 @@
     </row>
     <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A274" s="6">
-        <v>341</v>
+        <v>388</v>
       </c>
       <c r="B274" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="275" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B275" s="8"/>
-    </row>
-    <row r="278" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A278" s="5" t="s">
-        <v>252</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="C274" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D274" s="6"/>
+    </row>
+    <row r="275" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A275" s="6">
+        <v>394</v>
+      </c>
+      <c r="B275" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C275" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D275" s="6"/>
+    </row>
+    <row r="276" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A276" s="6">
+        <v>224</v>
+      </c>
+      <c r="B276" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="C276" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D276" s="6"/>
+    </row>
+    <row r="277" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A277" s="6">
+        <v>227</v>
+      </c>
+      <c r="B277" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C277" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D277" s="6"/>
+    </row>
+    <row r="278" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A278" s="6">
+        <v>385</v>
+      </c>
+      <c r="B278" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C278" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D278" s="6"/>
     </row>
     <row r="279" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A279" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B279" s="6"/>
-      <c r="C279" s="6" t="s">
-        <v>54</v>
-      </c>
+      <c r="A279" s="6">
+        <v>84</v>
+      </c>
+      <c r="B279" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="C279" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D279" s="6"/>
     </row>
     <row r="280" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A280" s="6">
-        <v>389</v>
-      </c>
-      <c r="B280" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="C280" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A280" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="B280" s="7"/>
+      <c r="C280" s="6"/>
       <c r="D280" s="6"/>
     </row>
     <row r="281" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="6">
-        <v>136</v>
+        <v>215</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
@@ -4276,61 +4330,71 @@
     </row>
     <row r="282" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A282" s="6">
-        <v>318</v>
+        <v>347</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="285" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A285" s="5" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="286" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A286" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B286" s="6"/>
-      <c r="C286" s="6" t="s">
-        <v>54</v>
-      </c>
+        <v>246</v>
+      </c>
+      <c r="C282" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D282" s="6"/>
+    </row>
+    <row r="283" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A283" s="6">
+        <v>218</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D283" s="6"/>
+    </row>
+    <row r="284" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A284" s="6">
+        <v>332</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C284" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D284" s="6"/>
+    </row>
+    <row r="285" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A285" s="6">
+        <v>341</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="286" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A286" t="s">
+        <v>305</v>
+      </c>
+      <c r="B286" s="8"/>
     </row>
     <row r="287" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A287" s="6">
-        <v>207</v>
-      </c>
-      <c r="B287" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C287" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D287" s="6"/>
-    </row>
-    <row r="288" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A288" s="6">
-        <v>210</v>
-      </c>
-      <c r="B288" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D288" s="6"/>
-    </row>
-    <row r="289" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A289" s="6">
-        <v>269</v>
-      </c>
-      <c r="B289" s="2" t="s">
-        <v>259</v>
-      </c>
+        <v>1021</v>
+      </c>
+      <c r="B287" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B288" s="8"/>
+    </row>
+    <row r="289" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B289" s="8"/>
     </row>
     <row r="292" spans="1:4" ht="25" x14ac:dyDescent="0.25">
       <c r="A292" s="5" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="293" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -4344,10 +4408,10 @@
     </row>
     <row r="294" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A294" s="6">
-        <v>384</v>
-      </c>
-      <c r="B294" s="2" t="s">
-        <v>261</v>
+        <v>389</v>
+      </c>
+      <c r="B294" s="3" t="s">
+        <v>251</v>
       </c>
       <c r="C294" s="2" t="s">
         <v>2</v>
@@ -4356,10 +4420,10 @@
     </row>
     <row r="295" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A295" s="6">
-        <v>398</v>
-      </c>
-      <c r="B295" s="2" t="s">
-        <v>262</v>
+        <v>136</v>
+      </c>
+      <c r="B295" s="3" t="s">
+        <v>252</v>
       </c>
       <c r="C295" s="2" t="s">
         <v>2</v>
@@ -4368,117 +4432,78 @@
     </row>
     <row r="296" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A296" s="6">
-        <v>382</v>
-      </c>
-      <c r="B296" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="C296" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D296" s="6"/>
-    </row>
-    <row r="297" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A297" s="6">
-        <v>380</v>
-      </c>
-      <c r="B297" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="C297" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D297" s="6"/>
-    </row>
-    <row r="298" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A298" s="6">
-        <v>381</v>
-      </c>
-      <c r="B298" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C298" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D298" s="6"/>
-    </row>
-    <row r="299" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A299" s="6">
-        <v>138</v>
-      </c>
-      <c r="B299" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="302" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A302" s="5" t="s">
-        <v>267</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="B296" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="299" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A299" s="5" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="300" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A300" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B300" s="6"/>
+      <c r="C300" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="301" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A301" s="6">
+        <v>207</v>
+      </c>
+      <c r="B301" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C301" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D301" s="6"/>
+    </row>
+    <row r="302" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A302" s="6">
+        <v>210</v>
+      </c>
+      <c r="B302" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="C302" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D302" s="6"/>
     </row>
     <row r="303" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A303" s="6" t="s">
+      <c r="A303" s="6">
+        <v>269</v>
+      </c>
+      <c r="B303" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="306" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A306" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="307" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A307" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B303" s="6"/>
-      <c r="C303" s="6"/>
-      <c r="D303" s="6"/>
-    </row>
-    <row r="304" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A304" s="6">
-        <v>359</v>
-      </c>
-      <c r="B304" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="C304" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D304" s="6"/>
-    </row>
-    <row r="305" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A305" s="6">
-        <v>346</v>
-      </c>
-      <c r="B305" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="C305" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D305" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="306" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A306" s="6">
-        <v>362</v>
-      </c>
-      <c r="B306" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="C306" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D306" s="6"/>
-    </row>
-    <row r="307" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A307" s="6">
-        <v>281</v>
-      </c>
-      <c r="B307" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="C307" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D307" s="6"/>
+      <c r="B307" s="6"/>
+      <c r="C307" s="6" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="308" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A308" s="6">
-        <v>284</v>
-      </c>
-      <c r="B308" s="3" t="s">
-        <v>272</v>
+        <v>384</v>
+      </c>
+      <c r="B308" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="C308" s="2" t="s">
         <v>2</v>
@@ -4487,10 +4512,10 @@
     </row>
     <row r="309" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A309" s="6">
-        <v>251</v>
-      </c>
-      <c r="B309" s="3" t="s">
-        <v>273</v>
+        <v>398</v>
+      </c>
+      <c r="B309" s="2" t="s">
+        <v>260</v>
       </c>
       <c r="C309" s="2" t="s">
         <v>2</v>
@@ -4499,10 +4524,10 @@
     </row>
     <row r="310" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A310" s="6">
-        <v>288</v>
-      </c>
-      <c r="B310" s="3" t="s">
-        <v>274</v>
+        <v>382</v>
+      </c>
+      <c r="B310" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C310" s="2" t="s">
         <v>2</v>
@@ -4511,10 +4536,10 @@
     </row>
     <row r="311" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A311" s="6">
-        <v>170</v>
+        <v>380</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -4523,10 +4548,10 @@
     </row>
     <row r="312" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A312" s="6">
-        <v>348</v>
+        <v>381</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C312" s="2" t="s">
         <v>2</v>
@@ -4535,70 +4560,31 @@
     </row>
     <row r="313" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A313" s="6">
-        <v>379</v>
+        <v>138</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C313" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D313" s="6"/>
-    </row>
-    <row r="314" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A314" s="6">
-        <v>353</v>
-      </c>
-      <c r="B314" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="C314" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D314" s="6"/>
-    </row>
-    <row r="315" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A315" s="6">
-        <v>146</v>
-      </c>
-      <c r="B315" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C315" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D315" s="6"/>
-    </row>
-    <row r="316" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A316" s="6">
-        <v>355</v>
-      </c>
-      <c r="B316" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="C316" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D316" s="6"/>
+        <v>264</v>
+      </c>
+    </row>
+    <row r="316" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A316" s="5" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="317" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A317" s="6">
-        <v>303</v>
-      </c>
-      <c r="B317" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="C317" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="A317" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B317" s="6"/>
+      <c r="C317" s="6"/>
       <c r="D317" s="6"/>
     </row>
     <row r="318" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A318" s="6">
-        <v>304</v>
-      </c>
-      <c r="B318" s="2" t="s">
-        <v>282</v>
+        <v>359</v>
+      </c>
+      <c r="B318" s="3" t="s">
+        <v>266</v>
       </c>
       <c r="C318" s="2" t="s">
         <v>2</v>
@@ -4607,51 +4593,374 @@
     </row>
     <row r="319" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A319" s="6">
-        <v>307</v>
-      </c>
-      <c r="B319" s="2" t="s">
-        <v>283</v>
+        <v>346</v>
+      </c>
+      <c r="B319" s="3" t="s">
+        <v>267</v>
       </c>
       <c r="C319" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D319" s="6" t="s">
-        <v>284</v>
+        <v>179</v>
       </c>
     </row>
     <row r="320" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A320" s="6">
+        <v>362</v>
+      </c>
+      <c r="B320" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C320" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D320" s="6"/>
+    </row>
+    <row r="321" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A321" s="6">
+        <v>281</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D321" s="6"/>
+    </row>
+    <row r="322" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A322" s="6">
+        <v>284</v>
+      </c>
+      <c r="B322" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="C322" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D322" s="6"/>
+    </row>
+    <row r="323" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A323" s="6">
+        <v>251</v>
+      </c>
+      <c r="B323" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C323" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D323" s="6"/>
+    </row>
+    <row r="324" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A324" s="6">
+        <v>288</v>
+      </c>
+      <c r="B324" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="C324" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D324" s="6"/>
+    </row>
+    <row r="325" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A325" s="6">
+        <v>170</v>
+      </c>
+      <c r="B325" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="C325" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D325" s="6"/>
+    </row>
+    <row r="326" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A326" s="6">
+        <v>348</v>
+      </c>
+      <c r="B326" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C326" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D326" s="6"/>
+    </row>
+    <row r="327" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A327" s="6">
+        <v>379</v>
+      </c>
+      <c r="B327" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C327" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D327" s="6"/>
+    </row>
+    <row r="328" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A328" s="6">
+        <v>353</v>
+      </c>
+      <c r="B328" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C328" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D328" s="6"/>
+    </row>
+    <row r="329" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A329" s="6">
+        <v>146</v>
+      </c>
+      <c r="B329" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C329" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D329" s="6"/>
+    </row>
+    <row r="330" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A330" s="6">
+        <v>355</v>
+      </c>
+      <c r="B330" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C330" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D330" s="6"/>
+    </row>
+    <row r="331" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A331" s="6">
+        <v>303</v>
+      </c>
+      <c r="B331" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="C331" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D331" s="6"/>
+    </row>
+    <row r="332" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A332" s="6">
+        <v>304</v>
+      </c>
+      <c r="B332" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C332" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D332" s="6"/>
+    </row>
+    <row r="333" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A333" s="6">
+        <v>307</v>
+      </c>
+      <c r="B333" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="C333" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D333" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="334" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A334" s="6">
         <v>308</v>
       </c>
-      <c r="B320" s="2" t="s">
+      <c r="B334" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C334" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D334" s="6" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="335" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A335" s="6">
+        <v>705</v>
+      </c>
+      <c r="B335" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="337" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A337" s="6">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="338" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A338">
+        <v>697</v>
+      </c>
+      <c r="B338" t="s">
         <v>285</v>
       </c>
-      <c r="C320" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D320" s="6" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="321" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A321" s="6">
-        <v>705</v>
-      </c>
-      <c r="B321" s="2" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="323" spans="1:2" ht="17" x14ac:dyDescent="0.2">
-      <c r="A323" s="6">
-        <v>3.31</v>
-      </c>
-    </row>
-    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A324">
-        <v>697</v>
-      </c>
-      <c r="B324" t="s">
-        <v>287</v>
+    </row>
+    <row r="341" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A341" s="9" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="342" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A342" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B342" s="1"/>
+      <c r="C342" s="1"/>
+    </row>
+    <row r="343" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A343" s="1">
+        <v>35</v>
+      </c>
+      <c r="B343" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="C343" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D343" s="1"/>
+    </row>
+    <row r="344" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A344" s="1">
+        <v>33</v>
+      </c>
+      <c r="B344" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C344" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D344" s="1"/>
+    </row>
+    <row r="345" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A345" s="1">
+        <v>81</v>
+      </c>
+      <c r="B345" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="C345" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D345" s="1"/>
+    </row>
+    <row r="346" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A346" s="1">
+        <v>153</v>
+      </c>
+      <c r="B346" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C346" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D346" s="1"/>
+    </row>
+    <row r="347" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A347" s="1">
+        <v>154</v>
+      </c>
+      <c r="B347" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="C347" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D347" s="1"/>
+    </row>
+    <row r="348" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A348" s="1">
+        <v>162</v>
+      </c>
+      <c r="B348" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C348" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D348" s="1"/>
+    </row>
+    <row r="349" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A349" s="1">
+        <v>374</v>
+      </c>
+      <c r="B349" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C349" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D349" s="1"/>
+    </row>
+    <row r="350" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A350" s="1">
+        <v>34</v>
+      </c>
+      <c r="B350" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C350" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D350" s="1"/>
+    </row>
+    <row r="351" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A351" s="1">
+        <v>315</v>
+      </c>
+      <c r="B351" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D351" s="1"/>
+    </row>
+    <row r="352" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
+        <v>300</v>
+      </c>
+      <c r="B352" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C352" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D352" s="1"/>
+    </row>
+    <row r="353" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A353" s="1">
+        <v>354</v>
+      </c>
+      <c r="B353" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" ht="26" x14ac:dyDescent="0.3">
+      <c r="A356" s="9" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A357">
+        <v>500</v>
+      </c>
+      <c r="B357" t="s">
+        <v>303</v>
       </c>
     </row>
   </sheetData>
@@ -4703,84 +5012,84 @@
     <hyperlink ref="C155" r:id="rId45" display="https://cspiration.com/login" xr:uid="{8B14C05B-DD8F-D443-8EAA-F17CA50D7366}"/>
     <hyperlink ref="B156" r:id="rId46" display="https://leetcode.com/problems/max-sum-of-rectangle-no-larger-than-k/description/" xr:uid="{4AA58D7A-2220-7E48-94A8-240A6AFC7EB7}"/>
     <hyperlink ref="C156" r:id="rId47" display="https://cspiration.com/login" xr:uid="{38081C3C-1B84-3A42-8B82-08867C75BE08}"/>
-    <hyperlink ref="B158" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
-    <hyperlink ref="C158" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
-    <hyperlink ref="B159" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
-    <hyperlink ref="C159" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
-    <hyperlink ref="B160" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
-    <hyperlink ref="C160" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
-    <hyperlink ref="B161" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
-    <hyperlink ref="C161" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
-    <hyperlink ref="B162" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
-    <hyperlink ref="C162" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
-    <hyperlink ref="B163" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
-    <hyperlink ref="B169" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
-    <hyperlink ref="C169" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
-    <hyperlink ref="B170" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
-    <hyperlink ref="C170" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
-    <hyperlink ref="B171" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
-    <hyperlink ref="C171" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
-    <hyperlink ref="B172" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
-    <hyperlink ref="C172" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
-    <hyperlink ref="B173" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
-    <hyperlink ref="C173" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
-    <hyperlink ref="B174" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
-    <hyperlink ref="C174" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
-    <hyperlink ref="B175" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
-    <hyperlink ref="C175" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
-    <hyperlink ref="B176" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
-    <hyperlink ref="C176" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
-    <hyperlink ref="B177" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
-    <hyperlink ref="C177" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
-    <hyperlink ref="B178" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
-    <hyperlink ref="C178" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
-    <hyperlink ref="B179" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
-    <hyperlink ref="C179" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
-    <hyperlink ref="B180" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
-    <hyperlink ref="C180" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
-    <hyperlink ref="B181" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
-    <hyperlink ref="C181" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
-    <hyperlink ref="B182" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
-    <hyperlink ref="C182" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
-    <hyperlink ref="B184" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
-    <hyperlink ref="C184" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
-    <hyperlink ref="B185" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
-    <hyperlink ref="C185" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
-    <hyperlink ref="B186" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
-    <hyperlink ref="C186" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
-    <hyperlink ref="B187" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
-    <hyperlink ref="C187" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
-    <hyperlink ref="B188" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
-    <hyperlink ref="C188" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
-    <hyperlink ref="B189" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
-    <hyperlink ref="C189" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
-    <hyperlink ref="B190" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
-    <hyperlink ref="C190" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
-    <hyperlink ref="B191" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
-    <hyperlink ref="C191" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
-    <hyperlink ref="B192" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
-    <hyperlink ref="B197" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
-    <hyperlink ref="C197" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
-    <hyperlink ref="B198" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
-    <hyperlink ref="C198" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
-    <hyperlink ref="B199" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
-    <hyperlink ref="C199" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
-    <hyperlink ref="B200" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
-    <hyperlink ref="C200" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
-    <hyperlink ref="B201" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
-    <hyperlink ref="C201" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
-    <hyperlink ref="B202" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
-    <hyperlink ref="C202" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
-    <hyperlink ref="B204" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
-    <hyperlink ref="C204" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
-    <hyperlink ref="B205" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
-    <hyperlink ref="C205" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
-    <hyperlink ref="B203" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
-    <hyperlink ref="B211" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
-    <hyperlink ref="C211" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
-    <hyperlink ref="B212" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
-    <hyperlink ref="C212" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
-    <hyperlink ref="B213" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
+    <hyperlink ref="B159" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
+    <hyperlink ref="C159" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
+    <hyperlink ref="B160" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
+    <hyperlink ref="C160" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
+    <hyperlink ref="B161" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
+    <hyperlink ref="C161" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
+    <hyperlink ref="B162" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
+    <hyperlink ref="C162" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
+    <hyperlink ref="B163" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
+    <hyperlink ref="C163" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
+    <hyperlink ref="B164" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
+    <hyperlink ref="B180" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
+    <hyperlink ref="C180" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
+    <hyperlink ref="B181" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
+    <hyperlink ref="C181" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
+    <hyperlink ref="B182" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
+    <hyperlink ref="C182" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
+    <hyperlink ref="B183" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
+    <hyperlink ref="C183" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
+    <hyperlink ref="B184" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
+    <hyperlink ref="C184" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
+    <hyperlink ref="B185" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
+    <hyperlink ref="C185" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
+    <hyperlink ref="B186" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
+    <hyperlink ref="C186" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
+    <hyperlink ref="B187" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
+    <hyperlink ref="C187" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
+    <hyperlink ref="B188" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
+    <hyperlink ref="C188" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
+    <hyperlink ref="B189" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
+    <hyperlink ref="C189" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
+    <hyperlink ref="B190" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
+    <hyperlink ref="C190" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
+    <hyperlink ref="B191" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
+    <hyperlink ref="C191" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
+    <hyperlink ref="B192" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
+    <hyperlink ref="C192" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
+    <hyperlink ref="B193" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
+    <hyperlink ref="C193" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
+    <hyperlink ref="B195" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
+    <hyperlink ref="C195" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
+    <hyperlink ref="B196" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
+    <hyperlink ref="C196" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
+    <hyperlink ref="B197" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
+    <hyperlink ref="C197" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
+    <hyperlink ref="B198" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
+    <hyperlink ref="C198" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
+    <hyperlink ref="B199" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
+    <hyperlink ref="C199" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
+    <hyperlink ref="B200" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
+    <hyperlink ref="C200" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
+    <hyperlink ref="B201" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
+    <hyperlink ref="C201" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
+    <hyperlink ref="B202" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
+    <hyperlink ref="C202" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
+    <hyperlink ref="B203" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
+    <hyperlink ref="B208" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
+    <hyperlink ref="C208" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
+    <hyperlink ref="B209" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
+    <hyperlink ref="C209" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
+    <hyperlink ref="B210" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
+    <hyperlink ref="C210" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
+    <hyperlink ref="B211" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
+    <hyperlink ref="C211" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
+    <hyperlink ref="B212" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
+    <hyperlink ref="C212" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
+    <hyperlink ref="B213" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
+    <hyperlink ref="C213" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
+    <hyperlink ref="B215" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
+    <hyperlink ref="C215" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
+    <hyperlink ref="B216" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
+    <hyperlink ref="C216" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
+    <hyperlink ref="B214" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
+    <hyperlink ref="B222" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
+    <hyperlink ref="C222" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
+    <hyperlink ref="B223" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
+    <hyperlink ref="C223" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
+    <hyperlink ref="B224" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
     <hyperlink ref="B80" r:id="rId126" display="https://leetcode.com/problems/minimum-depth-of-binary-tree/description/" xr:uid="{89D22C44-568D-2A43-84A7-D669E16D4993}"/>
     <hyperlink ref="C80" r:id="rId127" display="https://cspiration.com/login" xr:uid="{CDC90D9B-21B1-9F4E-BBAE-19128D12CFDA}"/>
     <hyperlink ref="B82" r:id="rId128" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/description/" xr:uid="{93D570CB-F2FC-D841-9EFB-185B9F3C2E70}"/>
@@ -4991,144 +5300,167 @@
     <hyperlink ref="C61" r:id="rId333" display="https://cspiration.com/login" xr:uid="{C5087984-A06B-4248-8E74-E2539F4CAF6A}"/>
     <hyperlink ref="B62" r:id="rId334" display="https://leetcode.com/problems/repeated-dna-sequences/description/" xr:uid="{52566213-99F8-BA41-B322-FDF32A868B37}"/>
     <hyperlink ref="C62" r:id="rId335" display="https://cspiration.com/login" xr:uid="{149752EA-7A00-384E-BE6B-4D94705BC736}"/>
-    <hyperlink ref="B219" r:id="rId336" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
-    <hyperlink ref="C219" r:id="rId337" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
-    <hyperlink ref="B220" r:id="rId338" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
-    <hyperlink ref="C220" r:id="rId339" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
-    <hyperlink ref="B221" r:id="rId340" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
-    <hyperlink ref="C221" r:id="rId341" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
-    <hyperlink ref="B223" r:id="rId342" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
-    <hyperlink ref="C223" r:id="rId343" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
-    <hyperlink ref="B229" r:id="rId344" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
-    <hyperlink ref="C229" r:id="rId345" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
-    <hyperlink ref="B228" r:id="rId346" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
-    <hyperlink ref="C228" r:id="rId347" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
-    <hyperlink ref="B230" r:id="rId348" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
-    <hyperlink ref="C230" r:id="rId349" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
-    <hyperlink ref="B235" r:id="rId350" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
-    <hyperlink ref="C235" r:id="rId351" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
-    <hyperlink ref="B236" r:id="rId352" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
-    <hyperlink ref="C236" r:id="rId353" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
-    <hyperlink ref="B237" r:id="rId354" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
-    <hyperlink ref="C237" r:id="rId355" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
-    <hyperlink ref="B238" r:id="rId356" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
-    <hyperlink ref="C238" r:id="rId357" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
-    <hyperlink ref="B239" r:id="rId358" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
-    <hyperlink ref="C239" r:id="rId359" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
-    <hyperlink ref="B240" r:id="rId360" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
-    <hyperlink ref="C240" r:id="rId361" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
-    <hyperlink ref="B241" r:id="rId362" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
-    <hyperlink ref="C241" r:id="rId363" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
-    <hyperlink ref="B242" r:id="rId364" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
-    <hyperlink ref="C242" r:id="rId365" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
-    <hyperlink ref="B243" r:id="rId366" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
-    <hyperlink ref="C243" r:id="rId367" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
-    <hyperlink ref="B244" r:id="rId368" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
-    <hyperlink ref="C244" r:id="rId369" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
-    <hyperlink ref="B245" r:id="rId370" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
-    <hyperlink ref="C245" r:id="rId371" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
-    <hyperlink ref="B246" r:id="rId372" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
-    <hyperlink ref="C246" r:id="rId373" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
-    <hyperlink ref="B247" r:id="rId374" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
-    <hyperlink ref="C247" r:id="rId375" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
-    <hyperlink ref="B248" r:id="rId376" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
-    <hyperlink ref="C248" r:id="rId377" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
-    <hyperlink ref="B249" r:id="rId378" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
-    <hyperlink ref="C249" r:id="rId379" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
-    <hyperlink ref="B250" r:id="rId380" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
-    <hyperlink ref="C250" r:id="rId381" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
-    <hyperlink ref="B251" r:id="rId382" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
-    <hyperlink ref="B258" r:id="rId383" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
-    <hyperlink ref="C258" r:id="rId384" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
-    <hyperlink ref="B259" r:id="rId385" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{156CAAE5-6351-9947-BB71-247BCB4199E4}"/>
-    <hyperlink ref="C259" r:id="rId386" display="https://cspiration.com/login" xr:uid="{B32FCD33-3793-1145-9B85-1C19988C5512}"/>
-    <hyperlink ref="B260" r:id="rId387" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{988FA989-097D-3643-AFD0-51D5DE85FC28}"/>
-    <hyperlink ref="C260" r:id="rId388" display="https://cspiration.com/login" xr:uid="{236098E8-3353-2343-96D1-B31CFD341154}"/>
-    <hyperlink ref="B261" r:id="rId389" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
-    <hyperlink ref="C261" r:id="rId390" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
-    <hyperlink ref="B262" r:id="rId391" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
-    <hyperlink ref="C262" r:id="rId392" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
-    <hyperlink ref="B263" r:id="rId393" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
-    <hyperlink ref="C263" r:id="rId394" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
-    <hyperlink ref="B264" r:id="rId395" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
-    <hyperlink ref="C264" r:id="rId396" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
-    <hyperlink ref="B265" r:id="rId397" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
-    <hyperlink ref="C265" r:id="rId398" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
-    <hyperlink ref="B266" r:id="rId399" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
-    <hyperlink ref="C266" r:id="rId400" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
-    <hyperlink ref="B267" r:id="rId401" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
-    <hyperlink ref="C267" r:id="rId402" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
-    <hyperlink ref="B268" r:id="rId403" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
-    <hyperlink ref="C268" r:id="rId404" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
-    <hyperlink ref="B270" r:id="rId405" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
-    <hyperlink ref="C270" r:id="rId406" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
-    <hyperlink ref="B271" r:id="rId407" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
-    <hyperlink ref="C271" r:id="rId408" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
-    <hyperlink ref="B272" r:id="rId409" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
-    <hyperlink ref="C272" r:id="rId410" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
-    <hyperlink ref="B273" r:id="rId411" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
-    <hyperlink ref="C273" r:id="rId412" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
-    <hyperlink ref="B274" r:id="rId413" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
-    <hyperlink ref="B280" r:id="rId414" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
-    <hyperlink ref="C280" r:id="rId415" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
-    <hyperlink ref="B281" r:id="rId416" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
-    <hyperlink ref="C281" r:id="rId417" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
-    <hyperlink ref="B282" r:id="rId418" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
-    <hyperlink ref="B287" r:id="rId419" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
-    <hyperlink ref="C287" r:id="rId420" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
-    <hyperlink ref="B288" r:id="rId421" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
-    <hyperlink ref="C288" r:id="rId422" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
-    <hyperlink ref="B289" r:id="rId423" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
-    <hyperlink ref="B294" r:id="rId424" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
-    <hyperlink ref="C294" r:id="rId425" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
-    <hyperlink ref="B295" r:id="rId426" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
-    <hyperlink ref="C295" r:id="rId427" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
-    <hyperlink ref="B296" r:id="rId428" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
-    <hyperlink ref="C296" r:id="rId429" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
-    <hyperlink ref="B297" r:id="rId430" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
-    <hyperlink ref="C297" r:id="rId431" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
-    <hyperlink ref="B298" r:id="rId432" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
-    <hyperlink ref="C298" r:id="rId433" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
-    <hyperlink ref="B299" r:id="rId434" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
-    <hyperlink ref="B304" r:id="rId435" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
-    <hyperlink ref="C304" r:id="rId436" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
-    <hyperlink ref="B305" r:id="rId437" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
-    <hyperlink ref="C305" r:id="rId438" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
-    <hyperlink ref="B306" r:id="rId439" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
-    <hyperlink ref="C306" r:id="rId440" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
-    <hyperlink ref="B307" r:id="rId441" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
-    <hyperlink ref="C307" r:id="rId442" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
-    <hyperlink ref="B308" r:id="rId443" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
-    <hyperlink ref="C308" r:id="rId444" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
-    <hyperlink ref="B309" r:id="rId445" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
-    <hyperlink ref="C309" r:id="rId446" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
-    <hyperlink ref="B310" r:id="rId447" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
-    <hyperlink ref="C310" r:id="rId448" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
-    <hyperlink ref="B311" r:id="rId449" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
-    <hyperlink ref="C311" r:id="rId450" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
-    <hyperlink ref="B312" r:id="rId451" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
-    <hyperlink ref="C312" r:id="rId452" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
-    <hyperlink ref="B313" r:id="rId453" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
-    <hyperlink ref="C313" r:id="rId454" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
-    <hyperlink ref="B314" r:id="rId455" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
-    <hyperlink ref="C314" r:id="rId456" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
-    <hyperlink ref="B315" r:id="rId457" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
-    <hyperlink ref="C315" r:id="rId458" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
-    <hyperlink ref="B316" r:id="rId459" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
-    <hyperlink ref="C316" r:id="rId460" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
-    <hyperlink ref="B317" r:id="rId461" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
-    <hyperlink ref="C317" r:id="rId462" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
-    <hyperlink ref="B318" r:id="rId463" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
-    <hyperlink ref="C318" r:id="rId464" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
-    <hyperlink ref="B319" r:id="rId465" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
-    <hyperlink ref="C319" r:id="rId466" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
-    <hyperlink ref="B320" r:id="rId467" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
-    <hyperlink ref="C320" r:id="rId468" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
-    <hyperlink ref="B321" r:id="rId469" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
-    <hyperlink ref="B133" r:id="rId470" xr:uid="{6E505C5D-7486-774A-8436-0B2D9A806CE7}"/>
-    <hyperlink ref="B154" r:id="rId471" xr:uid="{8066B6F4-349C-104A-B6B1-4C5FDFBC5FE9}"/>
-    <hyperlink ref="B164" r:id="rId472" xr:uid="{13747061-B8D2-6041-B323-BA395125DCAA}"/>
-    <hyperlink ref="B206" r:id="rId473" xr:uid="{2D2F7CE9-7323-F34F-AA6B-4FECD6A6C804}"/>
+    <hyperlink ref="B230" r:id="rId336" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
+    <hyperlink ref="C230" r:id="rId337" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
+    <hyperlink ref="B231" r:id="rId338" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
+    <hyperlink ref="C231" r:id="rId339" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
+    <hyperlink ref="B232" r:id="rId340" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
+    <hyperlink ref="C232" r:id="rId341" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
+    <hyperlink ref="B234" r:id="rId342" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
+    <hyperlink ref="C234" r:id="rId343" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
+    <hyperlink ref="B240" r:id="rId344" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
+    <hyperlink ref="C240" r:id="rId345" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
+    <hyperlink ref="B239" r:id="rId346" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
+    <hyperlink ref="C239" r:id="rId347" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
+    <hyperlink ref="B241" r:id="rId348" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
+    <hyperlink ref="C241" r:id="rId349" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
+    <hyperlink ref="B246" r:id="rId350" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
+    <hyperlink ref="C246" r:id="rId351" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
+    <hyperlink ref="B247" r:id="rId352" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
+    <hyperlink ref="C247" r:id="rId353" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
+    <hyperlink ref="B248" r:id="rId354" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
+    <hyperlink ref="C248" r:id="rId355" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
+    <hyperlink ref="B249" r:id="rId356" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
+    <hyperlink ref="C249" r:id="rId357" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
+    <hyperlink ref="B250" r:id="rId358" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
+    <hyperlink ref="C250" r:id="rId359" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
+    <hyperlink ref="B251" r:id="rId360" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
+    <hyperlink ref="C251" r:id="rId361" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
+    <hyperlink ref="B252" r:id="rId362" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
+    <hyperlink ref="C252" r:id="rId363" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
+    <hyperlink ref="B253" r:id="rId364" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
+    <hyperlink ref="C253" r:id="rId365" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
+    <hyperlink ref="B254" r:id="rId366" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
+    <hyperlink ref="C254" r:id="rId367" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
+    <hyperlink ref="B255" r:id="rId368" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
+    <hyperlink ref="C255" r:id="rId369" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
+    <hyperlink ref="B256" r:id="rId370" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
+    <hyperlink ref="C256" r:id="rId371" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
+    <hyperlink ref="B257" r:id="rId372" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
+    <hyperlink ref="C257" r:id="rId373" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
+    <hyperlink ref="B258" r:id="rId374" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
+    <hyperlink ref="C258" r:id="rId375" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
+    <hyperlink ref="B259" r:id="rId376" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
+    <hyperlink ref="C259" r:id="rId377" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
+    <hyperlink ref="B260" r:id="rId378" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
+    <hyperlink ref="C260" r:id="rId379" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
+    <hyperlink ref="B261" r:id="rId380" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
+    <hyperlink ref="C261" r:id="rId381" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
+    <hyperlink ref="B262" r:id="rId382" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
+    <hyperlink ref="B269" r:id="rId383" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
+    <hyperlink ref="C269" r:id="rId384" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
+    <hyperlink ref="B272" r:id="rId385" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
+    <hyperlink ref="C272" r:id="rId386" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
+    <hyperlink ref="B273" r:id="rId387" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
+    <hyperlink ref="C273" r:id="rId388" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
+    <hyperlink ref="B274" r:id="rId389" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
+    <hyperlink ref="C274" r:id="rId390" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
+    <hyperlink ref="B275" r:id="rId391" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
+    <hyperlink ref="C275" r:id="rId392" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
+    <hyperlink ref="B276" r:id="rId393" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
+    <hyperlink ref="C276" r:id="rId394" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
+    <hyperlink ref="B277" r:id="rId395" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
+    <hyperlink ref="C277" r:id="rId396" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
+    <hyperlink ref="B278" r:id="rId397" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
+    <hyperlink ref="C278" r:id="rId398" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
+    <hyperlink ref="B279" r:id="rId399" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
+    <hyperlink ref="C279" r:id="rId400" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
+    <hyperlink ref="B281" r:id="rId401" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
+    <hyperlink ref="C281" r:id="rId402" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
+    <hyperlink ref="B282" r:id="rId403" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
+    <hyperlink ref="C282" r:id="rId404" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
+    <hyperlink ref="B283" r:id="rId405" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
+    <hyperlink ref="C283" r:id="rId406" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
+    <hyperlink ref="B284" r:id="rId407" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
+    <hyperlink ref="C284" r:id="rId408" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
+    <hyperlink ref="B285" r:id="rId409" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
+    <hyperlink ref="B294" r:id="rId410" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
+    <hyperlink ref="C294" r:id="rId411" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
+    <hyperlink ref="B295" r:id="rId412" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
+    <hyperlink ref="C295" r:id="rId413" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
+    <hyperlink ref="B296" r:id="rId414" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
+    <hyperlink ref="B301" r:id="rId415" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
+    <hyperlink ref="C301" r:id="rId416" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
+    <hyperlink ref="B302" r:id="rId417" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
+    <hyperlink ref="C302" r:id="rId418" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
+    <hyperlink ref="B303" r:id="rId419" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
+    <hyperlink ref="B308" r:id="rId420" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
+    <hyperlink ref="C308" r:id="rId421" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
+    <hyperlink ref="B309" r:id="rId422" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
+    <hyperlink ref="C309" r:id="rId423" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
+    <hyperlink ref="B310" r:id="rId424" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
+    <hyperlink ref="C310" r:id="rId425" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
+    <hyperlink ref="B311" r:id="rId426" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
+    <hyperlink ref="C311" r:id="rId427" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
+    <hyperlink ref="B312" r:id="rId428" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
+    <hyperlink ref="C312" r:id="rId429" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
+    <hyperlink ref="B313" r:id="rId430" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
+    <hyperlink ref="B318" r:id="rId431" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
+    <hyperlink ref="C318" r:id="rId432" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
+    <hyperlink ref="B319" r:id="rId433" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
+    <hyperlink ref="C319" r:id="rId434" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
+    <hyperlink ref="B320" r:id="rId435" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
+    <hyperlink ref="C320" r:id="rId436" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
+    <hyperlink ref="B321" r:id="rId437" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
+    <hyperlink ref="C321" r:id="rId438" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
+    <hyperlink ref="B322" r:id="rId439" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
+    <hyperlink ref="C322" r:id="rId440" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
+    <hyperlink ref="B323" r:id="rId441" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
+    <hyperlink ref="C323" r:id="rId442" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
+    <hyperlink ref="B324" r:id="rId443" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
+    <hyperlink ref="C324" r:id="rId444" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
+    <hyperlink ref="B325" r:id="rId445" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
+    <hyperlink ref="C325" r:id="rId446" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
+    <hyperlink ref="B326" r:id="rId447" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
+    <hyperlink ref="C326" r:id="rId448" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
+    <hyperlink ref="B327" r:id="rId449" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
+    <hyperlink ref="C327" r:id="rId450" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
+    <hyperlink ref="B328" r:id="rId451" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
+    <hyperlink ref="C328" r:id="rId452" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
+    <hyperlink ref="B329" r:id="rId453" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
+    <hyperlink ref="C329" r:id="rId454" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
+    <hyperlink ref="B330" r:id="rId455" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
+    <hyperlink ref="C330" r:id="rId456" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
+    <hyperlink ref="B331" r:id="rId457" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
+    <hyperlink ref="C331" r:id="rId458" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
+    <hyperlink ref="B332" r:id="rId459" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
+    <hyperlink ref="C332" r:id="rId460" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
+    <hyperlink ref="B333" r:id="rId461" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
+    <hyperlink ref="C333" r:id="rId462" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
+    <hyperlink ref="B334" r:id="rId463" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
+    <hyperlink ref="C334" r:id="rId464" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
+    <hyperlink ref="B335" r:id="rId465" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
+    <hyperlink ref="B133" r:id="rId466" xr:uid="{6E505C5D-7486-774A-8436-0B2D9A806CE7}"/>
+    <hyperlink ref="B154" r:id="rId467" xr:uid="{8066B6F4-349C-104A-B6B1-4C5FDFBC5FE9}"/>
+    <hyperlink ref="B165" r:id="rId468" xr:uid="{13747061-B8D2-6041-B323-BA395125DCAA}"/>
+    <hyperlink ref="B217" r:id="rId469" xr:uid="{2D2F7CE9-7323-F34F-AA6B-4FECD6A6C804}"/>
+    <hyperlink ref="B343" r:id="rId470" display="https://leetcode.com/problems/search-insert-position/description/" xr:uid="{EB4E5B68-F05A-0C4B-9F53-41E4DBCA4F9E}"/>
+    <hyperlink ref="C343" r:id="rId471" display="https://cspiration.com/login" xr:uid="{CA1BBCD7-117A-A64E-8F77-852F33D02DB2}"/>
+    <hyperlink ref="B344" r:id="rId472" display="https://leetcode.com/problems/search-in-rotated-sorted-array/description/" xr:uid="{5B45788F-BB03-4843-BD6A-B976C9FCAEF1}"/>
+    <hyperlink ref="C344" r:id="rId473" display="https://cspiration.com/login" xr:uid="{551CAD20-3D2A-A64A-B23A-A01403C05DE0}"/>
+    <hyperlink ref="B345" r:id="rId474" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{89F11509-794F-0147-A002-99DBFE4011DC}"/>
+    <hyperlink ref="C345" r:id="rId475" display="https://cspiration.com/login" xr:uid="{A8D71102-8F66-8143-AADE-EC0B951315AF}"/>
+    <hyperlink ref="B346" r:id="rId476" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/description/" xr:uid="{A4765584-11DB-8C47-A9D8-28BCD3B3DB04}"/>
+    <hyperlink ref="C346" r:id="rId477" display="https://cspiration.com/login" xr:uid="{67A40D64-8C16-AB40-AF02-EC047B85587D}"/>
+    <hyperlink ref="B347" r:id="rId478" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/description/" xr:uid="{1C321054-4E86-0A4C-A5A9-D1503A97B9B0}"/>
+    <hyperlink ref="C347" r:id="rId479" display="https://cspiration.com/login" xr:uid="{4230A88F-C71C-F14B-89AA-04DA1B742A89}"/>
+    <hyperlink ref="B348" r:id="rId480" display="https://leetcode.com/problems/find-peak-element/description/" xr:uid="{736794C5-518A-194B-A096-354260C26D19}"/>
+    <hyperlink ref="C348" r:id="rId481" display="https://cspiration.com/login" xr:uid="{CC616423-7FF6-4546-BE49-14971E421AB1}"/>
+    <hyperlink ref="B349" r:id="rId482" display="https://leetcode.com/problems/guess-number-higher-or-lower/" xr:uid="{AA2881B4-D507-6C4E-B5AC-66556CE2E240}"/>
+    <hyperlink ref="C349" r:id="rId483" display="https://cspiration.com/login" xr:uid="{497BA16C-CBAB-CD4C-B123-9991F3A2E286}"/>
+    <hyperlink ref="B350" r:id="rId484" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/description/" xr:uid="{D78ED803-9C52-3C4E-8DAB-2FE615A62AB4}"/>
+    <hyperlink ref="C350" r:id="rId485" display="https://cspiration.com/login" xr:uid="{A8AD4217-A555-BA44-A724-8A04E7730E30}"/>
+    <hyperlink ref="B351" r:id="rId486" display="https://leetcode.com/problems/count-of-smaller-numbers-after-self/description/" xr:uid="{39F3DFF8-98F3-604E-9124-DD7F0D40F1B0}"/>
+    <hyperlink ref="C351" r:id="rId487" display="https://cspiration.com/login" xr:uid="{3561FB2C-CD0E-A746-8C4B-80613899C341}"/>
+    <hyperlink ref="B352" r:id="rId488" display="https://leetcode.com/problems/longest-increasing-subsequence/description/" xr:uid="{E9195674-DC99-4B46-B0EE-98194075832A}"/>
+    <hyperlink ref="C352" r:id="rId489" display="https://cspiration.com/login" xr:uid="{916F2DEE-639E-C943-A663-2517B8604445}"/>
+    <hyperlink ref="B353" r:id="rId490" display="https://leetcode.com/problems/russian-doll-envelopes/description/" xr:uid="{320B423A-BCFA-CE44-9951-2BD15ECD57E2}"/>
+    <hyperlink ref="B170" r:id="rId491" xr:uid="{600A5416-B5C9-BA47-892A-EE12A30AA3C9}"/>
+    <hyperlink ref="B174" r:id="rId492" xr:uid="{EADB0E54-5800-704D-A97B-CDE42026CFF8}"/>
+    <hyperlink ref="B287" r:id="rId493" xr:uid="{49EE6590-FC3C-C54F-A151-AA1FC6EF5061}"/>
+    <hyperlink ref="B270" r:id="rId494" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{E018DFB4-01AC-F645-8B90-8199997E6DD0}"/>
+    <hyperlink ref="C270" r:id="rId495" display="https://cspiration.com/login" xr:uid="{706E0A6D-CD70-2245-A6EA-B10034698AA6}"/>
+    <hyperlink ref="B271" r:id="rId496" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{0DF8CEC5-24F8-E745-8AEF-C177BA8C38D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
new start with the first 25
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABB2AE0-9867-E347-8BD0-25400CBC28AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924297E4-8276-8842-96DA-312CB9ED7C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
@@ -1594,8 +1594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
   <dimension ref="A1:H445"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A257" sqref="A257"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1634,7 +1634,7 @@
       <c r="A4" s="6">
         <v>27</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>318</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1646,7 +1646,7 @@
       <c r="A5" s="6">
         <v>26</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>319</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1658,7 +1658,7 @@
       <c r="A6" s="6">
         <v>80</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>320</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1670,7 +1670,7 @@
       <c r="A7" s="6">
         <v>277</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>321</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1682,7 +1682,7 @@
       <c r="A8" s="6">
         <v>189</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>322</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1694,7 +1694,7 @@
       <c r="A9" s="6">
         <v>41</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>323</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1706,7 +1706,7 @@
       <c r="A10" s="6">
         <v>299</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>324</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1718,7 +1718,7 @@
       <c r="A11" s="6">
         <v>134</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>325</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1730,7 +1730,7 @@
       <c r="A12" s="6">
         <v>118</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>326</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1744,7 +1744,7 @@
       <c r="A13" s="6">
         <v>119</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>328</v>
       </c>
       <c r="C13" s="2" t="s">

</xml_diff>

<commit_message>
pause for reviewing first 200, should start from dp next time
</commit_message>
<xml_diff>
--- a/track.xlsx
+++ b/track.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leslieren/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5E94B2-234C-D748-ABDA-77960634683A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AFD23F-73CF-514A-BE91-0FC6B85C7B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="15740" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
+    <workbookView xWindow="780" yWindow="660" windowWidth="27640" windowHeight="15740" activeTab="2" xr2:uid="{8E59BB28-1D73-BC40-82B7-CA1810B7C545}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="bycat" sheetId="1" r:id="rId1"/>
+    <sheet name="vmware" sheetId="2" r:id="rId2"/>
+    <sheet name="amazon" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="419">
   <si>
     <t>144</t>
   </si>
@@ -1185,6 +1187,111 @@
   </si>
   <si>
     <t>Unique Binary Search Trees II</t>
+  </si>
+  <si>
+    <t>Count Good Numbers</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/company/vmware/</t>
+  </si>
+  <si>
+    <t>146. LRU Cache</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lru-cache/</t>
+  </si>
+  <si>
+    <t>1347. Minimum Number of Steps to Make Two Strings Anagram</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-number-of-steps-to-make-two-strings-anagram/</t>
+  </si>
+  <si>
+    <t>careful!</t>
+  </si>
+  <si>
+    <t>460. LFU Cache</t>
+  </si>
+  <si>
+    <t>not yet</t>
+  </si>
+  <si>
+    <t>LFU Cache</t>
+  </si>
+  <si>
+    <t>1669. Merge In Between Linked Lists</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/merge-in-between-linked-lists/</t>
+  </si>
+  <si>
+    <t>All Nodes Distance K in Binary Tree</t>
+  </si>
+  <si>
+    <t>https://www.1point3acres.com/bbs/forum.php?mod=viewthread&amp;tid=776168&amp;ctid=232535</t>
+  </si>
+  <si>
+    <t>https://wdxtub.com/interview/14520850399861.html</t>
+  </si>
+  <si>
+    <t>127. Word Ladder</t>
+  </si>
+  <si>
+    <t>56. Merge Intervals</t>
+  </si>
+  <si>
+    <t>863. All Nodes Distance K in Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/all-nodes-distance-k-in-binary-tree/</t>
+  </si>
+  <si>
+    <t>328. Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>204. Count Primes</t>
+  </si>
+  <si>
+    <t>349. Intersection of Two Arrays</t>
+  </si>
+  <si>
+    <t>76. Minimum Window Substring</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Least Number of Unique Integers after K Removals</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/least-number-of-unique-integers-after-k-removals/</t>
+  </si>
+  <si>
+    <t>Least Number of Unique Integers after K Removals</t>
+  </si>
+  <si>
+    <t>testid</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/robot-bounded-in-circle/</t>
+  </si>
+  <si>
+    <t>Robot Bounded In Circle</t>
+  </si>
+  <si>
+    <t>Maximum Average Subtree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-average-subtree/</t>
+  </si>
+  <si>
+    <t>Maximum Area of a Piece of Cake After Horizontal and Vertical Cuts</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/maximum-area-of-a-piece-of-cake-after-horizontal-and-vertical-cuts/</t>
+  </si>
+  <si>
+    <t>K Closest Points to Origin</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/k-closest-points-to-origin/</t>
   </si>
 </sst>
 </file>
@@ -1592,10 +1699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0A4AFC-62FA-E94E-BE80-E68967C2241E}">
-  <dimension ref="A1:H445"/>
+  <dimension ref="A1:H446"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A217" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A230" sqref="A230"/>
+    <sheetView topLeftCell="A61" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2514,6 +2621,14 @@
         <v>298</v>
       </c>
     </row>
+    <row r="78" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>1481</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
     <row r="82" spans="1:8" ht="25" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>68</v>
@@ -3782,8 +3897,13 @@
         <v>48</v>
       </c>
     </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B190" s="8"/>
+    <row r="190" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A190" s="1">
+        <v>863</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B191" s="8"/>
@@ -4157,31 +4277,29 @@
       <c r="D225" s="6"/>
     </row>
     <row r="226" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A226" s="6" t="s">
+      <c r="A226" s="6">
+        <v>300</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C226" s="2"/>
+      <c r="D226" s="6"/>
+    </row>
+    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A227" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B226" s="7"/>
-      <c r="C226" s="6"/>
-      <c r="D226" s="6"/>
-    </row>
-    <row r="227" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A227" s="6">
-        <v>256</v>
-      </c>
-      <c r="B227" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C227" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B227" s="7"/>
+      <c r="C227" s="6"/>
       <c r="D227" s="6"/>
     </row>
     <row r="228" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A228" s="6">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>2</v>
@@ -4190,10 +4308,10 @@
     </row>
     <row r="229" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A229" s="6">
-        <v>64</v>
+        <v>265</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C229" s="2" t="s">
         <v>2</v>
@@ -4202,10 +4320,10 @@
     </row>
     <row r="230" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A230" s="6">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C230" s="2" t="s">
         <v>2</v>
@@ -4214,10 +4332,10 @@
     </row>
     <row r="231" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A231" s="6">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="B231" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C231" s="2" t="s">
         <v>2</v>
@@ -4226,10 +4344,10 @@
     </row>
     <row r="232" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A232" s="6">
-        <v>174</v>
+        <v>97</v>
       </c>
       <c r="B232" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C232" s="2" t="s">
         <v>2</v>
@@ -4238,10 +4356,10 @@
     </row>
     <row r="233" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A233" s="6">
-        <v>221</v>
+        <v>174</v>
       </c>
       <c r="B233" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C233" s="2" t="s">
         <v>2</v>
@@ -4250,69 +4368,69 @@
     </row>
     <row r="234" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A234" s="6">
-        <v>84</v>
+        <v>221</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="C234" s="2"/>
+        <v>92</v>
+      </c>
+      <c r="C234" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="D234" s="6"/>
     </row>
     <row r="235" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A235" s="6">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C235" s="2" t="s">
-        <v>2</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="C235" s="2"/>
       <c r="D235" s="6"/>
     </row>
     <row r="236" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A236" s="6">
+        <v>85</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C236" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D236" s="6"/>
+    </row>
+    <row r="237" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A237" s="6">
         <v>363</v>
       </c>
-      <c r="B236" s="3" t="s">
+      <c r="B237" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C236" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D236" s="6" t="s">
+      <c r="C237" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D237" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="237" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="D237" s="6"/>
-    </row>
     <row r="238" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A238" s="6" t="s">
+      <c r="D238" s="6"/>
+    </row>
+    <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A239" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B238" s="7"/>
-      <c r="C238" s="6"/>
-      <c r="D238" s="6"/>
-    </row>
-    <row r="239" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A239" s="6">
-        <v>198</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="C239" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B239" s="7"/>
+      <c r="C239" s="6"/>
       <c r="D239" s="6"/>
     </row>
     <row r="240" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A240" s="6">
-        <v>213</v>
+        <v>198</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C240" s="2" t="s">
         <v>2</v>
@@ -4321,10 +4439,10 @@
     </row>
     <row r="241" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A241" s="6">
-        <v>276</v>
+        <v>213</v>
       </c>
       <c r="B241" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C241" s="2" t="s">
         <v>2</v>
@@ -4333,10 +4451,10 @@
     </row>
     <row r="242" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A242" s="6">
-        <v>91</v>
+        <v>276</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C242" s="2" t="s">
         <v>2</v>
@@ -4345,10 +4463,10 @@
     </row>
     <row r="243" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A243" s="6">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="B243" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C243" s="2" t="s">
         <v>2</v>
@@ -4357,43 +4475,48 @@
     </row>
     <row r="244" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A244" s="6">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="B244" s="3" t="s">
-        <v>102</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="C244" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D244" s="6"/>
     </row>
     <row r="245" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A245" s="6">
+        <v>44</v>
+      </c>
+      <c r="B245" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A246" s="6">
         <v>1048</v>
       </c>
-      <c r="B245" s="2" t="s">
+      <c r="B246" s="2" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="246" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A246" s="6" t="s">
+    <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A247" s="6" t="s">
         <v>302</v>
       </c>
-      <c r="B246" s="2"/>
-    </row>
-    <row r="247" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A247" s="6">
-        <v>746</v>
-      </c>
-      <c r="B247" s="3"/>
-      <c r="C247" s="2"/>
+      <c r="B247" s="2"/>
     </row>
     <row r="248" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A248" s="6">
-        <v>1025</v>
+        <v>746</v>
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="2"/>
     </row>
     <row r="249" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A249" s="6">
-        <v>1139</v>
+        <v>1025</v>
       </c>
       <c r="B249" s="3"/>
       <c r="C249" s="2"/>
@@ -4402,92 +4525,87 @@
       <c r="A250" s="6">
         <v>1139</v>
       </c>
-      <c r="B250" s="3" t="s">
-        <v>301</v>
-      </c>
+      <c r="B250" s="3"/>
       <c r="C250" s="2"/>
     </row>
     <row r="251" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A251" s="6">
-        <v>740</v>
+        <v>1139</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>301</v>
       </c>
       <c r="C251" s="2"/>
     </row>
     <row r="252" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A252" s="6">
-        <v>464</v>
-      </c>
-      <c r="B252" s="3"/>
+        <v>740</v>
+      </c>
       <c r="C252" s="2"/>
     </row>
     <row r="253" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A253" s="6">
-        <v>523</v>
+        <v>464</v>
       </c>
       <c r="B253" s="3"/>
       <c r="C253" s="2"/>
     </row>
     <row r="254" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A254" s="6">
-        <v>956</v>
-      </c>
-      <c r="B254" s="3" t="s">
-        <v>303</v>
-      </c>
+        <v>523</v>
+      </c>
+      <c r="B254" s="3"/>
       <c r="C254" s="2"/>
     </row>
     <row r="255" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A255" s="6">
+        <v>956</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="C255" s="2"/>
+    </row>
+    <row r="256" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A256" s="6">
         <v>1320</v>
       </c>
-      <c r="B255" s="3"/>
-      <c r="C255" s="2"/>
-    </row>
-    <row r="256" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A256" s="6"/>
       <c r="B256" s="3"/>
       <c r="C256" s="2"/>
     </row>
-    <row r="257" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A257" s="5" t="s">
+    <row r="257" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A257" s="6"/>
+      <c r="B257" s="3"/>
+      <c r="C257" s="2"/>
+    </row>
+    <row r="258" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A258" s="5" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="258" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A258" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B258" s="6"/>
-      <c r="C258" s="6" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="259" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A259" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B259" s="6"/>
+      <c r="C259" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A260" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B259" s="6"/>
-      <c r="C259" s="6"/>
-      <c r="D259" s="6"/>
-    </row>
-    <row r="260" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A260" s="6">
-        <v>206</v>
-      </c>
-      <c r="B260" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C260" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B260" s="6"/>
+      <c r="C260" s="6"/>
       <c r="D260" s="6"/>
     </row>
     <row r="261" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A261" s="6">
-        <v>141</v>
-      </c>
-      <c r="B261" s="3" t="s">
-        <v>106</v>
+        <v>206</v>
+      </c>
+      <c r="B261" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="C261" s="2" t="s">
         <v>2</v>
@@ -4496,10 +4614,10 @@
     </row>
     <row r="262" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A262" s="6">
-        <v>24</v>
-      </c>
-      <c r="B262" s="10" t="s">
-        <v>107</v>
+        <v>141</v>
+      </c>
+      <c r="B262" s="3" t="s">
+        <v>106</v>
       </c>
       <c r="C262" s="2" t="s">
         <v>2</v>
@@ -4508,10 +4626,10 @@
     </row>
     <row r="263" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A263" s="6">
-        <v>328</v>
-      </c>
-      <c r="B263" s="3" t="s">
-        <v>108</v>
+        <v>24</v>
+      </c>
+      <c r="B263" s="10" t="s">
+        <v>107</v>
       </c>
       <c r="C263" s="2" t="s">
         <v>2</v>
@@ -4520,10 +4638,10 @@
     </row>
     <row r="264" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A264" s="6">
-        <v>92</v>
+        <v>328</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C264" s="2" t="s">
         <v>2</v>
@@ -4532,10 +4650,10 @@
     </row>
     <row r="265" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A265" s="6">
-        <v>237</v>
+        <v>92</v>
       </c>
       <c r="B265" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C265" s="2" t="s">
         <v>2</v>
@@ -4544,10 +4662,10 @@
     </row>
     <row r="266" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A266" s="6">
-        <v>19</v>
+        <v>237</v>
       </c>
       <c r="B266" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C266" s="2" t="s">
         <v>2</v>
@@ -4556,10 +4674,10 @@
     </row>
     <row r="267" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A267" s="6">
-        <v>83</v>
+        <v>19</v>
       </c>
       <c r="B267" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C267" s="2" t="s">
         <v>2</v>
@@ -4568,10 +4686,10 @@
     </row>
     <row r="268" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A268" s="6">
-        <v>203</v>
+        <v>83</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C268" s="2" t="s">
         <v>2</v>
@@ -4580,10 +4698,10 @@
     </row>
     <row r="269" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A269" s="6">
-        <v>82</v>
-      </c>
-      <c r="B269" s="10" t="s">
-        <v>114</v>
+        <v>203</v>
+      </c>
+      <c r="B269" s="3" t="s">
+        <v>113</v>
       </c>
       <c r="C269" s="2" t="s">
         <v>2</v>
@@ -4592,10 +4710,10 @@
     </row>
     <row r="270" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A270" s="6">
-        <v>369</v>
-      </c>
-      <c r="B270" s="3" t="s">
-        <v>115</v>
+        <v>82</v>
+      </c>
+      <c r="B270" s="10" t="s">
+        <v>114</v>
       </c>
       <c r="C270" s="2" t="s">
         <v>2</v>
@@ -4604,10 +4722,10 @@
     </row>
     <row r="271" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A271" s="6">
-        <v>2</v>
+        <v>369</v>
       </c>
       <c r="B271" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C271" s="2" t="s">
         <v>2</v>
@@ -4616,10 +4734,10 @@
     </row>
     <row r="272" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A272" s="6">
-        <v>160</v>
+        <v>2</v>
       </c>
       <c r="B272" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C272" s="2" t="s">
         <v>2</v>
@@ -4628,42 +4746,42 @@
     </row>
     <row r="273" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A273" s="6">
+        <v>160</v>
+      </c>
+      <c r="B273" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C273" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D273" s="6"/>
+    </row>
+    <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A274" s="6">
         <v>21</v>
       </c>
-      <c r="B273" s="3" t="s">
+      <c r="B274" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C273" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D273" s="6"/>
-    </row>
-    <row r="274" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A274" s="6" t="s">
+      <c r="C274" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D274" s="6"/>
+    </row>
+    <row r="275" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A275" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B274" s="7"/>
-      <c r="C274" s="6"/>
-      <c r="D274" s="6"/>
-    </row>
-    <row r="275" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A275" s="6">
-        <v>234</v>
-      </c>
-      <c r="B275" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="C275" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B275" s="7"/>
+      <c r="C275" s="6"/>
       <c r="D275" s="6"/>
     </row>
     <row r="276" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A276" s="6">
-        <v>143</v>
+        <v>234</v>
       </c>
       <c r="B276" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C276" s="2" t="s">
         <v>2</v>
@@ -4672,10 +4790,10 @@
     </row>
     <row r="277" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A277" s="6">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C277" s="2" t="s">
         <v>2</v>
@@ -4684,10 +4802,10 @@
     </row>
     <row r="278" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A278" s="6">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B278" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C278" s="2" t="s">
         <v>2</v>
@@ -4696,10 +4814,10 @@
     </row>
     <row r="279" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A279" s="6">
-        <v>25</v>
+        <v>148</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C279" s="2" t="s">
         <v>2</v>
@@ -4708,10 +4826,10 @@
     </row>
     <row r="280" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A280" s="6">
-        <v>61</v>
+        <v>25</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C280" s="2" t="s">
         <v>2</v>
@@ -4720,10 +4838,10 @@
     </row>
     <row r="281" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A281" s="6">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C281" s="2" t="s">
         <v>2</v>
@@ -4732,10 +4850,10 @@
     </row>
     <row r="282" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A282" s="6">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="B282" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C282" s="2" t="s">
         <v>2</v>
@@ -4744,44 +4862,44 @@
     </row>
     <row r="283" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A283" s="6">
+        <v>23</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C283" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D283" s="6"/>
+    </row>
+    <row r="284" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A284" s="6">
         <v>147</v>
       </c>
-      <c r="B283" s="3" t="s">
+      <c r="B284" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="286" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A286" s="5" t="s">
+    <row r="287" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A287" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="287" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A287" s="6" t="s">
+    <row r="288" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A288" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B287" s="6"/>
-      <c r="C287" s="6" t="s">
+      <c r="B288" s="6"/>
+      <c r="C288" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="288" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A288" s="6">
-        <v>200</v>
-      </c>
-      <c r="B288" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C288" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D288" s="6"/>
     </row>
     <row r="289" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A289" s="6">
-        <v>286</v>
+        <v>200</v>
       </c>
       <c r="B289" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C289" s="2" t="s">
         <v>2</v>
@@ -4790,10 +4908,10 @@
     </row>
     <row r="290" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A290" s="6">
-        <v>130</v>
+        <v>286</v>
       </c>
       <c r="B290" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C290" s="2" t="s">
         <v>2</v>
@@ -4802,10 +4920,10 @@
     </row>
     <row r="291" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A291" s="6">
-        <v>339</v>
+        <v>130</v>
       </c>
       <c r="B291" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C291" s="2" t="s">
         <v>2</v>
@@ -4814,10 +4932,10 @@
     </row>
     <row r="292" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A292" s="6">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="B292" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C292" s="2" t="s">
         <v>2</v>
@@ -4826,10 +4944,10 @@
     </row>
     <row r="293" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A293" s="6">
-        <v>127</v>
+        <v>364</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C293" s="2" t="s">
         <v>2</v>
@@ -4838,30 +4956,30 @@
     </row>
     <row r="294" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A294" s="6">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>138</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C294" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D294" s="6"/>
     </row>
     <row r="295" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A295" s="6">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B295" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C295" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D295" s="6"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="296" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A296" s="6">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B296" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C296" s="2" t="s">
         <v>2</v>
@@ -4870,51 +4988,51 @@
     </row>
     <row r="297" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A297" s="6">
+        <v>52</v>
+      </c>
+      <c r="B297" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C297" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D297" s="6"/>
+    </row>
+    <row r="298" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A298" s="6">
         <v>1192</v>
       </c>
-      <c r="B297" s="3" t="s">
+      <c r="B298" s="3" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="299" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A299" s="6"/>
-      <c r="B299" s="3"/>
-      <c r="C299" s="2"/>
-      <c r="D299" s="6"/>
-    </row>
-    <row r="300" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A300" s="5" t="s">
+    <row r="300" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A300" s="6"/>
+      <c r="B300" s="3"/>
+      <c r="C300" s="2"/>
+      <c r="D300" s="6"/>
+    </row>
+    <row r="301" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A301" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B300" s="8"/>
-    </row>
-    <row r="301" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A301" s="6" t="s">
+      <c r="B301" s="8"/>
+    </row>
+    <row r="302" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A302" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B301" s="7"/>
-      <c r="C301" s="6" t="s">
+      <c r="B302" s="7"/>
+      <c r="C302" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A302" s="6">
-        <v>261</v>
-      </c>
-      <c r="B302" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C302" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D302" s="6"/>
     </row>
     <row r="303" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A303" s="6">
-        <v>323</v>
+        <v>261</v>
       </c>
       <c r="B303" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C303" s="2" t="s">
         <v>2</v>
@@ -4923,62 +5041,62 @@
     </row>
     <row r="304" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A304" s="6">
+        <v>323</v>
+      </c>
+      <c r="B304" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C304" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D304" s="6"/>
+    </row>
+    <row r="305" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A305" s="6">
         <v>305</v>
       </c>
-      <c r="B304" s="3" t="s">
+      <c r="B305" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="305" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B305" s="8"/>
     </row>
     <row r="306" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B306" s="8"/>
     </row>
-    <row r="307" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A307" s="5" t="s">
+    <row r="307" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B307" s="8"/>
+    </row>
+    <row r="308" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A308" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="B307" s="8"/>
-    </row>
-    <row r="308" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A308" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B308" s="7"/>
-      <c r="C308" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D308" s="6" t="s">
-        <v>55</v>
-      </c>
+      <c r="B308" s="8"/>
     </row>
     <row r="309" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A309" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B309" s="7"/>
+      <c r="C309" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D309" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="310" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A310" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="B309" s="7"/>
-      <c r="C309" s="6"/>
-      <c r="D309" s="6"/>
-    </row>
-    <row r="310" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A310" s="6">
-        <v>133</v>
-      </c>
-      <c r="B310" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C310" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B310" s="7"/>
+      <c r="C310" s="6"/>
       <c r="D310" s="6"/>
     </row>
     <row r="311" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A311" s="6">
-        <v>399</v>
+        <v>133</v>
       </c>
       <c r="B311" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C311" s="2" t="s">
         <v>2</v>
@@ -4987,75 +5105,75 @@
     </row>
     <row r="312" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A312" s="6">
+        <v>399</v>
+      </c>
+      <c r="B312" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C312" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D312" s="6"/>
+    </row>
+    <row r="313" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A313" s="6">
         <v>310</v>
       </c>
-      <c r="B312" s="3" t="s">
+      <c r="B313" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C312" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D312" s="6"/>
-    </row>
-    <row r="313" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A313" s="6" t="s">
+      <c r="C313" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D313" s="6"/>
+    </row>
+    <row r="314" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A314" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="B313" s="7"/>
-      <c r="C313" s="6"/>
-      <c r="D313" s="6"/>
-    </row>
-    <row r="314" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A314" s="6">
+      <c r="B314" s="7"/>
+      <c r="C314" s="6"/>
+      <c r="D314" s="6"/>
+    </row>
+    <row r="315" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A315" s="6">
         <v>149</v>
       </c>
-      <c r="B314" s="3" t="s">
+      <c r="B315" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C314" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D314" s="6"/>
-    </row>
-    <row r="315" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B315" s="8"/>
+      <c r="C315" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D315" s="6"/>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B316" s="8"/>
     </row>
-    <row r="317" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A317" s="5" t="s">
+    <row r="317" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B317" s="8"/>
+    </row>
+    <row r="318" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A318" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="B317" s="8"/>
-    </row>
-    <row r="318" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A318" s="6" t="s">
+      <c r="B318" s="8"/>
+    </row>
+    <row r="319" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A319" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B318" s="7"/>
-      <c r="C318" s="6" t="s">
+      <c r="B319" s="7"/>
+      <c r="C319" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="319" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A319" s="6">
-        <v>208</v>
-      </c>
-      <c r="B319" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C319" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D319" s="6"/>
     </row>
     <row r="320" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A320" s="6">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C320" s="2" t="s">
         <v>2</v>
@@ -5064,48 +5182,48 @@
     </row>
     <row r="321" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A321" s="6">
+        <v>211</v>
+      </c>
+      <c r="B321" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C321" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D321" s="6"/>
+    </row>
+    <row r="322" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A322" s="6">
         <v>212</v>
       </c>
-      <c r="B321" s="3" t="s">
+      <c r="B322" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C321" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D321" s="6"/>
-    </row>
-    <row r="324" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A324" s="5" t="s">
+      <c r="C322" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D322" s="6"/>
+    </row>
+    <row r="325" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A325" s="5" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="325" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A325" s="6" t="s">
+    <row r="326" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A326" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B325" s="6"/>
-      <c r="C325" s="6" t="s">
+      <c r="B326" s="6"/>
+      <c r="C326" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="326" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A326" s="6">
-        <v>48</v>
-      </c>
-      <c r="B326" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="C326" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D326" s="6"/>
     </row>
     <row r="327" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A327" s="6">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C327" s="2" t="s">
         <v>2</v>
@@ -5114,10 +5232,10 @@
     </row>
     <row r="328" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A328" s="6">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C328" s="2" t="s">
         <v>2</v>
@@ -5126,10 +5244,10 @@
     </row>
     <row r="329" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A329" s="6">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C329" s="2" t="s">
         <v>2</v>
@@ -5138,10 +5256,10 @@
     </row>
     <row r="330" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A330" s="6">
-        <v>311</v>
+        <v>73</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C330" s="2" t="s">
         <v>2</v>
@@ -5150,10 +5268,10 @@
     </row>
     <row r="331" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A331" s="6">
-        <v>329</v>
+        <v>311</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C331" s="2" t="s">
         <v>2</v>
@@ -5162,10 +5280,10 @@
     </row>
     <row r="332" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A332" s="6">
-        <v>378</v>
+        <v>329</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C332" s="2" t="s">
         <v>2</v>
@@ -5174,10 +5292,10 @@
     </row>
     <row r="333" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A333" s="6">
-        <v>74</v>
+        <v>378</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C333" s="2" t="s">
         <v>2</v>
@@ -5186,10 +5304,10 @@
     </row>
     <row r="334" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A334" s="6">
-        <v>240</v>
+        <v>74</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C334" s="2" t="s">
         <v>2</v>
@@ -5198,10 +5316,10 @@
     </row>
     <row r="335" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A335" s="6">
-        <v>370</v>
+        <v>240</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C335" s="2" t="s">
         <v>2</v>
@@ -5210,10 +5328,10 @@
     </row>
     <row r="336" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A336" s="6">
-        <v>79</v>
+        <v>370</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C336" s="2" t="s">
         <v>2</v>
@@ -5222,10 +5340,10 @@
     </row>
     <row r="337" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A337" s="6">
-        <v>296</v>
+        <v>79</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C337" s="2" t="s">
         <v>2</v>
@@ -5234,10 +5352,10 @@
     </row>
     <row r="338" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A338" s="6">
-        <v>361</v>
+        <v>296</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C338" s="2" t="s">
         <v>2</v>
@@ -5246,10 +5364,10 @@
     </row>
     <row r="339" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A339" s="6">
-        <v>317</v>
+        <v>361</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C339" s="2" t="s">
         <v>2</v>
@@ -5258,10 +5376,10 @@
     </row>
     <row r="340" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A340" s="6">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C340" s="2" t="s">
         <v>2</v>
@@ -5270,10 +5388,10 @@
     </row>
     <row r="341" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A341" s="6">
-        <v>36</v>
+        <v>302</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C341" s="2" t="s">
         <v>2</v>
@@ -5282,83 +5400,83 @@
     </row>
     <row r="342" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A342" s="6">
+        <v>36</v>
+      </c>
+      <c r="B342" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C342" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D342" s="6"/>
+    </row>
+    <row r="343" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A343" s="6">
         <v>37</v>
       </c>
-      <c r="B342" s="2" t="s">
+      <c r="B343" s="2" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="346" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A346" s="5" t="s">
+    <row r="347" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A347" s="5" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="347" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A347" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B347" s="6"/>
-      <c r="C347" s="6"/>
-      <c r="D347" s="6"/>
     </row>
     <row r="348" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A348" s="6" t="s">
-        <v>231</v>
+        <v>53</v>
       </c>
       <c r="B348" s="6"/>
       <c r="C348" s="6"/>
       <c r="D348" s="6"/>
     </row>
     <row r="349" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A349" s="6">
+      <c r="A349" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="B349" s="6"/>
+      <c r="C349" s="6"/>
+      <c r="D349" s="6"/>
+    </row>
+    <row r="350" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A350" s="6">
         <v>155</v>
       </c>
-      <c r="B349" s="3" t="s">
+      <c r="B350" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="C349" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D349" s="6"/>
-    </row>
-    <row r="350" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A350" s="1">
-        <v>232</v>
-      </c>
-      <c r="B350" s="2" t="s">
-        <v>305</v>
-      </c>
       <c r="C350" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D350" s="1"/>
+      <c r="D350" s="6"/>
     </row>
     <row r="351" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A351" s="1">
+        <v>232</v>
+      </c>
+      <c r="B351" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="C351" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D351" s="1"/>
+    </row>
+    <row r="352" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A352" s="1">
         <v>225</v>
       </c>
-      <c r="B351" s="2" t="s">
+      <c r="B352" s="2" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="352" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A352" s="6">
-        <v>150</v>
-      </c>
-      <c r="B352" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="C352" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D352" s="6"/>
     </row>
     <row r="353" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A353" s="6">
-        <v>71</v>
+        <v>150</v>
       </c>
       <c r="B353" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C353" s="2" t="s">
         <v>2</v>
@@ -5367,10 +5485,10 @@
     </row>
     <row r="354" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A354" s="6">
-        <v>388</v>
+        <v>71</v>
       </c>
       <c r="B354" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C354" s="2" t="s">
         <v>2</v>
@@ -5379,10 +5497,10 @@
     </row>
     <row r="355" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A355" s="6">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C355" s="2" t="s">
         <v>2</v>
@@ -5391,10 +5509,10 @@
     </row>
     <row r="356" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A356" s="6">
-        <v>224</v>
+        <v>394</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C356" s="2" t="s">
         <v>2</v>
@@ -5403,10 +5521,10 @@
     </row>
     <row r="357" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A357" s="6">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B357" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C357" s="2" t="s">
         <v>2</v>
@@ -5415,10 +5533,10 @@
     </row>
     <row r="358" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A358" s="6">
-        <v>385</v>
+        <v>227</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C358" s="2" t="s">
         <v>2</v>
@@ -5427,42 +5545,42 @@
     </row>
     <row r="359" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A359" s="6">
+        <v>385</v>
+      </c>
+      <c r="B359" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C359" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D359" s="6"/>
+    </row>
+    <row r="360" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A360" s="6">
         <v>84</v>
       </c>
-      <c r="B359" s="3" t="s">
+      <c r="B360" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="C359" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D359" s="6"/>
-    </row>
-    <row r="360" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A360" s="6" t="s">
+      <c r="C360" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D360" s="6"/>
+    </row>
+    <row r="361" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A361" s="6" t="s">
         <v>241</v>
       </c>
-      <c r="B360" s="7"/>
-      <c r="C360" s="6"/>
-      <c r="D360" s="6"/>
-    </row>
-    <row r="361" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A361" s="6">
-        <v>215</v>
-      </c>
-      <c r="B361" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="C361" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B361" s="7"/>
+      <c r="C361" s="6"/>
       <c r="D361" s="6"/>
     </row>
     <row r="362" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A362" s="6">
-        <v>347</v>
+        <v>215</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C362" s="2" t="s">
         <v>2</v>
@@ -5471,10 +5589,10 @@
     </row>
     <row r="363" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A363" s="6">
-        <v>218</v>
+        <v>347</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C363" s="2" t="s">
         <v>2</v>
@@ -5483,10 +5601,10 @@
     </row>
     <row r="364" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A364" s="6">
-        <v>332</v>
+        <v>218</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C364" s="2" t="s">
         <v>2</v>
@@ -5495,94 +5613,94 @@
     </row>
     <row r="365" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A365" s="6">
+        <v>332</v>
+      </c>
+      <c r="B365" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C365" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D365" s="6"/>
+    </row>
+    <row r="366" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A366" s="6">
         <v>341</v>
       </c>
-      <c r="B365" s="3" t="s">
+      <c r="B366" s="3" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A366" t="s">
+    <row r="367" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A367" t="s">
         <v>302</v>
       </c>
-      <c r="B366" s="8"/>
-    </row>
-    <row r="367" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A367" s="6">
-        <v>1021</v>
-      </c>
-      <c r="B367" s="3" t="s">
-        <v>304</v>
-      </c>
+      <c r="B367" s="8"/>
     </row>
     <row r="368" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A368" s="6">
-        <v>456</v>
+        <v>1021</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="369" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A369" s="6">
-        <v>636</v>
+        <v>456</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="370" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A370" s="6">
-        <v>735</v>
+        <v>636</v>
       </c>
       <c r="B370" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="371" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A371" s="6">
+        <v>735</v>
+      </c>
+      <c r="B371" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="372" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A372" s="6">
         <v>880</v>
       </c>
-      <c r="B371" s="3" t="s">
+      <c r="B372" s="3" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="372" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A372" s="6"/>
-      <c r="B372" s="3"/>
-    </row>
-    <row r="375" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A375" s="5" t="s">
+    <row r="373" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A373" s="6"/>
+      <c r="B373" s="3"/>
+    </row>
+    <row r="376" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A376" s="5" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="376" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A376" s="6" t="s">
+    <row r="377" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A377" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B376" s="6"/>
-      <c r="C376" s="6" t="s">
+      <c r="B377" s="6"/>
+      <c r="C377" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="377" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A377" s="6">
-        <v>389</v>
-      </c>
-      <c r="B377" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C377" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D377" s="6"/>
     </row>
     <row r="378" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A378" s="6">
-        <v>136</v>
+        <v>389</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C378" s="2" t="s">
         <v>2</v>
@@ -5591,70 +5709,70 @@
     </row>
     <row r="379" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A379" s="6">
-        <v>318</v>
+        <v>136</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>250</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C379" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D379" s="6"/>
     </row>
     <row r="380" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A380" s="6">
+        <v>318</v>
+      </c>
+      <c r="B380" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="381" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A381" s="6">
         <v>169</v>
       </c>
-      <c r="B380" s="3" t="s">
+      <c r="B381" s="3" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="381" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A381" s="6"/>
-      <c r="B381" s="3" t="s">
+    <row r="382" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A382" s="6"/>
+      <c r="B382" s="3" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="382" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A382" s="6">
+    <row r="383" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A383" s="6">
         <v>268</v>
       </c>
-      <c r="B382" s="3" t="s">
+      <c r="B383" s="3" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="383" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A383" s="6"/>
-      <c r="B383" s="3"/>
-    </row>
-    <row r="386" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A386" s="5" t="s">
+    <row r="384" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A384" s="6"/>
+      <c r="B384" s="3"/>
+    </row>
+    <row r="387" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A387" s="5" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="387" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A387" s="6" t="s">
+    <row r="388" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A388" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B387" s="6"/>
-      <c r="C387" s="6" t="s">
+      <c r="B388" s="6"/>
+      <c r="C388" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="388" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A388" s="6">
-        <v>207</v>
-      </c>
-      <c r="B388" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="C388" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D388" s="6"/>
     </row>
     <row r="389" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A389" s="6">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C389" s="2" t="s">
         <v>2</v>
@@ -5663,44 +5781,44 @@
     </row>
     <row r="390" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A390" s="6">
+        <v>210</v>
+      </c>
+      <c r="B390" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D390" s="6"/>
+    </row>
+    <row r="391" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A391" s="6">
         <v>269</v>
       </c>
-      <c r="B390" s="2" t="s">
+      <c r="B391" s="2" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="393" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A393" s="5" t="s">
+    <row r="394" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A394" s="5" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="394" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A394" s="6" t="s">
+    <row r="395" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A395" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B394" s="6"/>
-      <c r="C394" s="6" t="s">
+      <c r="B395" s="6"/>
+      <c r="C395" s="6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="395" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A395" s="6">
-        <v>384</v>
-      </c>
-      <c r="B395" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C395" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D395" s="6"/>
     </row>
     <row r="396" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A396" s="6">
-        <v>398</v>
+        <v>384</v>
       </c>
       <c r="B396" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C396" s="2" t="s">
         <v>2</v>
@@ -5709,10 +5827,10 @@
     </row>
     <row r="397" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A397" s="6">
-        <v>382</v>
+        <v>398</v>
       </c>
       <c r="B397" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C397" s="2" t="s">
         <v>2</v>
@@ -5721,10 +5839,10 @@
     </row>
     <row r="398" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A398" s="6">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B398" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C398" s="2" t="s">
         <v>2</v>
@@ -5733,10 +5851,10 @@
     </row>
     <row r="399" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A399" s="6">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B399" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C399" s="2" t="s">
         <v>2</v>
@@ -5745,69 +5863,69 @@
     </row>
     <row r="400" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A400" s="6">
+        <v>381</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C400" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D400" s="6"/>
+    </row>
+    <row r="401" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A401" s="6">
         <v>138</v>
       </c>
-      <c r="B400" s="2" t="s">
+      <c r="B401" s="2" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="403" spans="1:4" ht="25" x14ac:dyDescent="0.25">
-      <c r="A403" s="5" t="s">
+    <row r="404" spans="1:4" ht="25" x14ac:dyDescent="0.25">
+      <c r="A404" s="5" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="404" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A404" s="6" t="s">
+    <row r="405" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A405" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B404" s="6"/>
-      <c r="C404" s="6"/>
-      <c r="D404" s="6"/>
-    </row>
-    <row r="405" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A405" s="6">
-        <v>359</v>
-      </c>
-      <c r="B405" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="C405" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="B405" s="6"/>
+      <c r="C405" s="6"/>
       <c r="D405" s="6"/>
     </row>
     <row r="406" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A406" s="6">
-        <v>346</v>
+        <v>359</v>
       </c>
       <c r="B406" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C406" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D406" s="6" t="s">
-        <v>176</v>
-      </c>
+      <c r="D406" s="6"/>
     </row>
     <row r="407" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A407" s="6">
-        <v>362</v>
+        <v>346</v>
       </c>
       <c r="B407" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C407" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D407" s="6"/>
+      <c r="D407" s="6" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="408" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A408" s="6">
-        <v>281</v>
+        <v>362</v>
       </c>
       <c r="B408" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C408" s="2" t="s">
         <v>2</v>
@@ -5816,10 +5934,10 @@
     </row>
     <row r="409" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A409" s="6">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B409" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C409" s="2" t="s">
         <v>2</v>
@@ -5828,10 +5946,10 @@
     </row>
     <row r="410" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A410" s="6">
-        <v>251</v>
+        <v>284</v>
       </c>
       <c r="B410" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C410" s="2" t="s">
         <v>2</v>
@@ -5840,10 +5958,10 @@
     </row>
     <row r="411" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A411" s="6">
-        <v>288</v>
+        <v>251</v>
       </c>
       <c r="B411" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C411" s="2" t="s">
         <v>2</v>
@@ -5852,10 +5970,10 @@
     </row>
     <row r="412" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A412" s="6">
-        <v>170</v>
-      </c>
-      <c r="B412" s="2" t="s">
-        <v>270</v>
+        <v>288</v>
+      </c>
+      <c r="B412" s="3" t="s">
+        <v>269</v>
       </c>
       <c r="C412" s="2" t="s">
         <v>2</v>
@@ -5864,10 +5982,10 @@
     </row>
     <row r="413" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A413" s="6">
-        <v>348</v>
+        <v>170</v>
       </c>
       <c r="B413" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C413" s="2" t="s">
         <v>2</v>
@@ -5876,10 +5994,10 @@
     </row>
     <row r="414" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A414" s="6">
-        <v>379</v>
+        <v>348</v>
       </c>
       <c r="B414" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C414" s="2" t="s">
         <v>2</v>
@@ -5888,10 +6006,10 @@
     </row>
     <row r="415" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A415" s="6">
-        <v>353</v>
+        <v>379</v>
       </c>
       <c r="B415" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C415" s="2" t="s">
         <v>2</v>
@@ -5900,10 +6018,10 @@
     </row>
     <row r="416" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A416" s="6">
-        <v>146</v>
+        <v>353</v>
       </c>
       <c r="B416" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C416" s="2" t="s">
         <v>2</v>
@@ -5912,10 +6030,10 @@
     </row>
     <row r="417" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A417" s="6">
-        <v>355</v>
+        <v>146</v>
       </c>
       <c r="B417" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C417" s="2" t="s">
         <v>2</v>
@@ -5924,10 +6042,10 @@
     </row>
     <row r="418" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A418" s="6">
-        <v>303</v>
+        <v>355</v>
       </c>
       <c r="B418" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C418" s="2" t="s">
         <v>2</v>
@@ -5936,10 +6054,10 @@
     </row>
     <row r="419" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A419" s="6">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B419" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C419" s="2" t="s">
         <v>2</v>
@@ -5948,24 +6066,22 @@
     </row>
     <row r="420" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A420" s="6">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B420" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C420" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D420" s="6" t="s">
-        <v>279</v>
-      </c>
+      <c r="D420" s="6"/>
     </row>
     <row r="421" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A421" s="6">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B421" s="2" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C421" s="2" t="s">
         <v>2</v>
@@ -5976,55 +6092,65 @@
     </row>
     <row r="422" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A422" s="6">
+        <v>308</v>
+      </c>
+      <c r="B422" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="C422" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D422" s="6" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="423" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A423" s="6">
         <v>705</v>
       </c>
-      <c r="B422" s="2" t="s">
+      <c r="B423" s="2" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="424" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A424" s="6">
+        <v>460</v>
+      </c>
+      <c r="B424" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="425" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A425" s="6">
         <v>3.31</v>
       </c>
     </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A425">
+    <row r="426" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A426">
         <v>697</v>
       </c>
-      <c r="B425" t="s">
+      <c r="B426" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="428" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A428" s="9" t="s">
+    <row r="429" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A429" s="9" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="429" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A429" s="1" t="s">
+    <row r="430" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A430" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B429" s="1"/>
-      <c r="C429" s="1"/>
-    </row>
-    <row r="430" spans="1:4" ht="17" x14ac:dyDescent="0.2">
-      <c r="A430" s="1">
-        <v>35</v>
-      </c>
-      <c r="B430" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="C430" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D430" s="1"/>
+      <c r="B430" s="1"/>
+      <c r="C430" s="1"/>
     </row>
     <row r="431" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A431" s="1">
-        <v>33</v>
-      </c>
-      <c r="B431" s="3" t="s">
-        <v>289</v>
+        <v>35</v>
+      </c>
+      <c r="B431" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="C431" s="2" t="s">
         <v>2</v>
@@ -6033,10 +6159,10 @@
     </row>
     <row r="432" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A432" s="1">
-        <v>81</v>
+        <v>33</v>
       </c>
       <c r="B432" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C432" s="2" t="s">
         <v>2</v>
@@ -6045,10 +6171,10 @@
     </row>
     <row r="433" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A433" s="1">
-        <v>153</v>
+        <v>81</v>
       </c>
       <c r="B433" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C433" s="2" t="s">
         <v>2</v>
@@ -6057,10 +6183,10 @@
     </row>
     <row r="434" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A434" s="1">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B434" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C434" s="2" t="s">
         <v>2</v>
@@ -6069,10 +6195,10 @@
     </row>
     <row r="435" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A435" s="1">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="B435" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C435" s="2" t="s">
         <v>2</v>
@@ -6081,10 +6207,10 @@
     </row>
     <row r="436" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A436" s="1">
-        <v>374</v>
+        <v>162</v>
       </c>
       <c r="B436" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C436" s="2" t="s">
         <v>2</v>
@@ -6093,10 +6219,10 @@
     </row>
     <row r="437" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A437" s="1">
-        <v>34</v>
+        <v>374</v>
       </c>
       <c r="B437" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C437" s="2" t="s">
         <v>2</v>
@@ -6105,10 +6231,10 @@
     </row>
     <row r="438" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A438" s="1">
-        <v>315</v>
+        <v>34</v>
       </c>
       <c r="B438" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C438" s="2" t="s">
         <v>2</v>
@@ -6117,10 +6243,10 @@
     </row>
     <row r="439" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A439" s="1">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="B439" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C439" s="2" t="s">
         <v>2</v>
@@ -6129,38 +6255,58 @@
     </row>
     <row r="440" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A440" s="1">
-        <v>354</v>
+        <v>300</v>
       </c>
       <c r="B440" s="3" t="s">
-        <v>298</v>
-      </c>
+        <v>297</v>
+      </c>
+      <c r="C440" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D440" s="1"/>
     </row>
     <row r="441" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A441" s="1">
-        <v>4</v>
-      </c>
-      <c r="B441" s="2" t="s">
-        <v>314</v>
+        <v>354</v>
+      </c>
+      <c r="B441" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="442" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A442" s="1">
+        <v>4</v>
+      </c>
+      <c r="B442" s="2" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="443" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A443" s="1">
         <v>50</v>
       </c>
-      <c r="B442" s="2" t="s">
+      <c r="B443" s="2" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="444" spans="1:4" ht="26" x14ac:dyDescent="0.3">
-      <c r="A444" s="9" t="s">
+    <row r="444" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+      <c r="A444" s="1">
+        <v>1922</v>
+      </c>
+      <c r="B444" s="2" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="445" spans="1:4" ht="26" x14ac:dyDescent="0.3">
+      <c r="A445" s="9" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="445" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A445">
+    <row r="446" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A446">
         <v>500</v>
       </c>
-      <c r="B445" t="s">
+      <c r="B446" t="s">
         <v>300</v>
       </c>
     </row>
@@ -6195,102 +6341,102 @@
     <hyperlink ref="C224" r:id="rId27" display="https://cspiration.com/login" xr:uid="{7CC75275-A0BF-C447-8C55-0AB512699970}"/>
     <hyperlink ref="B225" r:id="rId28" display="https://leetcode.com/problems/coin-change/description/" xr:uid="{4751D5B9-78E7-1647-A94D-B787C4C6DAC8}"/>
     <hyperlink ref="C225" r:id="rId29" display="https://cspiration.com/login" xr:uid="{28C04F21-7959-C243-A6A5-4EEA9824A11F}"/>
-    <hyperlink ref="B227" r:id="rId30" display="https://leetcode.com/problems/paint-house/description/" xr:uid="{214172F9-8AF6-3E47-B357-DF0ECA938323}"/>
-    <hyperlink ref="C227" r:id="rId31" display="https://cspiration.com/login" xr:uid="{E1DF89A1-C035-F641-8768-CBBCF01F840F}"/>
-    <hyperlink ref="B228" r:id="rId32" display="https://leetcode.com/problems/paint-house-ii/description/" xr:uid="{9A4DE787-F88D-2F4A-9F27-C1B70F6CD59D}"/>
-    <hyperlink ref="C228" r:id="rId33" display="https://cspiration.com/login" xr:uid="{97F2541A-D555-D84A-865E-1D86921D157B}"/>
-    <hyperlink ref="B229" r:id="rId34" display="https://leetcode.com/problems/minimum-path-sum/description/" xr:uid="{69C8688F-4E28-BA40-B91B-34FDFE61D22A}"/>
-    <hyperlink ref="C229" r:id="rId35" display="https://cspiration.com/login" xr:uid="{92947D08-E356-434A-AEBF-317ED0F505A2}"/>
-    <hyperlink ref="B230" r:id="rId36" display="https://leetcode.com/problems/edit-distance/description/" xr:uid="{8F920DC0-1839-3048-83E2-C217B9F055B4}"/>
-    <hyperlink ref="C230" r:id="rId37" display="https://cspiration.com/login" xr:uid="{114A9E34-5844-E643-8A42-B88E7BEE5AE8}"/>
-    <hyperlink ref="B231" r:id="rId38" display="https://leetcode.com/problems/interleaving-string/description/" xr:uid="{FB04174A-9C48-A348-94FC-5E90C130B28F}"/>
-    <hyperlink ref="C231" r:id="rId39" display="https://cspiration.com/login" xr:uid="{55EDDBB2-B431-BD49-A244-D1CDABCE4E26}"/>
-    <hyperlink ref="B232" r:id="rId40" display="https://leetcode.com/problems/dungeon-game/description/" xr:uid="{155A6047-D8EB-8547-834B-33CBBC47B8EA}"/>
-    <hyperlink ref="C232" r:id="rId41" display="https://cspiration.com/login" xr:uid="{6C5529D1-8C55-094E-A7F6-EE2EE2045AA3}"/>
-    <hyperlink ref="B233" r:id="rId42" display="https://leetcode.com/problems/maximal-square/description/" xr:uid="{4A8B0E3C-5E97-5C47-9A6E-2C2EDA6A9395}"/>
-    <hyperlink ref="C233" r:id="rId43" display="https://cspiration.com/login" xr:uid="{74A87B70-E6B2-4E4F-922E-9B55F53872E6}"/>
-    <hyperlink ref="B235" r:id="rId44" display="https://leetcode.com/problems/maximal-rectangle/description/" xr:uid="{3ADA6959-F24D-6146-B3F0-E982EB0C68F5}"/>
-    <hyperlink ref="C235" r:id="rId45" display="https://cspiration.com/login" xr:uid="{8B14C05B-DD8F-D443-8EAA-F17CA50D7366}"/>
-    <hyperlink ref="B236" r:id="rId46" display="https://leetcode.com/problems/max-sum-of-rectangle-no-larger-than-k/description/" xr:uid="{4AA58D7A-2220-7E48-94A8-240A6AFC7EB7}"/>
-    <hyperlink ref="C236" r:id="rId47" display="https://cspiration.com/login" xr:uid="{38081C3C-1B84-3A42-8B82-08867C75BE08}"/>
-    <hyperlink ref="B239" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
-    <hyperlink ref="C239" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
-    <hyperlink ref="B240" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
-    <hyperlink ref="C240" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
-    <hyperlink ref="B241" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
-    <hyperlink ref="C241" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
-    <hyperlink ref="B242" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
-    <hyperlink ref="C242" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
-    <hyperlink ref="B243" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
-    <hyperlink ref="C243" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
-    <hyperlink ref="B244" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
-    <hyperlink ref="B260" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
-    <hyperlink ref="C260" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
-    <hyperlink ref="B261" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
-    <hyperlink ref="C261" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
-    <hyperlink ref="B262" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
-    <hyperlink ref="C262" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
-    <hyperlink ref="B263" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
-    <hyperlink ref="C263" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
-    <hyperlink ref="B264" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
-    <hyperlink ref="C264" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
-    <hyperlink ref="B265" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
-    <hyperlink ref="C265" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
-    <hyperlink ref="B266" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
-    <hyperlink ref="C266" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
-    <hyperlink ref="B267" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
-    <hyperlink ref="C267" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
-    <hyperlink ref="B268" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
-    <hyperlink ref="C268" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
-    <hyperlink ref="B269" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
-    <hyperlink ref="C269" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
-    <hyperlink ref="B270" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
-    <hyperlink ref="C270" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
-    <hyperlink ref="B271" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
-    <hyperlink ref="C271" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
-    <hyperlink ref="B272" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
-    <hyperlink ref="C272" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
-    <hyperlink ref="B273" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
-    <hyperlink ref="C273" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
-    <hyperlink ref="B275" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
-    <hyperlink ref="C275" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
-    <hyperlink ref="B276" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
-    <hyperlink ref="C276" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
-    <hyperlink ref="B277" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
-    <hyperlink ref="C277" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
-    <hyperlink ref="B278" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
-    <hyperlink ref="C278" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
-    <hyperlink ref="B279" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
-    <hyperlink ref="C279" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
-    <hyperlink ref="B280" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
-    <hyperlink ref="C280" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
-    <hyperlink ref="B281" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
-    <hyperlink ref="C281" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
-    <hyperlink ref="B282" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
-    <hyperlink ref="C282" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
-    <hyperlink ref="B283" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
-    <hyperlink ref="B288" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
-    <hyperlink ref="C288" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
-    <hyperlink ref="B289" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
-    <hyperlink ref="C289" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
-    <hyperlink ref="B290" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
-    <hyperlink ref="C290" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
-    <hyperlink ref="B291" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
-    <hyperlink ref="C291" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
-    <hyperlink ref="B292" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
-    <hyperlink ref="C292" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
-    <hyperlink ref="B293" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
-    <hyperlink ref="C293" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
-    <hyperlink ref="B295" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
-    <hyperlink ref="C295" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
-    <hyperlink ref="B296" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
-    <hyperlink ref="C296" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
-    <hyperlink ref="B294" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
-    <hyperlink ref="B302" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
-    <hyperlink ref="C302" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
-    <hyperlink ref="B303" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
-    <hyperlink ref="C303" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
-    <hyperlink ref="B304" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
+    <hyperlink ref="B228" r:id="rId30" display="https://leetcode.com/problems/paint-house/description/" xr:uid="{214172F9-8AF6-3E47-B357-DF0ECA938323}"/>
+    <hyperlink ref="C228" r:id="rId31" display="https://cspiration.com/login" xr:uid="{E1DF89A1-C035-F641-8768-CBBCF01F840F}"/>
+    <hyperlink ref="B229" r:id="rId32" display="https://leetcode.com/problems/paint-house-ii/description/" xr:uid="{9A4DE787-F88D-2F4A-9F27-C1B70F6CD59D}"/>
+    <hyperlink ref="C229" r:id="rId33" display="https://cspiration.com/login" xr:uid="{97F2541A-D555-D84A-865E-1D86921D157B}"/>
+    <hyperlink ref="B230" r:id="rId34" display="https://leetcode.com/problems/minimum-path-sum/description/" xr:uid="{69C8688F-4E28-BA40-B91B-34FDFE61D22A}"/>
+    <hyperlink ref="C230" r:id="rId35" display="https://cspiration.com/login" xr:uid="{92947D08-E356-434A-AEBF-317ED0F505A2}"/>
+    <hyperlink ref="B231" r:id="rId36" display="https://leetcode.com/problems/edit-distance/description/" xr:uid="{8F920DC0-1839-3048-83E2-C217B9F055B4}"/>
+    <hyperlink ref="C231" r:id="rId37" display="https://cspiration.com/login" xr:uid="{114A9E34-5844-E643-8A42-B88E7BEE5AE8}"/>
+    <hyperlink ref="B232" r:id="rId38" display="https://leetcode.com/problems/interleaving-string/description/" xr:uid="{FB04174A-9C48-A348-94FC-5E90C130B28F}"/>
+    <hyperlink ref="C232" r:id="rId39" display="https://cspiration.com/login" xr:uid="{55EDDBB2-B431-BD49-A244-D1CDABCE4E26}"/>
+    <hyperlink ref="B233" r:id="rId40" display="https://leetcode.com/problems/dungeon-game/description/" xr:uid="{155A6047-D8EB-8547-834B-33CBBC47B8EA}"/>
+    <hyperlink ref="C233" r:id="rId41" display="https://cspiration.com/login" xr:uid="{6C5529D1-8C55-094E-A7F6-EE2EE2045AA3}"/>
+    <hyperlink ref="B234" r:id="rId42" display="https://leetcode.com/problems/maximal-square/description/" xr:uid="{4A8B0E3C-5E97-5C47-9A6E-2C2EDA6A9395}"/>
+    <hyperlink ref="C234" r:id="rId43" display="https://cspiration.com/login" xr:uid="{74A87B70-E6B2-4E4F-922E-9B55F53872E6}"/>
+    <hyperlink ref="B236" r:id="rId44" display="https://leetcode.com/problems/maximal-rectangle/description/" xr:uid="{3ADA6959-F24D-6146-B3F0-E982EB0C68F5}"/>
+    <hyperlink ref="C236" r:id="rId45" display="https://cspiration.com/login" xr:uid="{8B14C05B-DD8F-D443-8EAA-F17CA50D7366}"/>
+    <hyperlink ref="B237" r:id="rId46" display="https://leetcode.com/problems/max-sum-of-rectangle-no-larger-than-k/description/" xr:uid="{4AA58D7A-2220-7E48-94A8-240A6AFC7EB7}"/>
+    <hyperlink ref="C237" r:id="rId47" display="https://cspiration.com/login" xr:uid="{38081C3C-1B84-3A42-8B82-08867C75BE08}"/>
+    <hyperlink ref="B240" r:id="rId48" display="https://leetcode.com/problems/house-robber/" xr:uid="{B5F79A46-6E6F-8D4D-889A-60A17000B0ED}"/>
+    <hyperlink ref="C240" r:id="rId49" display="https://cspiration.com/login" xr:uid="{40EE7912-E2ED-8F48-927A-5A0F117CEC11}"/>
+    <hyperlink ref="B241" r:id="rId50" xr:uid="{DA479ECE-2810-4D46-9167-CD93688286E5}"/>
+    <hyperlink ref="C241" r:id="rId51" display="https://cspiration.com/login" xr:uid="{0B397A8A-6F6D-074D-B34F-CBCC7962B019}"/>
+    <hyperlink ref="B242" r:id="rId52" display="https://leetcode.com/problems/paint-fence/description/" xr:uid="{8DF87316-E5E3-A64B-A7C7-B412886C0D62}"/>
+    <hyperlink ref="C242" r:id="rId53" display="https://cspiration.com/login" xr:uid="{6E65F3C4-E1DF-704A-B81E-19F926EFE944}"/>
+    <hyperlink ref="B243" r:id="rId54" display="https://leetcode.com/problems/decode-ways/description/" xr:uid="{2DC138A9-B627-AB47-870B-14C94AB6B5A4}"/>
+    <hyperlink ref="C243" r:id="rId55" display="https://cspiration.com/login" xr:uid="{5A7C9135-5860-E948-BD21-C28BD1B3E946}"/>
+    <hyperlink ref="B244" r:id="rId56" display="https://leetcode.com/problems/regular-expression-matching/description/" xr:uid="{7D23B339-6C91-614E-AA49-72CB80D8755F}"/>
+    <hyperlink ref="C244" r:id="rId57" display="https://cspiration.com/login" xr:uid="{11D5A1C5-180C-5441-9789-596C0046C716}"/>
+    <hyperlink ref="B245" r:id="rId58" display="https://leetcode.com/problems/wildcard-matching/description/" xr:uid="{30C25CED-6E0E-1744-B664-F8C8620F6075}"/>
+    <hyperlink ref="B261" r:id="rId59" display="https://leetcode.com/problems/reverse-linked-list/description/" xr:uid="{CAD13304-EA56-2F44-88DC-9847AB46A009}"/>
+    <hyperlink ref="C261" r:id="rId60" display="https://cspiration.com/login" xr:uid="{EEC2B0F6-4485-EF40-9194-9F4EEA02F22A}"/>
+    <hyperlink ref="B262" r:id="rId61" display="https://leetcode.com/problems/linked-list-cycle/description/" xr:uid="{4FF87EA4-A503-4B49-87BA-62460FACC174}"/>
+    <hyperlink ref="C262" r:id="rId62" display="https://cspiration.com/login" xr:uid="{2DB2DFAD-3FB0-6D4E-9313-5085428A8CFC}"/>
+    <hyperlink ref="B263" r:id="rId63" display="https://leetcode.com/problems/swap-nodes-in-pairs/description/" xr:uid="{6D7DEEF5-7FBB-E84E-914B-265CD96477D2}"/>
+    <hyperlink ref="C263" r:id="rId64" display="https://cspiration.com/login" xr:uid="{514CAD90-796B-F448-A3DC-33D8613DF5B1}"/>
+    <hyperlink ref="B264" r:id="rId65" display="https://leetcode.com/problems/odd-even-linked-list/description/" xr:uid="{69C095DA-C246-B14D-853C-13F1A137AECA}"/>
+    <hyperlink ref="C264" r:id="rId66" display="https://cspiration.com/login" xr:uid="{684EE302-5E2B-8F42-9B02-16D97EC48A9E}"/>
+    <hyperlink ref="B265" r:id="rId67" display="https://leetcode.com/problems/reverse-linked-list-ii/description/" xr:uid="{C591448F-1446-604A-BF63-B4B8E771CAE4}"/>
+    <hyperlink ref="C265" r:id="rId68" display="https://cspiration.com/login" xr:uid="{AD139FD1-62E2-DE44-9EAD-FB7CE24CFEC6}"/>
+    <hyperlink ref="B266" r:id="rId69" display="https://leetcode.com/problems/delete-node-in-a-linked-list/description/" xr:uid="{A3C665A2-4693-4E48-9309-83A49B99EB9E}"/>
+    <hyperlink ref="C266" r:id="rId70" display="https://cspiration.com/login" xr:uid="{FB2A27A5-F4E1-4348-ABC3-DFB3C11A3805}"/>
+    <hyperlink ref="B267" r:id="rId71" display="https://leetcode.com/problems/remove-nth-node-from-end-of-list/description/" xr:uid="{936FBC23-FBA0-8041-B01E-927C44DBFBD0}"/>
+    <hyperlink ref="C267" r:id="rId72" display="https://cspiration.com/login" xr:uid="{3A577495-48A7-3E4B-B2EF-CA1F5B535933}"/>
+    <hyperlink ref="B268" r:id="rId73" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list/description/" xr:uid="{CC7DDE3B-80A1-C949-9A7B-0BAD12D0B738}"/>
+    <hyperlink ref="C268" r:id="rId74" display="https://cspiration.com/login" xr:uid="{7EA05564-C028-584C-A89F-4B344D5446DC}"/>
+    <hyperlink ref="B269" r:id="rId75" display="https://leetcode.com/problems/remove-linked-list-elements/description/" xr:uid="{C103719A-34B5-4648-B53B-B44C590DF483}"/>
+    <hyperlink ref="C269" r:id="rId76" display="https://cspiration.com/login" xr:uid="{911D9C1F-B252-0C44-B709-A88E12866DB8}"/>
+    <hyperlink ref="B270" r:id="rId77" display="https://leetcode.com/problems/remove-duplicates-from-sorted-list-ii/description/" xr:uid="{659D5183-DD4E-8D47-B021-9AA1D4C417EC}"/>
+    <hyperlink ref="C270" r:id="rId78" display="https://cspiration.com/login" xr:uid="{5605BF37-B4B3-D347-B524-042D61B8AB56}"/>
+    <hyperlink ref="B271" r:id="rId79" display="https://leetcode.com/problems/plus-one-linked-list/description/" xr:uid="{B0513CEC-73FA-E446-9EDB-D84142ACA483}"/>
+    <hyperlink ref="C271" r:id="rId80" display="https://cspiration.com/login" xr:uid="{10119304-066A-6247-80D0-401AA1203D0D}"/>
+    <hyperlink ref="B272" r:id="rId81" display="https://leetcode.com/problems/add-two-numbers/description/" xr:uid="{93006D26-E920-6C49-B26A-FCB8CAB1ACA3}"/>
+    <hyperlink ref="C272" r:id="rId82" display="https://cspiration.com/login" xr:uid="{9291616C-0B43-C94B-8A1E-8F898F4BF56B}"/>
+    <hyperlink ref="B273" r:id="rId83" display="https://leetcode.com/problems/intersection-of-two-linked-lists/description/" xr:uid="{1FA22F67-4FD1-9042-A730-D5586D418640}"/>
+    <hyperlink ref="C273" r:id="rId84" display="https://cspiration.com/login" xr:uid="{35A8D267-2907-7841-858E-4D9067911073}"/>
+    <hyperlink ref="B274" r:id="rId85" display="https://leetcode.com/problems/merge-two-sorted-lists/description/" xr:uid="{B4017010-0B98-A146-993E-1784ADCBA2ED}"/>
+    <hyperlink ref="C274" r:id="rId86" display="https://cspiration.com/login" xr:uid="{621DD98A-3C93-3645-B68C-CA4ED618EE02}"/>
+    <hyperlink ref="B276" r:id="rId87" display="https://leetcode.com/problems/palindrome-linked-list/description/" xr:uid="{8246AC1C-1D21-4040-87D8-0C088584A020}"/>
+    <hyperlink ref="C276" r:id="rId88" display="https://cspiration.com/login" xr:uid="{967A4BA0-C65A-AB47-97BE-157F10FE4DB7}"/>
+    <hyperlink ref="B277" r:id="rId89" display="https://leetcode.com/problems/reorder-list/description/" xr:uid="{78F44725-1FA2-D241-8683-EE8B2ED5FA0B}"/>
+    <hyperlink ref="C277" r:id="rId90" display="https://cspiration.com/login" xr:uid="{6C7AF4CB-7495-7148-A674-7878A9F00B7A}"/>
+    <hyperlink ref="B278" r:id="rId91" display="https://leetcode.com/problems/linked-list-cycle-ii/description/" xr:uid="{7614D580-270B-BA4B-95E7-882D4141A0E9}"/>
+    <hyperlink ref="C278" r:id="rId92" display="https://cspiration.com/login" xr:uid="{910601B3-BDE1-E54F-B6A7-F89C17F9424F}"/>
+    <hyperlink ref="B279" r:id="rId93" display="https://leetcode.com/problems/sort-list/description/" xr:uid="{E32778EB-01D7-9545-8442-3B4CFBC2B3BC}"/>
+    <hyperlink ref="C279" r:id="rId94" display="https://cspiration.com/login" xr:uid="{62472AF2-4F6F-3643-960E-F5889C4A4F00}"/>
+    <hyperlink ref="B280" r:id="rId95" display="https://leetcode.com/problems/reverse-nodes-in-k-group/description/" xr:uid="{01D9B3AE-536F-8A4C-90F2-F9960A62121F}"/>
+    <hyperlink ref="C280" r:id="rId96" display="https://cspiration.com/login" xr:uid="{499891E2-9FA3-6D4F-B1BF-FF821B50DC7F}"/>
+    <hyperlink ref="B281" r:id="rId97" display="https://leetcode.com/problems/rotate-list/description/" xr:uid="{676DED51-3A3A-7A44-9090-B3319F92D1F5}"/>
+    <hyperlink ref="C281" r:id="rId98" display="https://cspiration.com/login" xr:uid="{62C8D600-08B2-B049-8ED4-3989C28788DB}"/>
+    <hyperlink ref="B282" r:id="rId99" display="https://leetcode.com/problems/partition-list/description/" xr:uid="{1A0016B2-865D-8648-B9C1-009775D448B9}"/>
+    <hyperlink ref="C282" r:id="rId100" display="https://cspiration.com/login" xr:uid="{F67C87BE-0A6D-4E43-8B60-EE98D2553167}"/>
+    <hyperlink ref="B283" r:id="rId101" display="https://leetcode.com/problems/merge-k-sorted-lists/description/" xr:uid="{AB470A71-9B7C-DD4D-A53C-D986109A764A}"/>
+    <hyperlink ref="C283" r:id="rId102" display="https://cspiration.com/login" xr:uid="{389A6086-F8A2-1A4C-90D7-865417B49C2E}"/>
+    <hyperlink ref="B284" r:id="rId103" display="https://leetcode.com/problems/insertion-sort-list/description/" xr:uid="{435F18B5-F857-FE40-AEB8-BC637F8007F6}"/>
+    <hyperlink ref="B289" r:id="rId104" display="https://leetcode.com/problems/number-of-islands/" xr:uid="{17D6F74D-E884-8346-80CA-C43FAFD204E0}"/>
+    <hyperlink ref="C289" r:id="rId105" display="https://cspiration.com/login" xr:uid="{5B75D74F-E84F-1749-89B8-F2F96B20B5DF}"/>
+    <hyperlink ref="B290" r:id="rId106" display="https://leetcode.com/problems/walls-and-gates/description/" xr:uid="{F15086C1-E83C-6749-9F98-C2FE6061D983}"/>
+    <hyperlink ref="C290" r:id="rId107" display="https://cspiration.com/login" xr:uid="{C11E20A3-768E-204B-A6A7-87721BBD91F2}"/>
+    <hyperlink ref="B291" r:id="rId108" display="https://leetcode.com/problems/surrounded-regions/description/" xr:uid="{13C0DF7E-F852-7048-8D5A-1494162FBD03}"/>
+    <hyperlink ref="C291" r:id="rId109" display="https://cspiration.com/login" xr:uid="{91126A94-99DE-7142-9CB0-1A5A4AC524B2}"/>
+    <hyperlink ref="B292" r:id="rId110" display="https://leetcode.com/problems/nested-list-weight-sum/description/" xr:uid="{E7980BDA-D944-614B-BB28-B03847BEF845}"/>
+    <hyperlink ref="C292" r:id="rId111" display="https://cspiration.com/login" xr:uid="{412FD8CC-DFA9-C242-838C-0B0C00423954}"/>
+    <hyperlink ref="B293" r:id="rId112" display="https://leetcode.com/problems/nested-list-weight-sum-ii/description/" xr:uid="{5F518178-7D34-894B-AFB1-4359E09F5303}"/>
+    <hyperlink ref="C293" r:id="rId113" display="https://cspiration.com/login" xr:uid="{A316D189-16C5-264D-B0B9-3ECE99D2BCAE}"/>
+    <hyperlink ref="B294" r:id="rId114" display="https://leetcode.com/problems/word-ladder/description/" xr:uid="{1546D9A2-6405-E445-A9E8-0FEB5B7A6A92}"/>
+    <hyperlink ref="C294" r:id="rId115" display="https://cspiration.com/login" xr:uid="{66335B9A-3643-EA44-A95E-77568BECFBFC}"/>
+    <hyperlink ref="B296" r:id="rId116" display="https://leetcode.com/problems/n-queens/" xr:uid="{989C02AD-8353-FA40-B6B2-7B3417C6D65A}"/>
+    <hyperlink ref="C296" r:id="rId117" display="https://cspiration.com/login" xr:uid="{74CDF51A-C100-4B4B-95BA-A7BFDFBB247F}"/>
+    <hyperlink ref="B297" r:id="rId118" display="https://leetcode.com/problems/n-queens-ii/description/" xr:uid="{CC4D02DA-3B9F-1B4D-A5AE-32B6014A8377}"/>
+    <hyperlink ref="C297" r:id="rId119" display="https://cspiration.com/login" xr:uid="{386CCEE6-EB73-DC46-9B1D-1D2761A09916}"/>
+    <hyperlink ref="B295" r:id="rId120" display="https://leetcode.com/problems/word-ladder-ii/description/" xr:uid="{4806144A-562E-064F-AE97-03B015936AE9}"/>
+    <hyperlink ref="B303" r:id="rId121" display="https://leetcode.com/problems/graph-valid-tree/description/" xr:uid="{0C7AB482-8E3B-AE4E-95F7-71384A61046F}"/>
+    <hyperlink ref="C303" r:id="rId122" display="https://cspiration.com/login" xr:uid="{66A9F717-5A05-CB41-A5FE-7139AEE4B2DB}"/>
+    <hyperlink ref="B304" r:id="rId123" display="https://leetcode.com/problems/number-of-connected-components-in-an-undirected-graph/description/" xr:uid="{70C86389-E813-DE4D-8FA6-8789189E3004}"/>
+    <hyperlink ref="C304" r:id="rId124" display="https://cspiration.com/login" xr:uid="{1450EFE5-357E-6145-B5D0-87DF6219A644}"/>
+    <hyperlink ref="B305" r:id="rId125" display="https://leetcode.com/problems/number-of-islands-ii/description/" xr:uid="{E823C3A6-A86F-964C-8988-1E7E87DD764D}"/>
     <hyperlink ref="B159" r:id="rId126" display="https://leetcode.com/problems/minimum-depth-of-binary-tree/description/" xr:uid="{89D22C44-568D-2A43-84A7-D669E16D4993}"/>
     <hyperlink ref="C159" r:id="rId127" display="https://cspiration.com/login" xr:uid="{CDC90D9B-21B1-9F4E-BBAE-19128D12CFDA}"/>
     <hyperlink ref="B161" r:id="rId128" display="https://leetcode.com/problems/maximum-depth-of-binary-tree/description/" xr:uid="{93D570CB-F2FC-D841-9EFB-185B9F3C2E70}"/>
@@ -6435,175 +6581,175 @@
     <hyperlink ref="C140" r:id="rId267" display="https://cspiration.com/login" xr:uid="{C5087984-A06B-4248-8E74-E2539F4CAF6A}"/>
     <hyperlink ref="B141" r:id="rId268" display="https://leetcode.com/problems/repeated-dna-sequences/description/" xr:uid="{52566213-99F8-BA41-B322-FDF32A868B37}"/>
     <hyperlink ref="C141" r:id="rId269" display="https://cspiration.com/login" xr:uid="{149752EA-7A00-384E-BE6B-4D94705BC736}"/>
-    <hyperlink ref="B310" r:id="rId270" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
-    <hyperlink ref="C310" r:id="rId271" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
-    <hyperlink ref="B311" r:id="rId272" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
-    <hyperlink ref="C311" r:id="rId273" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
-    <hyperlink ref="B312" r:id="rId274" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
-    <hyperlink ref="C312" r:id="rId275" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
-    <hyperlink ref="B314" r:id="rId276" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
-    <hyperlink ref="C314" r:id="rId277" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
-    <hyperlink ref="B320" r:id="rId278" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
-    <hyperlink ref="C320" r:id="rId279" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
-    <hyperlink ref="B319" r:id="rId280" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
-    <hyperlink ref="C319" r:id="rId281" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
-    <hyperlink ref="B321" r:id="rId282" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
-    <hyperlink ref="C321" r:id="rId283" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
-    <hyperlink ref="B326" r:id="rId284" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
-    <hyperlink ref="C326" r:id="rId285" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
-    <hyperlink ref="B327" r:id="rId286" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
-    <hyperlink ref="C327" r:id="rId287" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
-    <hyperlink ref="B328" r:id="rId288" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
-    <hyperlink ref="C328" r:id="rId289" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
-    <hyperlink ref="B329" r:id="rId290" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
-    <hyperlink ref="C329" r:id="rId291" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
-    <hyperlink ref="B330" r:id="rId292" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
-    <hyperlink ref="C330" r:id="rId293" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
-    <hyperlink ref="B331" r:id="rId294" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
-    <hyperlink ref="C331" r:id="rId295" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
-    <hyperlink ref="B332" r:id="rId296" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
-    <hyperlink ref="C332" r:id="rId297" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
-    <hyperlink ref="B333" r:id="rId298" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
-    <hyperlink ref="C333" r:id="rId299" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
-    <hyperlink ref="B334" r:id="rId300" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
-    <hyperlink ref="C334" r:id="rId301" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
-    <hyperlink ref="B335" r:id="rId302" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
-    <hyperlink ref="C335" r:id="rId303" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
-    <hyperlink ref="B336" r:id="rId304" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
-    <hyperlink ref="C336" r:id="rId305" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
-    <hyperlink ref="B337" r:id="rId306" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
-    <hyperlink ref="C337" r:id="rId307" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
-    <hyperlink ref="B338" r:id="rId308" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
-    <hyperlink ref="C338" r:id="rId309" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
-    <hyperlink ref="B339" r:id="rId310" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
-    <hyperlink ref="C339" r:id="rId311" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
-    <hyperlink ref="B340" r:id="rId312" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
-    <hyperlink ref="C340" r:id="rId313" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
-    <hyperlink ref="B341" r:id="rId314" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
-    <hyperlink ref="C341" r:id="rId315" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
-    <hyperlink ref="B342" r:id="rId316" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
-    <hyperlink ref="B349" r:id="rId317" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
-    <hyperlink ref="C349" r:id="rId318" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
-    <hyperlink ref="B352" r:id="rId319" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
-    <hyperlink ref="C352" r:id="rId320" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
-    <hyperlink ref="B353" r:id="rId321" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
-    <hyperlink ref="C353" r:id="rId322" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
-    <hyperlink ref="B354" r:id="rId323" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
-    <hyperlink ref="C354" r:id="rId324" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
-    <hyperlink ref="B355" r:id="rId325" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
-    <hyperlink ref="C355" r:id="rId326" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
-    <hyperlink ref="B356" r:id="rId327" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
-    <hyperlink ref="C356" r:id="rId328" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
-    <hyperlink ref="B357" r:id="rId329" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
-    <hyperlink ref="C357" r:id="rId330" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
-    <hyperlink ref="B358" r:id="rId331" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
-    <hyperlink ref="C358" r:id="rId332" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
-    <hyperlink ref="B359" r:id="rId333" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
-    <hyperlink ref="C359" r:id="rId334" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
-    <hyperlink ref="B361" r:id="rId335" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
-    <hyperlink ref="C361" r:id="rId336" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
-    <hyperlink ref="B362" r:id="rId337" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
-    <hyperlink ref="C362" r:id="rId338" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
-    <hyperlink ref="B363" r:id="rId339" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
-    <hyperlink ref="C363" r:id="rId340" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
-    <hyperlink ref="B364" r:id="rId341" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
-    <hyperlink ref="C364" r:id="rId342" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
-    <hyperlink ref="B365" r:id="rId343" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
-    <hyperlink ref="B377" r:id="rId344" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
-    <hyperlink ref="C377" r:id="rId345" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
-    <hyperlink ref="B378" r:id="rId346" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
-    <hyperlink ref="C378" r:id="rId347" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
-    <hyperlink ref="B379" r:id="rId348" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
-    <hyperlink ref="B388" r:id="rId349" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
-    <hyperlink ref="C388" r:id="rId350" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
-    <hyperlink ref="B389" r:id="rId351" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
-    <hyperlink ref="C389" r:id="rId352" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
-    <hyperlink ref="B390" r:id="rId353" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
-    <hyperlink ref="B395" r:id="rId354" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
-    <hyperlink ref="C395" r:id="rId355" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
-    <hyperlink ref="B396" r:id="rId356" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
-    <hyperlink ref="C396" r:id="rId357" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
-    <hyperlink ref="B397" r:id="rId358" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
-    <hyperlink ref="C397" r:id="rId359" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
-    <hyperlink ref="B398" r:id="rId360" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
-    <hyperlink ref="C398" r:id="rId361" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
-    <hyperlink ref="B399" r:id="rId362" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
-    <hyperlink ref="C399" r:id="rId363" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
-    <hyperlink ref="B400" r:id="rId364" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
-    <hyperlink ref="B405" r:id="rId365" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
-    <hyperlink ref="C405" r:id="rId366" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
-    <hyperlink ref="B406" r:id="rId367" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
-    <hyperlink ref="C406" r:id="rId368" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
-    <hyperlink ref="B407" r:id="rId369" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
-    <hyperlink ref="C407" r:id="rId370" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
-    <hyperlink ref="B408" r:id="rId371" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
-    <hyperlink ref="C408" r:id="rId372" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
-    <hyperlink ref="B409" r:id="rId373" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
-    <hyperlink ref="C409" r:id="rId374" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
-    <hyperlink ref="B410" r:id="rId375" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
-    <hyperlink ref="C410" r:id="rId376" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
-    <hyperlink ref="B411" r:id="rId377" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
-    <hyperlink ref="C411" r:id="rId378" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
-    <hyperlink ref="B412" r:id="rId379" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
-    <hyperlink ref="C412" r:id="rId380" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
-    <hyperlink ref="B413" r:id="rId381" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
-    <hyperlink ref="C413" r:id="rId382" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
-    <hyperlink ref="B414" r:id="rId383" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
-    <hyperlink ref="C414" r:id="rId384" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
-    <hyperlink ref="B415" r:id="rId385" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
-    <hyperlink ref="C415" r:id="rId386" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
-    <hyperlink ref="B416" r:id="rId387" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
-    <hyperlink ref="C416" r:id="rId388" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
-    <hyperlink ref="B417" r:id="rId389" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
-    <hyperlink ref="C417" r:id="rId390" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
-    <hyperlink ref="B418" r:id="rId391" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
-    <hyperlink ref="C418" r:id="rId392" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
-    <hyperlink ref="B419" r:id="rId393" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
-    <hyperlink ref="C419" r:id="rId394" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
-    <hyperlink ref="B420" r:id="rId395" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
-    <hyperlink ref="C420" r:id="rId396" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
-    <hyperlink ref="B421" r:id="rId397" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
-    <hyperlink ref="C421" r:id="rId398" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
-    <hyperlink ref="B422" r:id="rId399" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
+    <hyperlink ref="B311" r:id="rId270" display="https://leetcode.com/problems/clone-graph/description/" xr:uid="{17716DFB-246E-F541-ADE8-3C4BD1A5E4A4}"/>
+    <hyperlink ref="C311" r:id="rId271" display="https://cspiration.com/login" xr:uid="{C1525D83-A13A-C447-8396-6EBF12F9B87D}"/>
+    <hyperlink ref="B312" r:id="rId272" display="https://leetcode.com/problems/evaluate-division/description/" xr:uid="{EAD87AE8-0480-3C4B-807B-D62A0472E319}"/>
+    <hyperlink ref="C312" r:id="rId273" display="https://cspiration.com/login" xr:uid="{43BD2347-F360-C04E-8364-8BBF7050275F}"/>
+    <hyperlink ref="B313" r:id="rId274" display="https://leetcode.com/problems/minimum-height-trees/description/" xr:uid="{BFD584EF-C833-874F-869D-8CC1D25F985B}"/>
+    <hyperlink ref="C313" r:id="rId275" display="https://cspiration.com/login" xr:uid="{7F15D8C0-1B84-FC4E-8CD8-570269CEFD38}"/>
+    <hyperlink ref="B315" r:id="rId276" display="https://leetcode.com/problems/max-points-on-a-line/description/" xr:uid="{3BA8787D-2860-5E4A-8156-7D9782B9ED8F}"/>
+    <hyperlink ref="C315" r:id="rId277" display="https://cspiration.com/login" xr:uid="{ED9C0BF3-78B4-9649-A40D-55F4832D2163}"/>
+    <hyperlink ref="B321" r:id="rId278" display="https://leetcode.com/problems/add-and-search-word-data-structure-design/description/" xr:uid="{9F5DD535-DEA6-A04A-BD8E-32AE2D311EA5}"/>
+    <hyperlink ref="C321" r:id="rId279" display="https://cspiration.com/login" xr:uid="{BB38E67E-4F97-7F42-8375-F71E32497AF2}"/>
+    <hyperlink ref="B320" r:id="rId280" display="https://leetcode.com/problems/implement-trie-prefix-tree/description/" xr:uid="{602E4DDD-36D7-4141-8092-E9C88B509111}"/>
+    <hyperlink ref="C320" r:id="rId281" display="https://cspiration.com/login" xr:uid="{0DED54BA-B698-6C41-BA3A-0C0A90A57FE9}"/>
+    <hyperlink ref="B322" r:id="rId282" display="https://leetcode.com/problems/word-search-ii/description/" xr:uid="{BBAAA406-4143-2547-84E9-7A53C0AEF74D}"/>
+    <hyperlink ref="C322" r:id="rId283" display="https://cspiration.com/login" xr:uid="{4609B9D0-3CC9-F44F-AA60-3C9F575CE95D}"/>
+    <hyperlink ref="B327" r:id="rId284" display="https://leetcode.com/problems/rotate-image/description/" xr:uid="{7307FDFA-5175-714A-8C7E-899B03D3C7AF}"/>
+    <hyperlink ref="C327" r:id="rId285" display="https://cspiration.com/login" xr:uid="{3A588833-5167-014E-808A-F94B9CB85E0A}"/>
+    <hyperlink ref="B328" r:id="rId286" display="https://leetcode.com/problems/spiral-matrix/description/" xr:uid="{9AE93216-8DD7-A24B-B766-81F3061DA63F}"/>
+    <hyperlink ref="C328" r:id="rId287" display="https://cspiration.com/login" xr:uid="{9898ACCE-1ADF-DD46-8923-6FE2C62EEE1F}"/>
+    <hyperlink ref="B329" r:id="rId288" display="https://leetcode.com/problems/spiral-matrix-ii/description/" xr:uid="{5DA83711-B1C4-814A-B350-A1F809CFAF76}"/>
+    <hyperlink ref="C329" r:id="rId289" display="https://cspiration.com/login" xr:uid="{E4979D8E-F2E5-6244-ADDA-D0D154ADB9BF}"/>
+    <hyperlink ref="B330" r:id="rId290" display="https://leetcode.com/problems/set-matrix-zeroes/description/" xr:uid="{04EF3395-468F-B845-AC19-8228316BEBA2}"/>
+    <hyperlink ref="C330" r:id="rId291" display="https://cspiration.com/login" xr:uid="{E66FAA44-D058-8043-A7DE-1D91910F82DD}"/>
+    <hyperlink ref="B331" r:id="rId292" display="https://leetcode.com/problems/sparse-matrix-multiplication/description/" xr:uid="{85DA3A1B-C4F7-6541-A436-ED62CA4A3E3D}"/>
+    <hyperlink ref="C331" r:id="rId293" display="https://cspiration.com/login" xr:uid="{37B10385-D55D-144C-864E-C79F6E6C70B7}"/>
+    <hyperlink ref="B332" r:id="rId294" display="https://leetcode.com/problems/longest-increasing-path-in-a-matrix/description/" xr:uid="{4612E730-D4A1-F24A-91F9-6B84D724A9AA}"/>
+    <hyperlink ref="C332" r:id="rId295" display="https://cspiration.com/login" xr:uid="{48020AFF-15AF-8447-AEB1-CFA1A841DBDC}"/>
+    <hyperlink ref="B333" r:id="rId296" display="https://leetcode.com/problems/kth-smallest-element-in-a-sorted-matrix/description/" xr:uid="{1DB2B93E-91F8-BD41-A00C-9AE687F699C3}"/>
+    <hyperlink ref="C333" r:id="rId297" display="https://cspiration.com/login" xr:uid="{30C034AB-1F54-2A4B-90FB-7B7ACB3052BE}"/>
+    <hyperlink ref="B334" r:id="rId298" display="https://leetcode.com/problems/search-a-2d-matrix/description/" xr:uid="{84EC2CF6-27EF-0347-9EF7-9D72E688DACF}"/>
+    <hyperlink ref="C334" r:id="rId299" display="https://cspiration.com/login" xr:uid="{D768F166-2FDB-CB46-AFC4-3D9EF7E6996A}"/>
+    <hyperlink ref="B335" r:id="rId300" display="https://leetcode.com/problems/search-a-2d-matrix-ii/description/" xr:uid="{E4FC6BE3-8670-9F4C-A5E3-020B79037385}"/>
+    <hyperlink ref="C335" r:id="rId301" display="https://cspiration.com/login" xr:uid="{F0BAE054-2E32-B346-A580-CDC57F21DC7D}"/>
+    <hyperlink ref="B336" r:id="rId302" display="https://leetcode.com/problems/range-addition/description/" xr:uid="{9A9D88D0-4B57-FC4D-AE66-B99ADD36B56B}"/>
+    <hyperlink ref="C336" r:id="rId303" display="https://cspiration.com/login" xr:uid="{7578592E-C29A-274C-8D6A-7E66CEEE99DB}"/>
+    <hyperlink ref="B337" r:id="rId304" display="https://leetcode.com/problems/word-search/description/" xr:uid="{5C361A98-5D4B-8342-AA9F-ECD72819FF3A}"/>
+    <hyperlink ref="C337" r:id="rId305" display="https://cspiration.com/login" xr:uid="{C4E85BE7-30E0-3049-8A7D-65EAAD242F6D}"/>
+    <hyperlink ref="B338" r:id="rId306" display="https://leetcode.com/problems/best-meeting-point/description/" xr:uid="{5731611E-A5BD-8948-955E-76F1D35419C6}"/>
+    <hyperlink ref="C338" r:id="rId307" display="https://cspiration.com/login" xr:uid="{6283B299-8B71-054E-A520-475134B7EC3C}"/>
+    <hyperlink ref="B339" r:id="rId308" display="https://leetcode.com/problems/bomb-enemy/description/" xr:uid="{5D2AE67B-AEB6-B648-A655-14C4CEAF0EC9}"/>
+    <hyperlink ref="C339" r:id="rId309" display="https://cspiration.com/login" xr:uid="{51C365CC-F3F9-8A41-8572-030B0F235286}"/>
+    <hyperlink ref="B340" r:id="rId310" display="https://leetcode.com/problems/shortest-distance-from-all-buildings/description/" xr:uid="{01FA28DB-CD25-1847-988D-8850AE25D782}"/>
+    <hyperlink ref="C340" r:id="rId311" display="https://cspiration.com/login" xr:uid="{2E8877A5-12D6-D84C-8F71-A9EFAD59E8A6}"/>
+    <hyperlink ref="B341" r:id="rId312" display="https://leetcode.com/problems/smallest-rectangle-enclosing-black-pixels/description/" xr:uid="{9C9CED59-C64E-824B-BD25-F452F7D75C28}"/>
+    <hyperlink ref="C341" r:id="rId313" display="https://cspiration.com/login" xr:uid="{985B1C72-6710-5746-AB0A-2023D14851EA}"/>
+    <hyperlink ref="B342" r:id="rId314" display="https://leetcode.com/problems/valid-sudoku/description/" xr:uid="{F75E3219-E661-E84F-9E59-BFCEFF119471}"/>
+    <hyperlink ref="C342" r:id="rId315" display="https://cspiration.com/login" xr:uid="{2566F254-8F41-624D-8AF9-0CC515DC93AF}"/>
+    <hyperlink ref="B343" r:id="rId316" display="https://leetcode.com/problems/sudoku-solver/description/" xr:uid="{C4EC3782-1D22-4540-A1B1-496634458106}"/>
+    <hyperlink ref="B350" r:id="rId317" display="https://leetcode.com/problems/min-stack/description/" xr:uid="{F440DA6C-20D8-1E49-A81C-C8A49CB93BC9}"/>
+    <hyperlink ref="C350" r:id="rId318" display="https://cspiration.com/login" xr:uid="{E963DECD-3A68-1B43-A3C0-F2AFDF74F576}"/>
+    <hyperlink ref="B353" r:id="rId319" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/description/" xr:uid="{323CD140-1D2C-5641-B079-A0D3C11AF8B8}"/>
+    <hyperlink ref="C353" r:id="rId320" display="https://cspiration.com/login" xr:uid="{30B01ACF-66E3-6146-9688-46129789566A}"/>
+    <hyperlink ref="B354" r:id="rId321" display="https://leetcode.com/problems/simplify-path/description/" xr:uid="{75FBD68A-59CA-EE45-8E8C-28F03E9CBA5F}"/>
+    <hyperlink ref="C354" r:id="rId322" display="https://cspiration.com/login" xr:uid="{CE624768-19D2-C341-B07D-7BCB355BF810}"/>
+    <hyperlink ref="B355" r:id="rId323" display="https://leetcode.com/problems/longest-absolute-file-path/description/" xr:uid="{8EF19021-99C1-524C-898F-49588978F57A}"/>
+    <hyperlink ref="C355" r:id="rId324" display="https://cspiration.com/login" xr:uid="{04F37A49-5801-3147-8087-B39F80A727ED}"/>
+    <hyperlink ref="B356" r:id="rId325" display="https://leetcode.com/problems/decode-string/" xr:uid="{9016FCAA-2C5D-224A-A605-4250504D9E21}"/>
+    <hyperlink ref="C356" r:id="rId326" display="https://cspiration.com/login" xr:uid="{6E747762-EF48-BB40-A8FA-EF6BA9E17E47}"/>
+    <hyperlink ref="B357" r:id="rId327" display="https://leetcode.com/problems/basic-calculator/description/" xr:uid="{B249DA9B-A579-BB4F-935B-AD5D98893E39}"/>
+    <hyperlink ref="C357" r:id="rId328" display="https://cspiration.com/login" xr:uid="{C7575803-DF49-9541-AF76-6ED16908948B}"/>
+    <hyperlink ref="B358" r:id="rId329" display="https://leetcode.com/problems/basic-calculator-ii/description/" xr:uid="{ADAF461A-BF26-9942-A27D-92552BCE4985}"/>
+    <hyperlink ref="C358" r:id="rId330" display="https://cspiration.com/login" xr:uid="{AADCBF4E-E957-3545-9A9A-69BE463704B1}"/>
+    <hyperlink ref="B359" r:id="rId331" display="https://leetcode.com/problems/mini-parser/description/" xr:uid="{B560B158-C783-BC47-AF92-D3A950618B33}"/>
+    <hyperlink ref="C359" r:id="rId332" display="https://cspiration.com/login" xr:uid="{8BF22178-5CF9-0F4C-AF15-B49AB5678228}"/>
+    <hyperlink ref="B360" r:id="rId333" display="https://leetcode.com/problems/largest-rectangle-in-histogram/description/" xr:uid="{D16F87E5-024B-3A4E-88C4-9C9461BA5AF3}"/>
+    <hyperlink ref="C360" r:id="rId334" display="https://cspiration.com/login" xr:uid="{545E374B-11A8-044A-BBB8-9BCB32D98233}"/>
+    <hyperlink ref="B362" r:id="rId335" display="https://leetcode.com/problems/kth-largest-element-in-an-array/description/" xr:uid="{535F78CD-9788-9241-9324-FDE6E95A7471}"/>
+    <hyperlink ref="C362" r:id="rId336" display="https://cspiration.com/login" xr:uid="{5B3A0335-582B-E246-9766-A2C8D6A13712}"/>
+    <hyperlink ref="B363" r:id="rId337" display="https://leetcode.com/problems/top-k-frequent-elements/description/" xr:uid="{20529FD4-8DCF-1E46-B3A3-B56C38D09A62}"/>
+    <hyperlink ref="C363" r:id="rId338" display="https://cspiration.com/login" xr:uid="{2AE2DFEB-B48D-C84A-8C29-5028A8335313}"/>
+    <hyperlink ref="B364" r:id="rId339" display="https://leetcode.com/problems/the-skyline-problem/description/" xr:uid="{555ECA51-8403-0043-AB25-AE755F19D292}"/>
+    <hyperlink ref="C364" r:id="rId340" display="https://cspiration.com/login" xr:uid="{0EF78CCD-4794-5244-8022-DB100F29DA4B}"/>
+    <hyperlink ref="B365" r:id="rId341" display="https://leetcode.com/problems/reconstruct-itinerary/description/" xr:uid="{69F40E17-AD13-0A49-8754-0A3ABC9987A0}"/>
+    <hyperlink ref="C365" r:id="rId342" display="https://cspiration.com/login" xr:uid="{79513BEC-4210-DC47-93D5-503548661168}"/>
+    <hyperlink ref="B366" r:id="rId343" display="https://leetcode.com/problems/flatten-nested-list-iterator/" xr:uid="{DD35E978-B21B-134C-9EF0-5A3AE318503F}"/>
+    <hyperlink ref="B378" r:id="rId344" display="https://leetcode.com/problems/find-the-difference/description/" xr:uid="{66F0F98C-0493-9A4D-A44F-5BE4CC51AAE5}"/>
+    <hyperlink ref="C378" r:id="rId345" display="https://cspiration.com/login" xr:uid="{E3DD03DD-A45E-0D4C-AD1B-2D52F25A37F3}"/>
+    <hyperlink ref="B379" r:id="rId346" display="https://leetcode.com/problems/single-number/description/" xr:uid="{BED5E2B6-90CA-7B4E-90C7-C301DCFF560C}"/>
+    <hyperlink ref="C379" r:id="rId347" display="https://cspiration.com/login" xr:uid="{C82A5A87-6BE1-CC46-98A2-231459011793}"/>
+    <hyperlink ref="B380" r:id="rId348" display="https://leetcode.com/problems/maximum-product-of-word-lengths/description/" xr:uid="{E4C7AD05-DE05-D24D-BE33-6638EC5D9637}"/>
+    <hyperlink ref="B389" r:id="rId349" display="https://leetcode.com/problems/course-schedule/description/" xr:uid="{E656E48A-EA12-5849-9A80-C2BF41442E59}"/>
+    <hyperlink ref="C389" r:id="rId350" display="https://cspiration.com/login" xr:uid="{3EB935A0-4F51-E243-880C-8E53A49B7BDE}"/>
+    <hyperlink ref="B390" r:id="rId351" display="https://leetcode.com/problems/course-schedule-ii/description/" xr:uid="{82EC9748-3D96-FB40-9C82-D9EC67A70D5C}"/>
+    <hyperlink ref="C390" r:id="rId352" display="https://cspiration.com/login" xr:uid="{B87FC0EF-5581-1C4B-BA95-9A8EC85017C3}"/>
+    <hyperlink ref="B391" r:id="rId353" display="https://leetcode.com/problems/alien-dictionary/description/" xr:uid="{78548044-2481-0344-AFBC-83875B145CA1}"/>
+    <hyperlink ref="B396" r:id="rId354" display="https://leetcode.com/problems/shuffle-an-array/" xr:uid="{6453089E-CA54-134A-9FC0-3C8014FD77C2}"/>
+    <hyperlink ref="C396" r:id="rId355" display="https://cspiration.com/login" xr:uid="{D7CA8D38-E652-1148-ABB9-81EC04662763}"/>
+    <hyperlink ref="B397" r:id="rId356" display="https://leetcode.com/problems/random-pick-index/" xr:uid="{F131635D-4FB5-924E-B5CD-862EB3652B2B}"/>
+    <hyperlink ref="C397" r:id="rId357" display="https://cspiration.com/login" xr:uid="{A86BA5CD-BAC4-8C47-8EE4-B8955CCEA183}"/>
+    <hyperlink ref="B398" r:id="rId358" display="https://leetcode.com/problems/linked-list-random-node/" xr:uid="{A1888F03-0EB5-2748-A259-0B4A9CD4EF43}"/>
+    <hyperlink ref="C398" r:id="rId359" display="https://cspiration.com/login" xr:uid="{65FD45C5-DD3B-DE47-9E83-54C91C87729B}"/>
+    <hyperlink ref="B399" r:id="rId360" display="https://leetcode.com/problems/insert-delete-getrandom-o1/" xr:uid="{53D6868D-E06B-9E41-893E-10270AC574B1}"/>
+    <hyperlink ref="C399" r:id="rId361" display="https://cspiration.com/login" xr:uid="{365D07BD-17D4-C441-9A5F-1BB59E6D56A2}"/>
+    <hyperlink ref="B400" r:id="rId362" display="https://leetcode.com/problems/insert-delete-getrandom-o1-duplicates-allowed/" xr:uid="{9389641E-41E0-F942-8216-EAEBA38C85B4}"/>
+    <hyperlink ref="C400" r:id="rId363" display="https://cspiration.com/login" xr:uid="{904C4BB6-1E13-7645-B333-3A00537028EA}"/>
+    <hyperlink ref="B401" r:id="rId364" display="https://leetcode.com/problems/copy-list-with-random-pointer/" xr:uid="{502294E5-9F27-F348-972C-1CC0B327251B}"/>
+    <hyperlink ref="B406" r:id="rId365" display="https://leetcode.com/problems/logger-rate-limiter/description/" xr:uid="{C61A4B52-AD3D-BA46-87E4-308B4991A1BE}"/>
+    <hyperlink ref="C406" r:id="rId366" display="https://cspiration.com/login" xr:uid="{C8FA91CA-1A1C-A343-B72B-B268EFB0471E}"/>
+    <hyperlink ref="B407" r:id="rId367" display="https://leetcode.com/problems/moving-average-from-data-stream/description/" xr:uid="{955896A7-B8EF-CF43-8F66-08000C728103}"/>
+    <hyperlink ref="C407" r:id="rId368" display="https://cspiration.com/login" xr:uid="{06FDBA83-7621-E44B-9658-16FFE47879DC}"/>
+    <hyperlink ref="B408" r:id="rId369" display="https://leetcode.com/problems/design-hit-counter/description/" xr:uid="{DE173B81-DAF1-0340-8314-DDBF79277E83}"/>
+    <hyperlink ref="C408" r:id="rId370" display="https://cspiration.com/login" xr:uid="{182B161B-7264-FF46-8F20-8596394F1A3F}"/>
+    <hyperlink ref="B409" r:id="rId371" display="https://leetcode.com/problems/zigzag-iterator/description/" xr:uid="{11767196-3C22-2447-B8EC-1F07890F8388}"/>
+    <hyperlink ref="C409" r:id="rId372" display="https://cspiration.com/login" xr:uid="{A30AB03D-0BDD-5E44-9B2D-8E674E5C7E3D}"/>
+    <hyperlink ref="B410" r:id="rId373" display="https://leetcode.com/problems/peeking-iterator/description/" xr:uid="{C2F26E0B-1B42-6E4E-A18E-7C08BA7C1B42}"/>
+    <hyperlink ref="C410" r:id="rId374" display="https://cspiration.com/login" xr:uid="{44206301-520A-0A45-BA7F-A11BC827C366}"/>
+    <hyperlink ref="B411" r:id="rId375" display="https://leetcode.com/problems/flatten-2d-vector/description/s" xr:uid="{57450831-6D8B-FB48-A279-CE0A3323317E}"/>
+    <hyperlink ref="C411" r:id="rId376" display="https://cspiration.com/login" xr:uid="{96A57980-751B-8144-92C2-BABEE8F96631}"/>
+    <hyperlink ref="B412" r:id="rId377" display="https://leetcode.com/problems/unique-word-abbreviation/description/" xr:uid="{019A71BE-0695-A847-AF69-5D34ACD31E89}"/>
+    <hyperlink ref="C412" r:id="rId378" display="https://cspiration.com/login" xr:uid="{46A711DD-8C66-AA46-A32F-F202A28B9507}"/>
+    <hyperlink ref="B413" r:id="rId379" display="https://leetcode.com/problems/two-sum-iii-data-structure-design/description/" xr:uid="{AD3BBDDB-8328-6E4F-A75F-356936A16C4C}"/>
+    <hyperlink ref="C413" r:id="rId380" display="https://cspiration.com/login" xr:uid="{10FC6473-5D12-5149-AA22-84C76CFC6688}"/>
+    <hyperlink ref="B414" r:id="rId381" display="https://leetcode.com/problems/design-tic-tac-toe/description/" xr:uid="{AD8E2DF9-7942-4D46-BFD1-57F3D2AD44DB}"/>
+    <hyperlink ref="C414" r:id="rId382" display="https://cspiration.com/login" xr:uid="{37D69D5A-712E-184E-A378-56C63574860D}"/>
+    <hyperlink ref="B415" r:id="rId383" display="https://leetcode.com/problems/design-phone-directory/description/" xr:uid="{44CB5AA8-40CB-1548-A13A-8BDA618DEEEA}"/>
+    <hyperlink ref="C415" r:id="rId384" display="https://cspiration.com/login" xr:uid="{B574C4D4-D8CB-F149-A1B4-056134B8F32C}"/>
+    <hyperlink ref="B416" r:id="rId385" display="https://leetcode.com/problems/design-snake-game/description/" xr:uid="{324F0A0D-4EA3-714D-A979-76944830B25B}"/>
+    <hyperlink ref="C416" r:id="rId386" display="https://cspiration.com/login" xr:uid="{5493DA6E-560F-1F42-8BD3-30E74B52A9EE}"/>
+    <hyperlink ref="B417" r:id="rId387" display="https://leetcode.com/problems/lru-cache/description/" xr:uid="{F88E3B9C-4B90-E64B-8AD5-9CD4C40493C1}"/>
+    <hyperlink ref="C417" r:id="rId388" display="https://cspiration.com/login" xr:uid="{A9C08738-1151-DA4A-8104-F1370B908852}"/>
+    <hyperlink ref="B418" r:id="rId389" display="https://leetcode.com/problems/design-twitter/description/s" xr:uid="{7965E5BC-C0D4-4D4B-9EF8-5078FEF7C8CB}"/>
+    <hyperlink ref="C418" r:id="rId390" display="https://cspiration.com/login" xr:uid="{766F5950-D9AE-114C-B6FD-41A5E9E6488D}"/>
+    <hyperlink ref="B419" r:id="rId391" display="https://leetcode.com/problems/range-sum-query-immutable/description/" xr:uid="{DAE9AE27-DEB1-264D-983B-6882A6368AE9}"/>
+    <hyperlink ref="C419" r:id="rId392" display="https://cspiration.com/login" xr:uid="{9273492A-44F6-5A49-8A13-5F376FCD62E9}"/>
+    <hyperlink ref="B420" r:id="rId393" display="https://leetcode.com/problems/range-sum-query-2d-immutable/description/" xr:uid="{AAD316F4-6941-704B-BCAD-4CC426E56FB4}"/>
+    <hyperlink ref="C420" r:id="rId394" display="https://cspiration.com/login" xr:uid="{D97D8BB0-1CA8-2645-9A6B-2DA077BF821E}"/>
+    <hyperlink ref="B421" r:id="rId395" display="https://leetcode.com/problems/range-sum-query-mutable/description/" xr:uid="{0F4D6567-EC93-264D-BF9D-423DB12163FF}"/>
+    <hyperlink ref="C421" r:id="rId396" display="https://cspiration.com/login" xr:uid="{47C40B78-FDBF-4A44-8C69-EB0D78FC59E3}"/>
+    <hyperlink ref="B422" r:id="rId397" display="https://leetcode.com/problems/range-sum-query-2d-mutable/description/" xr:uid="{F43E9B26-EA0F-C24C-A60F-095FE73C872B}"/>
+    <hyperlink ref="C422" r:id="rId398" display="https://cspiration.com/login" xr:uid="{3D32B22A-9D2F-D04B-8B77-0953B2EA5193}"/>
+    <hyperlink ref="B423" r:id="rId399" xr:uid="{FE9627AB-7397-CB48-AB91-E04DF9F829E5}"/>
     <hyperlink ref="B213" r:id="rId400" xr:uid="{6E505C5D-7486-774A-8436-0B2D9A806CE7}"/>
-    <hyperlink ref="B245" r:id="rId401" xr:uid="{13747061-B8D2-6041-B323-BA395125DCAA}"/>
-    <hyperlink ref="B297" r:id="rId402" xr:uid="{2D2F7CE9-7323-F34F-AA6B-4FECD6A6C804}"/>
-    <hyperlink ref="B430" r:id="rId403" display="https://leetcode.com/problems/search-insert-position/description/" xr:uid="{EB4E5B68-F05A-0C4B-9F53-41E4DBCA4F9E}"/>
-    <hyperlink ref="C430" r:id="rId404" display="https://cspiration.com/login" xr:uid="{CA1BBCD7-117A-A64E-8F77-852F33D02DB2}"/>
-    <hyperlink ref="B431" r:id="rId405" display="https://leetcode.com/problems/search-in-rotated-sorted-array/description/" xr:uid="{5B45788F-BB03-4843-BD6A-B976C9FCAEF1}"/>
-    <hyperlink ref="C431" r:id="rId406" display="https://cspiration.com/login" xr:uid="{551CAD20-3D2A-A64A-B23A-A01403C05DE0}"/>
-    <hyperlink ref="B432" r:id="rId407" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{89F11509-794F-0147-A002-99DBFE4011DC}"/>
-    <hyperlink ref="C432" r:id="rId408" display="https://cspiration.com/login" xr:uid="{A8D71102-8F66-8143-AADE-EC0B951315AF}"/>
-    <hyperlink ref="B433" r:id="rId409" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/description/" xr:uid="{A4765584-11DB-8C47-A9D8-28BCD3B3DB04}"/>
-    <hyperlink ref="C433" r:id="rId410" display="https://cspiration.com/login" xr:uid="{67A40D64-8C16-AB40-AF02-EC047B85587D}"/>
-    <hyperlink ref="B434" r:id="rId411" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/description/" xr:uid="{1C321054-4E86-0A4C-A5A9-D1503A97B9B0}"/>
-    <hyperlink ref="C434" r:id="rId412" display="https://cspiration.com/login" xr:uid="{4230A88F-C71C-F14B-89AA-04DA1B742A89}"/>
-    <hyperlink ref="B435" r:id="rId413" display="https://leetcode.com/problems/find-peak-element/description/" xr:uid="{736794C5-518A-194B-A096-354260C26D19}"/>
-    <hyperlink ref="C435" r:id="rId414" display="https://cspiration.com/login" xr:uid="{CC616423-7FF6-4546-BE49-14971E421AB1}"/>
-    <hyperlink ref="B436" r:id="rId415" display="https://leetcode.com/problems/guess-number-higher-or-lower/" xr:uid="{AA2881B4-D507-6C4E-B5AC-66556CE2E240}"/>
-    <hyperlink ref="C436" r:id="rId416" display="https://cspiration.com/login" xr:uid="{497BA16C-CBAB-CD4C-B123-9991F3A2E286}"/>
-    <hyperlink ref="B437" r:id="rId417" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/description/" xr:uid="{D78ED803-9C52-3C4E-8DAB-2FE615A62AB4}"/>
-    <hyperlink ref="C437" r:id="rId418" display="https://cspiration.com/login" xr:uid="{A8AD4217-A555-BA44-A724-8A04E7730E30}"/>
-    <hyperlink ref="B438" r:id="rId419" display="https://leetcode.com/problems/count-of-smaller-numbers-after-self/description/" xr:uid="{39F3DFF8-98F3-604E-9124-DD7F0D40F1B0}"/>
-    <hyperlink ref="C438" r:id="rId420" display="https://cspiration.com/login" xr:uid="{3561FB2C-CD0E-A746-8C4B-80613899C341}"/>
-    <hyperlink ref="B439" r:id="rId421" display="https://leetcode.com/problems/longest-increasing-subsequence/description/" xr:uid="{E9195674-DC99-4B46-B0EE-98194075832A}"/>
-    <hyperlink ref="C439" r:id="rId422" display="https://cspiration.com/login" xr:uid="{916F2DEE-639E-C943-A663-2517B8604445}"/>
-    <hyperlink ref="B440" r:id="rId423" display="https://leetcode.com/problems/russian-doll-envelopes/description/" xr:uid="{320B423A-BCFA-CE44-9951-2BD15ECD57E2}"/>
-    <hyperlink ref="B250" r:id="rId424" xr:uid="{600A5416-B5C9-BA47-892A-EE12A30AA3C9}"/>
-    <hyperlink ref="B254" r:id="rId425" xr:uid="{EADB0E54-5800-704D-A97B-CDE42026CFF8}"/>
-    <hyperlink ref="B367" r:id="rId426" xr:uid="{49EE6590-FC3C-C54F-A151-AA1FC6EF5061}"/>
-    <hyperlink ref="B350" r:id="rId427" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{E018DFB4-01AC-F645-8B90-8199997E6DD0}"/>
-    <hyperlink ref="C350" r:id="rId428" display="https://cspiration.com/login" xr:uid="{706E0A6D-CD70-2245-A6EA-B10034698AA6}"/>
-    <hyperlink ref="B351" r:id="rId429" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{0DF8CEC5-24F8-E745-8AEF-C177BA8C38D8}"/>
-    <hyperlink ref="B368" r:id="rId430" xr:uid="{6D13D071-F78E-C442-8632-E396881ABD22}"/>
-    <hyperlink ref="B369" r:id="rId431" xr:uid="{B66856FD-8BB7-CF4C-9F54-EF95505D135F}"/>
-    <hyperlink ref="B370" r:id="rId432" xr:uid="{3202C9A2-D22F-454B-BEEC-EC2EF095CF78}"/>
-    <hyperlink ref="B371" r:id="rId433" xr:uid="{0F820F81-AD67-2D4C-B1D6-92E7AE13C361}"/>
-    <hyperlink ref="B234" r:id="rId434" xr:uid="{8066B6F4-349C-104A-B6B1-4C5FDFBC5FE9}"/>
-    <hyperlink ref="B380" r:id="rId435" xr:uid="{12FCA401-D49E-F648-925D-5AA92C613FEE}"/>
-    <hyperlink ref="B381" r:id="rId436" xr:uid="{2AC0AA2F-79DF-D044-84B7-A131AC44BC10}"/>
-    <hyperlink ref="B382" r:id="rId437" xr:uid="{7F474B46-9483-0F48-AE6E-83C002C6D472}"/>
-    <hyperlink ref="B441" r:id="rId438" xr:uid="{30FFAA64-911B-8A47-9B10-24A60021362C}"/>
+    <hyperlink ref="B246" r:id="rId401" xr:uid="{13747061-B8D2-6041-B323-BA395125DCAA}"/>
+    <hyperlink ref="B298" r:id="rId402" xr:uid="{2D2F7CE9-7323-F34F-AA6B-4FECD6A6C804}"/>
+    <hyperlink ref="B431" r:id="rId403" display="https://leetcode.com/problems/search-insert-position/description/" xr:uid="{EB4E5B68-F05A-0C4B-9F53-41E4DBCA4F9E}"/>
+    <hyperlink ref="C431" r:id="rId404" display="https://cspiration.com/login" xr:uid="{CA1BBCD7-117A-A64E-8F77-852F33D02DB2}"/>
+    <hyperlink ref="B432" r:id="rId405" display="https://leetcode.com/problems/search-in-rotated-sorted-array/description/" xr:uid="{5B45788F-BB03-4843-BD6A-B976C9FCAEF1}"/>
+    <hyperlink ref="C432" r:id="rId406" display="https://cspiration.com/login" xr:uid="{551CAD20-3D2A-A64A-B23A-A01403C05DE0}"/>
+    <hyperlink ref="B433" r:id="rId407" display="https://leetcode.com/problems/search-in-rotated-sorted-array-ii/description/" xr:uid="{89F11509-794F-0147-A002-99DBFE4011DC}"/>
+    <hyperlink ref="C433" r:id="rId408" display="https://cspiration.com/login" xr:uid="{A8D71102-8F66-8143-AADE-EC0B951315AF}"/>
+    <hyperlink ref="B434" r:id="rId409" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array/description/" xr:uid="{A4765584-11DB-8C47-A9D8-28BCD3B3DB04}"/>
+    <hyperlink ref="C434" r:id="rId410" display="https://cspiration.com/login" xr:uid="{67A40D64-8C16-AB40-AF02-EC047B85587D}"/>
+    <hyperlink ref="B435" r:id="rId411" display="https://leetcode.com/problems/find-minimum-in-rotated-sorted-array-ii/description/" xr:uid="{1C321054-4E86-0A4C-A5A9-D1503A97B9B0}"/>
+    <hyperlink ref="C435" r:id="rId412" display="https://cspiration.com/login" xr:uid="{4230A88F-C71C-F14B-89AA-04DA1B742A89}"/>
+    <hyperlink ref="B436" r:id="rId413" display="https://leetcode.com/problems/find-peak-element/description/" xr:uid="{736794C5-518A-194B-A096-354260C26D19}"/>
+    <hyperlink ref="C436" r:id="rId414" display="https://cspiration.com/login" xr:uid="{CC616423-7FF6-4546-BE49-14971E421AB1}"/>
+    <hyperlink ref="B437" r:id="rId415" display="https://leetcode.com/problems/guess-number-higher-or-lower/" xr:uid="{AA2881B4-D507-6C4E-B5AC-66556CE2E240}"/>
+    <hyperlink ref="C437" r:id="rId416" display="https://cspiration.com/login" xr:uid="{497BA16C-CBAB-CD4C-B123-9991F3A2E286}"/>
+    <hyperlink ref="B438" r:id="rId417" display="https://leetcode.com/problems/find-first-and-last-position-of-element-in-sorted-array/description/" xr:uid="{D78ED803-9C52-3C4E-8DAB-2FE615A62AB4}"/>
+    <hyperlink ref="C438" r:id="rId418" display="https://cspiration.com/login" xr:uid="{A8AD4217-A555-BA44-A724-8A04E7730E30}"/>
+    <hyperlink ref="B439" r:id="rId419" display="https://leetcode.com/problems/count-of-smaller-numbers-after-self/description/" xr:uid="{39F3DFF8-98F3-604E-9124-DD7F0D40F1B0}"/>
+    <hyperlink ref="C439" r:id="rId420" display="https://cspiration.com/login" xr:uid="{3561FB2C-CD0E-A746-8C4B-80613899C341}"/>
+    <hyperlink ref="B440" r:id="rId421" display="https://leetcode.com/problems/longest-increasing-subsequence/description/" xr:uid="{E9195674-DC99-4B46-B0EE-98194075832A}"/>
+    <hyperlink ref="C440" r:id="rId422" display="https://cspiration.com/login" xr:uid="{916F2DEE-639E-C943-A663-2517B8604445}"/>
+    <hyperlink ref="B441" r:id="rId423" display="https://leetcode.com/problems/russian-doll-envelopes/description/" xr:uid="{320B423A-BCFA-CE44-9951-2BD15ECD57E2}"/>
+    <hyperlink ref="B251" r:id="rId424" xr:uid="{600A5416-B5C9-BA47-892A-EE12A30AA3C9}"/>
+    <hyperlink ref="B255" r:id="rId425" xr:uid="{EADB0E54-5800-704D-A97B-CDE42026CFF8}"/>
+    <hyperlink ref="B368" r:id="rId426" xr:uid="{49EE6590-FC3C-C54F-A151-AA1FC6EF5061}"/>
+    <hyperlink ref="B351" r:id="rId427" display="https://leetcode.com/problems/implement-queue-using-stacks/description/" xr:uid="{E018DFB4-01AC-F645-8B90-8199997E6DD0}"/>
+    <hyperlink ref="C351" r:id="rId428" display="https://cspiration.com/login" xr:uid="{706E0A6D-CD70-2245-A6EA-B10034698AA6}"/>
+    <hyperlink ref="B352" r:id="rId429" display="https://leetcode.com/problems/implement-stack-using-queues/description/" xr:uid="{0DF8CEC5-24F8-E745-8AEF-C177BA8C38D8}"/>
+    <hyperlink ref="B369" r:id="rId430" xr:uid="{6D13D071-F78E-C442-8632-E396881ABD22}"/>
+    <hyperlink ref="B370" r:id="rId431" xr:uid="{B66856FD-8BB7-CF4C-9F54-EF95505D135F}"/>
+    <hyperlink ref="B371" r:id="rId432" xr:uid="{3202C9A2-D22F-454B-BEEC-EC2EF095CF78}"/>
+    <hyperlink ref="B372" r:id="rId433" xr:uid="{0F820F81-AD67-2D4C-B1D6-92E7AE13C361}"/>
+    <hyperlink ref="B235" r:id="rId434" xr:uid="{8066B6F4-349C-104A-B6B1-4C5FDFBC5FE9}"/>
+    <hyperlink ref="B381" r:id="rId435" xr:uid="{12FCA401-D49E-F648-925D-5AA92C613FEE}"/>
+    <hyperlink ref="B382" r:id="rId436" xr:uid="{2AC0AA2F-79DF-D044-84B7-A131AC44BC10}"/>
+    <hyperlink ref="B383" r:id="rId437" xr:uid="{7F474B46-9483-0F48-AE6E-83C002C6D472}"/>
+    <hyperlink ref="B442" r:id="rId438" xr:uid="{30FFAA64-911B-8A47-9B10-24A60021362C}"/>
     <hyperlink ref="B114" r:id="rId439" xr:uid="{328EC544-84F7-C546-82CB-6D867891F222}"/>
     <hyperlink ref="C113" r:id="rId440" display="https://cspiration.com/login" xr:uid="{B24A14A7-52F4-E249-B609-37F1D91D19AF}"/>
     <hyperlink ref="B113" r:id="rId441" display="https://leetcode.com/problems/valid-number/description/" xr:uid="{5B3E385E-B11A-C64D-8285-B8177A8BCDA4}"/>
@@ -6803,8 +6949,218 @@
     <hyperlink ref="C76" r:id="rId635" display="https://cspiration.com/login" xr:uid="{370A9C08-9397-6244-9A7C-D5A7706B5C33}"/>
     <hyperlink ref="B77" r:id="rId636" display="https://leetcode.com/problems/russian-doll-envelopes/description/" xr:uid="{F3713F37-2092-EE4F-9D0F-DF78CC7E6F5F}"/>
     <hyperlink ref="B40" r:id="rId637" xr:uid="{A8664FBD-4D0C-9F4E-B3FF-1A3A080A62BA}"/>
-    <hyperlink ref="B442" r:id="rId638" xr:uid="{470B60D0-0690-D646-A3F7-60EFD7D84914}"/>
+    <hyperlink ref="B443" r:id="rId638" xr:uid="{470B60D0-0690-D646-A3F7-60EFD7D84914}"/>
     <hyperlink ref="B188" r:id="rId639" xr:uid="{480C3FC1-E1AD-1549-AE5F-DCB9796EBAB6}"/>
+    <hyperlink ref="B444" r:id="rId640" xr:uid="{479C33DE-F0FB-4D48-8E33-1B3B609B8C06}"/>
+    <hyperlink ref="B226" r:id="rId641" xr:uid="{0E084F61-5CC3-634B-86CA-32EE4D7A8159}"/>
+    <hyperlink ref="B424" r:id="rId642" xr:uid="{3B627479-B599-9A4B-84E9-0B08FE576256}"/>
+    <hyperlink ref="B190" r:id="rId643" xr:uid="{8885AE70-00E5-254B-BA1C-AC2F4AAFC2EE}"/>
+    <hyperlink ref="B78" r:id="rId644" xr:uid="{866844FC-D136-D24D-A714-D9F7287029B9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F2D10D-1C28-0C44-9A30-1F016C7DDC26}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView zoomScale="165" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>386</v>
+      </c>
+      <c r="C3" t="s">
+        <v>390</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>388</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>391</v>
+      </c>
+      <c r="C5" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>394</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>401</v>
+      </c>
+      <c r="C9" t="s">
+        <v>392</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>404</v>
+      </c>
+      <c r="C11" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>406</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{2E7E144F-6FFE-5B49-AC01-8230ED6A4C57}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{D432FD45-55B8-184F-AFDC-6C0276A6443A}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{F300A87B-033E-3741-8569-8467875A5DB6}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{64E7D2ED-C313-2349-A1A0-41A9DFFA6169}"/>
+    <hyperlink ref="A2" r:id="rId5" xr:uid="{6DC7976D-BC10-3A46-A70F-0DF63CEAB1E7}"/>
+    <hyperlink ref="F9" r:id="rId6" xr:uid="{B2D22442-96A3-CB49-AA7B-0EEBC51B8B05}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66A5F11-ABDA-6C4E-B320-90D5F53E6BB6}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1481</v>
+      </c>
+      <c r="B3" t="s">
+        <v>407</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1120</v>
+      </c>
+      <c r="B4" t="s">
+        <v>413</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1041</v>
+      </c>
+      <c r="B5" t="s">
+        <v>412</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1465</v>
+      </c>
+      <c r="B6" t="s">
+        <v>415</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>973</v>
+      </c>
+      <c r="B7" t="s">
+        <v>417</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>418</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{DF5DB716-9032-F94A-B534-C14A60EF7A5D}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{86A494AE-B681-4F4C-9FB2-2183043B4CB5}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{799FFBB6-6DEB-364C-A1B4-799FDE7F453D}"/>
+    <hyperlink ref="F4" r:id="rId4" xr:uid="{3EA58E5D-363F-684C-B96D-8835A3BCDEF8}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{B505B52F-3BC7-4F41-9B30-F3ED7D1FD64F}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{E24F2577-00C5-4A4E-AF28-DBC03C13D8BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>